<commit_message>
needed updates to DataStructures
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/ShinyDashboardApp_HBEF/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{66F53E6A-7177-9A4D-A27A-158488FD3207}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{011F8598-62C8-B445-9CAB-3D724E81413D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="580" windowWidth="20080" windowHeight="17560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35060" yWindow="5360" windowWidth="24220" windowHeight="14600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="261">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -513,13 +513,7 @@
     <t>refNo</t>
   </si>
   <si>
-    <t>INT PRIMARY KEY</t>
-  </si>
-  <si>
     <t>VARCHAR(20)</t>
-  </si>
-  <si>
-    <t>DECIMAL(9,4)</t>
   </si>
   <si>
     <t>DATE</t>
@@ -528,13 +522,7 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>DECIMAL(4,4)</t>
-  </si>
-  <si>
     <t>SMALLINT</t>
-  </si>
-  <si>
-    <t>DECIMAL(6,4)</t>
   </si>
   <si>
     <t>VARCHAR(50)</t>
@@ -573,22 +561,10 @@
     <t>will eventually be filled in with Forest Servic data</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANC960 DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(4,4), Mg DECIMAL(4,4), K DECIMAL(4,4), Na DECIMAL(4,4), TMAl DECIMAL(4,4), OMAl DECIMAL(4,4), Al_ICP DECIMAL(4,4), NH4 DECIMAL(4,4), SO4 DECIMAL(4,4), NO3 DECIMAL(4,4), Cl DECIMAL(4,4), PO4 DECIMAL(4,4), DOC DECIMAL(4,4), TDN DECIMAL(4,4), DON DECIMAL(4,4), SiO2 DECIMAL(4,4), Mn DECIMAL(4,4), Fe DECIMAL(4,4), F DECIMAL(4,4), cationCharge DECIMAL(4,4), anionCharge DECIMAL(4,4), theoryCond DECIMAL(4,4), ionError DECIMAL(4,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(4,4)</t>
-  </si>
-  <si>
     <t>in *Lists*</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(9,4), precipETI DECIMAL(9,4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">data from pH 3Star </t>
-  </si>
-  <si>
-    <t>refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), pHmetrohm DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANC960 DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(4,4), Mg DECIMAL(4,4), K DECIMAL(4,4), Na DECIMAL(4,4), TMAl DECIMAL(4,4), OMAl DECIMAL(4,4), Al_ICP DECIMAL(4,4), NH4 DECIMAL(4,4), SO4 DECIMAL(4,4), NO3 DECIMAL(4,4), Cl DECIMAL(4,4), PO4 DECIMAL(4,4), DOC DECIMAL(4,4), TDN DECIMAL(4,4), DON DECIMAL(4,4), SiO2 DECIMAL(4,4), Mn DECIMAL(4,4), Fe DECIMAL(4,4), F DECIMAL(4,4), cationCharge DECIMAL(4,4), anionCharge DECIMAL(4,4), theoryCond DECIMAL(4,4), ionError DECIMAL(4,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(4,4)</t>
-  </si>
-  <si>
-    <t>refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), pHmetrohm DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
   </si>
   <si>
     <t>Date</t>
@@ -1018,12 +994,51 @@
   <si>
     <t>Output after standardizeClasses Current</t>
   </si>
+  <si>
+    <t>DECIMAL(8,4)</t>
+  </si>
+  <si>
+    <t>DECIMAL(10,4)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>Do not include in dataset; automatically generated upon upload.</t>
+  </si>
+  <si>
+    <t>DECIMAL(13,4)</t>
+  </si>
+  <si>
+    <t>INT PRIMARY KEY NOT NULL AUTO_INCREMENT</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4)</t>
+  </si>
+  <si>
+    <t>ALTER TABLE initial ADD INDEX (site), ADD INDEX (date), ADD INDEX (timeEST);</t>
+  </si>
+  <si>
+    <t>ALTER TABLE current ADD INDEX (site), ADD INDEX (date), ADD INDEX (timeEST);</t>
+  </si>
+  <si>
+    <t>ALTER TABLE historical ADD INDEX (site), ADD INDEX (date), ADD INDEX (timeEST);</t>
+  </si>
+  <si>
+    <t>ALTER TABLE sensor ADD INDEX (site), ADD INDEX (date), ADD INDEX (timeEST);</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1298,6 +1313,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -1484,7 +1505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1717,6 +1738,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2631,6 +2653,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1554B6EA-502F-D249-A755-56945D37144D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0DEDB3C-A3C6-5F4A-91FF-B2248A8A4BAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2931,7 +3061,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B789CDDB-5814-7844-98E7-4854F15F6979}">
-  <sheetPr>
+  <sheetPr codeName="Sheet7">
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:E15"/>
@@ -2947,10 +3077,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
@@ -2961,20 +3091,20 @@
         <v>43240</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C3" s="99" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D4" s="107" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -2982,39 +3112,39 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D6" s="107" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D7" s="108"/>
       <c r="E7" s="108" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="109" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D10" s="107" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D11" s="108"/>
       <c r="E11" s="108" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="E12" s="108" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D14" s="107" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -3031,7 +3161,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3046,42 +3176,44 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F1" s="98" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H1" s="98" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="104" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="117" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="99"/>
+        <v>253</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>251</v>
+      </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), pHmetrohm DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>170</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -3089,7 +3221,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="99"/>
       <c r="D3" t="str">
@@ -3102,20 +3234,23 @@
         <v>19</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">date DATE, </v>
       </c>
+      <c r="H4" s="118" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="99"/>
       <c r="D5" t="str">
@@ -3128,12 +3263,12 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C6" s="99"/>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(4,4), </v>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -3141,12 +3276,12 @@
         <v>26</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C7" s="99"/>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pHmetrohm DECIMAL(4,4), </v>
+        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -3154,7 +3289,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" t="str">
@@ -3167,12 +3302,12 @@
         <v>34</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(4,4), </v>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -3180,12 +3315,12 @@
         <v>36</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(4,4), </v>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -3193,12 +3328,12 @@
         <v>37</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(4,4), </v>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
@@ -3206,12 +3341,12 @@
         <v>38</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(4,4), </v>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
@@ -3219,7 +3354,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="99"/>
       <c r="D13" t="str">
@@ -3232,12 +3367,12 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>152</v>
+        <v>249</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(6,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -3245,12 +3380,12 @@
         <v>55</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(4,4), </v>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
@@ -3258,7 +3393,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" t="str">
@@ -3271,7 +3406,7 @@
         <v>62</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
@@ -3284,7 +3419,7 @@
         <v>64</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" t="str">
@@ -3448,8 +3583,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3464,46 +3599,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="103" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E1" s="98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G1" s="98" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I1" s="98" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="234" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="247" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="99"/>
+        <v>253</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>251</v>
+      </c>
       <c r="D2" s="99"/>
       <c r="E2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="G2" s="100" t="str">
         <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31,E32,E33,E34,E35,E36,E37,E38,E39,E40,E41,E42,E43,E44,E45,E46,E47)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), pHmetrohm DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANC960 DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(4,4), Mg DECIMAL(4,4), K DECIMAL(4,4), Na DECIMAL(4,4), TMAl DECIMAL(4,4), OMAl DECIMAL(4,4), Al_ICP DECIMAL(4,4), NH4 DECIMAL(4,4), SO4 DECIMAL(4,4), NO3 DECIMAL(4,4), Cl DECIMAL(4,4), PO4 DECIMAL(4,4), DOC DECIMAL(4,4), TDN DECIMAL(4,4), DON DECIMAL(4,4), SiO2 DECIMAL(4,4), Mn DECIMAL(4,4), Fe DECIMAL(4,4), F DECIMAL(4,4), cationCharge DECIMAL(4,4), anionCharge DECIMAL(4,4), theoryCond DECIMAL(4,4), ionError DECIMAL(4,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(4,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>169</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3511,7 +3648,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="99"/>
       <c r="D3" s="99"/>
@@ -3525,7 +3662,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" s="99"/>
@@ -3533,13 +3670,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">date DATE, </v>
       </c>
+      <c r="I4" s="118" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="99"/>
       <c r="D5" s="99"/>
@@ -3553,15 +3693,15 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D6" s="99"/>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(4,4), </v>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -3569,13 +3709,13 @@
         <v>26</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C7" s="99"/>
       <c r="D7" s="99"/>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pHmetrohm DECIMAL(4,4), </v>
+        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -3583,7 +3723,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" s="99"/>
@@ -3597,13 +3737,13 @@
         <v>34</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" s="99"/>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(4,4), </v>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3611,13 +3751,13 @@
         <v>36</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" s="99"/>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(4,4), </v>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -3625,13 +3765,13 @@
         <v>109</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" s="99"/>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANC960 DECIMAL(4,4), </v>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -3639,13 +3779,13 @@
         <v>37</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" s="99"/>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(4,4), </v>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -3653,13 +3793,13 @@
         <v>38</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C13" s="99"/>
       <c r="D13" s="99"/>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(4,4), </v>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -3667,7 +3807,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" s="99"/>
@@ -3681,13 +3821,13 @@
         <v>42</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>152</v>
+        <v>249</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" s="99"/>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(6,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -3695,13 +3835,13 @@
         <v>55</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" s="99"/>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(4,4), </v>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -3709,7 +3849,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" s="99"/>
@@ -3723,7 +3863,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" s="99"/>
@@ -3737,7 +3877,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C19" s="99"/>
       <c r="D19" s="99"/>
@@ -3751,7 +3891,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C20" s="99"/>
       <c r="D20" s="99"/>
@@ -3765,7 +3905,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C21" s="99"/>
       <c r="D21" s="99"/>
@@ -3779,13 +3919,13 @@
         <v>66</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(4,4), </v>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -3793,13 +3933,13 @@
         <v>70</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C23" s="99"/>
       <c r="D23" s="99"/>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(4,4), </v>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -3807,13 +3947,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C24" s="99"/>
       <c r="D24" s="99"/>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(4,4), </v>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -3821,13 +3961,13 @@
         <v>74</v>
       </c>
       <c r="B25" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C25" s="99"/>
       <c r="D25" s="99"/>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(4,4), </v>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -3835,13 +3975,13 @@
         <v>75</v>
       </c>
       <c r="B26" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C26" s="99"/>
       <c r="D26" s="99"/>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(4,4), </v>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -3849,13 +3989,13 @@
         <v>76</v>
       </c>
       <c r="B27" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C27" s="99"/>
       <c r="D27" s="99"/>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(4,4), </v>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -3863,13 +4003,13 @@
         <v>78</v>
       </c>
       <c r="B28" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C28" s="99"/>
       <c r="D28" s="99"/>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(4,4), </v>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -3877,13 +4017,13 @@
         <v>81</v>
       </c>
       <c r="B29" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C29" s="99"/>
       <c r="D29" s="99"/>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -3891,13 +4031,13 @@
         <v>82</v>
       </c>
       <c r="B30" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C30" s="99"/>
       <c r="D30" s="99"/>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -3905,13 +4045,13 @@
         <v>84</v>
       </c>
       <c r="B31" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C31" s="99"/>
       <c r="D31" s="99"/>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(4,4), </v>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -3919,13 +4059,13 @@
         <v>85</v>
       </c>
       <c r="B32" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C32" s="99"/>
       <c r="D32" s="99"/>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(4,4), </v>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -3933,13 +4073,13 @@
         <v>86</v>
       </c>
       <c r="B33" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C33" s="99"/>
       <c r="D33" s="99"/>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -3947,13 +4087,13 @@
         <v>89</v>
       </c>
       <c r="B34" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C34" s="99"/>
       <c r="D34" s="99"/>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(4,4), </v>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -3961,13 +4101,13 @@
         <v>90</v>
       </c>
       <c r="B35" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C35" s="99"/>
       <c r="D35" s="99"/>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(4,4), </v>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -3975,13 +4115,13 @@
         <v>91</v>
       </c>
       <c r="B36" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C36" s="99"/>
       <c r="D36" s="99"/>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(4,4), </v>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -3989,13 +4129,13 @@
         <v>92</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C37" s="99"/>
       <c r="D37" s="99"/>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(4,4), </v>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -4003,13 +4143,13 @@
         <v>93</v>
       </c>
       <c r="B38" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C38" s="99"/>
       <c r="D38" s="99"/>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(4,4), </v>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -4017,13 +4157,13 @@
         <v>94</v>
       </c>
       <c r="B39" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C39" s="99"/>
       <c r="D39" s="99"/>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(4,4), </v>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -4031,13 +4171,13 @@
         <v>95</v>
       </c>
       <c r="B40" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C40" s="99"/>
       <c r="D40" s="99"/>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(4,4), </v>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -4045,13 +4185,13 @@
         <v>97</v>
       </c>
       <c r="B41" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C41" s="99"/>
       <c r="D41" s="99"/>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(4,4), </v>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -4059,13 +4199,13 @@
         <v>98</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C42" s="99"/>
       <c r="D42" s="99"/>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(4,4), </v>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -4073,13 +4213,13 @@
         <v>100</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C43" s="99"/>
       <c r="D43" s="99"/>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(4,4), </v>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -4087,13 +4227,13 @@
         <v>101</v>
       </c>
       <c r="B44" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C44" s="99"/>
       <c r="D44" s="99"/>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(4,4), </v>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -4101,7 +4241,7 @@
         <v>102</v>
       </c>
       <c r="B45" s="99" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C45" s="99"/>
       <c r="D45" s="99"/>
@@ -4115,7 +4255,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C46" s="99"/>
       <c r="D46" s="99"/>
@@ -4129,18 +4269,18 @@
         <v>108</v>
       </c>
       <c r="B47" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C47" s="99"/>
       <c r="D47" s="99"/>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ionBalance DECIMAL(4,4), </v>
+        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="105" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4153,8 +4293,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4169,42 +4309,44 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F1" s="98" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H1" s="98" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="221" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="234" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="99"/>
+        <v>253</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>251</v>
+      </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(4,4), DIC SMALLINT, spCond DECIMAL(4,4), temp DECIMAL(4,4), ANC960 DECIMAL(4,4), ANCMet DECIMAL(4,4), gageHt DECIMAL(4,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(6,4), precipCatch DECIMAL(4,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(4,4), Mg DECIMAL(4,4), K DECIMAL(4,4), Na DECIMAL(4,4), TMAl DECIMAL(4,4), OMAl DECIMAL(4,4), Al_ICP DECIMAL(4,4), NH4 DECIMAL(4,4), SO4 DECIMAL(4,4), NO3 DECIMAL(4,4), Cl DECIMAL(4,4), PO4 DECIMAL(4,4), DOC DECIMAL(4,4), TDN DECIMAL(4,4), DON DECIMAL(4,4), SiO2 DECIMAL(4,4), Mn DECIMAL(4,4), Fe DECIMAL(4,4), F DECIMAL(4,4), cationCharge DECIMAL(4,4), anionCharge DECIMAL(4,4), theoryCond DECIMAL(4,4), ionError DECIMAL(4,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(4,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -4212,7 +4354,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="99"/>
       <c r="D3" t="str">
@@ -4225,20 +4367,23 @@
         <v>19</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">date DATE, </v>
       </c>
+      <c r="H4" s="118" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="99"/>
       <c r="D5" t="str">
@@ -4251,14 +4396,14 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(4,4), </v>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -4266,7 +4411,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="99"/>
       <c r="D7" t="str">
@@ -4279,12 +4424,12 @@
         <v>34</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(4,4), </v>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
@@ -4292,12 +4437,12 @@
         <v>36</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(4,4), </v>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -4305,12 +4450,12 @@
         <v>109</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANC960 DECIMAL(4,4), </v>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -4318,12 +4463,12 @@
         <v>37</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(4,4), </v>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
@@ -4331,12 +4476,12 @@
         <v>38</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(4,4), </v>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
@@ -4344,7 +4489,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="99"/>
       <c r="D13" t="str">
@@ -4357,12 +4502,12 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>152</v>
+        <v>249</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(6,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -4370,12 +4515,12 @@
         <v>55</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(4,4), </v>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
@@ -4383,7 +4528,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" t="str">
@@ -4396,7 +4541,7 @@
         <v>62</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
@@ -4409,7 +4554,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" t="str">
@@ -4422,7 +4567,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C19" s="99"/>
       <c r="D19" t="str">
@@ -4435,7 +4580,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C20" s="99"/>
       <c r="D20" t="str">
@@ -4448,12 +4593,12 @@
         <v>66</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C21" s="99"/>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(4,4), </v>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -4461,12 +4606,12 @@
         <v>70</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(4,4), </v>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -4474,12 +4619,12 @@
         <v>72</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C23" s="99"/>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(4,4), </v>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -4487,12 +4632,12 @@
         <v>74</v>
       </c>
       <c r="B24" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C24" s="99"/>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(4,4), </v>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -4500,12 +4645,12 @@
         <v>75</v>
       </c>
       <c r="B25" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C25" s="99"/>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(4,4), </v>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
@@ -4513,12 +4658,12 @@
         <v>76</v>
       </c>
       <c r="B26" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C26" s="99"/>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(4,4), </v>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -4526,14 +4671,14 @@
         <v>78</v>
       </c>
       <c r="B27" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C27" s="99" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(4,4), </v>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
@@ -4541,12 +4686,12 @@
         <v>81</v>
       </c>
       <c r="B28" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C28" s="99"/>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -4554,12 +4699,12 @@
         <v>82</v>
       </c>
       <c r="B29" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C29" s="99"/>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -4567,12 +4712,12 @@
         <v>84</v>
       </c>
       <c r="B30" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C30" s="99"/>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(4,4), </v>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
@@ -4580,12 +4725,12 @@
         <v>85</v>
       </c>
       <c r="B31" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C31" s="99"/>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(4,4), </v>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -4593,12 +4738,12 @@
         <v>86</v>
       </c>
       <c r="B32" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C32" s="99"/>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(4,4), </v>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -4606,12 +4751,12 @@
         <v>89</v>
       </c>
       <c r="B33" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C33" s="99"/>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(4,4), </v>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
@@ -4619,12 +4764,12 @@
         <v>90</v>
       </c>
       <c r="B34" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C34" s="99"/>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(4,4), </v>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -4632,12 +4777,12 @@
         <v>91</v>
       </c>
       <c r="B35" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C35" s="99"/>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(4,4), </v>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
@@ -4645,12 +4790,12 @@
         <v>92</v>
       </c>
       <c r="B36" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C36" s="99"/>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(4,4), </v>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
@@ -4658,12 +4803,12 @@
         <v>93</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C37" s="99"/>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(4,4), </v>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
@@ -4671,12 +4816,12 @@
         <v>94</v>
       </c>
       <c r="B38" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C38" s="99"/>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(4,4), </v>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
@@ -4684,12 +4829,12 @@
         <v>95</v>
       </c>
       <c r="B39" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C39" s="99"/>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(4,4), </v>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
@@ -4697,12 +4842,12 @@
         <v>97</v>
       </c>
       <c r="B40" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C40" s="99"/>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(4,4), </v>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
@@ -4710,12 +4855,12 @@
         <v>98</v>
       </c>
       <c r="B41" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C41" s="99"/>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(4,4), </v>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
@@ -4723,12 +4868,12 @@
         <v>100</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C42" s="99"/>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(4,4), </v>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
@@ -4736,12 +4881,12 @@
         <v>101</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C43" s="99"/>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(4,4), </v>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
@@ -4749,7 +4894,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="99" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C44" s="99"/>
       <c r="D44" t="str">
@@ -4762,7 +4907,7 @@
         <v>106</v>
       </c>
       <c r="B45" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C45" s="99"/>
       <c r="D45" t="str">
@@ -4775,12 +4920,12 @@
         <v>108</v>
       </c>
       <c r="B46" s="99" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C46" s="99"/>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ionBalance DECIMAL(4,4), </v>
+        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
     </row>
   </sheetData>
@@ -4793,8 +4938,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4809,42 +4954,44 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F1" s="98" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G1" s="98" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="99"/>
+        <v>253</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>251</v>
+      </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5, D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(9,4), precipETI DECIMAL(9,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
       </c>
       <c r="G2" s="102" t="s">
-        <v>167</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -4852,7 +4999,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C3" s="99"/>
       <c r="D3" t="str">
@@ -4865,7 +5012,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" t="str">
@@ -4873,14 +5020,16 @@
         <v xml:space="preserve">site VARCHAR(20), </v>
       </c>
       <c r="F4" s="100"/>
-      <c r="G4" s="102"/>
+      <c r="G4" s="118" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" s="99"/>
       <c r="D5" t="str">
@@ -4895,7 +5044,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="99"/>
       <c r="D6" t="str">
@@ -4910,14 +5059,14 @@
         <v>48</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
       <c r="C7" s="99" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7:D8" si="1">CONCATENATE(A7, " ",  B7, ", ")</f>
-        <v xml:space="preserve">flowSensor DECIMAL(9,4), </v>
+        <v xml:space="preserve">flowSensor DECIMAL(13,4), </v>
       </c>
       <c r="E7" s="99"/>
     </row>
@@ -4926,14 +5075,14 @@
         <v>56</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
       <c r="C8" s="99" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">precipETI DECIMAL(9,4), </v>
+        <v xml:space="preserve">precipETI DECIMAL(13,4), </v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -5153,9 +5302,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F953E5B-9006-6F45-8D30-64A5E11B6D26}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:BJ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -5175,399 +5325,399 @@
   <sheetData>
     <row r="1" spans="1:62" s="111" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="111" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B1" s="116" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C1" s="117" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D1" s="112" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E1" s="110"/>
       <c r="F1" s="110" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="G1" s="110" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H1" s="110"/>
       <c r="I1" s="110"/>
       <c r="J1" s="114" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="K1" s="114" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="L1" s="112" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="M1" s="112" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="112" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A2" s="110" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B2" s="113" t="s">
         <v>144</v>
       </c>
       <c r="C2" s="113" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E2" s="110" t="str">
         <f>IF(C2=D2, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J2" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="K2" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="L2" s="110" t="str">
         <f t="shared" ref="L2:L47" si="0">IF(J2=K2, " ", "!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N2" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="O2" s="110" t="str">
         <f>IF(C2=N2, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Q2" s="110" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="R2" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="S2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="T2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="U2" s="110" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="V2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="W2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="X2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="Y2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="Z2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AA2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AB2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AC2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AD2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AE2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AF2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AG2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AH2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AI2" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="AJ2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AK2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AL2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AM2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AN2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AO2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AP2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AQ2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AR2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AS2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AT2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AU2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AV2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AW2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AX2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AY2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AZ2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BA2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BB2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BC2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BD2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BE2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BF2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BG2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="BH2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="BI2" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="BJ2" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="110" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B3" s="113" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E3" s="110" t="str">
         <f t="shared" ref="E3:E47" si="1">IF(C3=D3, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J3" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K3" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L3" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N3" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O3" s="110" t="str">
         <f t="shared" ref="O3:O47" si="2">IF(C3=N3, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P3" s="110" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A4" s="110" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B4" s="113" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E4" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J4" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K4" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L4" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N4" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O4" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P4" s="110" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A5" s="110" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B5" s="113" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="113" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D5" s="110" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E5" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J5" s="115" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="K5" s="115" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="L5" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N5" s="110" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="O5" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P5" s="110" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A6" s="110" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B6" s="113" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E6" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J6" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K6" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L6" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="M6" s="110" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="N6" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O6" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P6" s="110" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A7" s="110" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B7" s="113" t="s">
         <v>137</v>
       </c>
       <c r="C7" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D7" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E7" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J7" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K7" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L7" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N7" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O7" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5576,29 +5726,29 @@
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A8" s="110" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B8" s="113" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D8" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E8" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F8" s="110" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G8" s="110" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J8" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K8" s="115" t="e">
         <v>#N/A</v>
@@ -5614,33 +5764,33 @@
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A9" s="110" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B9" s="113" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D9" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E9" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J9" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K9" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="L9" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N9" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O9" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5649,33 +5799,33 @@
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A10" s="110" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B10" s="113" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D10" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E10" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J10" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K10" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L10" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N10" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O10" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5684,33 +5834,33 @@
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A11" s="110" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B11" s="113" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D11" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E11" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J11" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K11" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L11" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N11" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O11" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5719,33 +5869,33 @@
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A12" s="110" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B12" s="113" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D12" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E12" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J12" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K12" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L12" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N12" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O12" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5754,39 +5904,39 @@
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A13" s="110" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B13" s="113" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D13" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E13" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F13" s="110" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G13" s="110" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J13" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K13" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L13" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N13" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O13" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5795,33 +5945,33 @@
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A14" s="110" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B14" s="113" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D14" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E14" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J14" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K14" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L14" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N14" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O14" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5830,33 +5980,33 @@
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A15" s="110" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B15" s="113" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D15" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E15" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J15" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K15" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L15" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N15" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O15" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5865,39 +6015,39 @@
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A16" s="110" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B16" s="113" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D16" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E16" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F16" s="110" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G16" s="110" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J16" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K16" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L16" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N16" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O16" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5906,36 +6056,36 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="110" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B17" s="113" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D17" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E17" s="110" t="str">
         <f t="shared" si="1"/>
         <v>!!!!!!!!!!!!!!!!!</v>
       </c>
       <c r="F17" s="110" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="J17" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K17" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L17" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N17" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O17" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5944,33 +6094,33 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="110" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B18" s="113" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D18" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E18" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J18" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K18" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L18" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N18" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O18" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5979,33 +6129,33 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="110" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B19" s="113" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D19" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E19" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J19" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K19" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="L19" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N19" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O19" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6014,33 +6164,33 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="110" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B20" s="113" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="113" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D20" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E20" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J20" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="K20" s="115" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="L20" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N20" s="110" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="O20" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6049,36 +6199,36 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="110" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B21" s="113" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D21" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E21" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F21" s="110" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="J21" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K21" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L21" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N21" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O21" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6087,33 +6237,33 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="110" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B22" s="113" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D22" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E22" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J22" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K22" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L22" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N22" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O22" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6122,33 +6272,33 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="110" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B23" s="113" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D23" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E23" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J23" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K23" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L23" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N23" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O23" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6157,33 +6307,33 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="110" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B24" s="113" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D24" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E24" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J24" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K24" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L24" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N24" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O24" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6192,33 +6342,33 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="110" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B25" s="113" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D25" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E25" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J25" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K25" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L25" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N25" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O25" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6227,33 +6377,33 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="110" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B26" s="113" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D26" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E26" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J26" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K26" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L26" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N26" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O26" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6262,33 +6412,33 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="110" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B27" s="113" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D27" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E27" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J27" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K27" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L27" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N27" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O27" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6297,33 +6447,33 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="110" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B28" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D28" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E28" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J28" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K28" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L28" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N28" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O28" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6332,33 +6482,33 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="110" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B29" s="113" t="s">
         <v>81</v>
       </c>
       <c r="C29" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D29" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E29" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J29" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K29" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L29" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N29" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O29" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6367,33 +6517,33 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="110" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B30" s="113" t="s">
         <v>82</v>
       </c>
       <c r="C30" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D30" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E30" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J30" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K30" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L30" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N30" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O30" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6402,33 +6552,33 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="110" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B31" s="113" t="s">
         <v>84</v>
       </c>
       <c r="C31" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D31" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E31" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J31" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K31" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L31" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N31" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O31" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6437,33 +6587,33 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="110" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B32" s="113" t="s">
         <v>85</v>
       </c>
       <c r="C32" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D32" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E32" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J32" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K32" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L32" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N32" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O32" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6472,33 +6622,33 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="110" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B33" s="113" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D33" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E33" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J33" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K33" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L33" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N33" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O33" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6507,33 +6657,33 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="110" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B34" s="113" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D34" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E34" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J34" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K34" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L34" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N34" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O34" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6542,33 +6692,33 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="110" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B35" s="113" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D35" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E35" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J35" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K35" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L35" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N35" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O35" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6577,33 +6727,33 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="110" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B36" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D36" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E36" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J36" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K36" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L36" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N36" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O36" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6612,33 +6762,33 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="110" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B37" s="113" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D37" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E37" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J37" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K37" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L37" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N37" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O37" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6647,33 +6797,33 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38" s="110" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B38" s="113" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D38" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E38" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J38" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K38" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L38" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N38" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O38" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6682,33 +6832,33 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" s="110" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B39" s="113" t="s">
         <v>94</v>
       </c>
       <c r="C39" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D39" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E39" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J39" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K39" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L39" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N39" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O39" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6717,33 +6867,33 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40" s="110" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B40" s="113" t="s">
         <v>95</v>
       </c>
       <c r="C40" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D40" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E40" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J40" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K40" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L40" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N40" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O40" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6752,33 +6902,33 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" s="110" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B41" s="113" t="s">
         <v>97</v>
       </c>
       <c r="C41" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D41" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E41" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J41" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K41" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L41" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N41" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O41" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6787,33 +6937,33 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" s="110" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B42" s="113" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D42" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E42" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J42" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K42" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L42" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N42" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O42" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6822,33 +6972,33 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="110" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B43" s="113" t="s">
         <v>100</v>
       </c>
       <c r="C43" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D43" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E43" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J43" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K43" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L43" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N43" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O43" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6857,33 +7007,33 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" s="110" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B44" s="113" t="s">
         <v>101</v>
       </c>
       <c r="C44" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D44" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E44" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J44" s="115" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K44" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L44" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N44" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O44" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6892,36 +7042,36 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45" s="110" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B45" s="113" t="s">
         <v>102</v>
       </c>
       <c r="C45" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D45" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E45" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G45" s="110" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J45" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K45" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L45" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N45" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O45" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6930,36 +7080,36 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46" s="110" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B46" s="113" t="s">
         <v>106</v>
       </c>
       <c r="C46" s="113" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D46" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E46" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G46" s="110" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J46" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K46" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L46" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N46" s="110" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="O46" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6968,33 +7118,33 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="110" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B47" s="113" t="s">
         <v>108</v>
       </c>
       <c r="C47" s="113" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D47" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E47" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J47" s="115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K47" s="115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L47" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N47" s="110" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O47" s="110" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
removed duplicates in current, changed datetime data class, testing flowGageHt
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CDC5EFE0-1D6B-5745-B7ED-93B41A3F79C6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A65BD8E-8C8C-3143-9CFF-6904FEF80BCC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35920" yWindow="3520" windowWidth="24220" windowHeight="14600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44960" yWindow="2500" windowWidth="24220" windowHeight="14600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="264">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -535,9 +535,6 @@
   </si>
   <si>
     <t>YEAR</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
   </si>
   <si>
     <t>VARCHAR(10)</t>
@@ -1034,13 +1031,16 @@
     <t>ALTER TABLE sensor ADD INDEX (site), ADD INDEX (date), ADD INDEX (timeEST);</t>
   </si>
   <si>
-    <t>has to be in "yyyy-mm-dd hh:mm:ss" format</t>
-  </si>
-  <si>
     <t xml:space="preserve">Excel formula: =CONCATENATE(B2, "_", TEXT(C2, "yyyymmdd"), "_", TEXT(D2,"[hh]mm")) this works if B2 is site, C2 is a date, and D2 is the time. </t>
   </si>
   <si>
     <t>Excel formula: '=IF(MONTH(C2)&gt;=6,YEAR(C2),YEAR(C2)-1) this works if C2 is formatted as a date</t>
+  </si>
+  <si>
+    <t>cannot have "%"</t>
+  </si>
+  <si>
+    <t>(DATETIME class was producing issues)</t>
   </si>
 </sst>
 </file>
@@ -2824,6 +2824,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72A0DE04-5F66-4342-8338-6345E7F740D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3140,10 +3194,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>163</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>164</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
@@ -3154,20 +3208,20 @@
         <v>43240</v>
       </c>
       <c r="B2" s="99" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="99" t="s">
         <v>165</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C3" s="99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D4" s="107" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -3175,39 +3229,39 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D6" s="107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D7" s="108"/>
       <c r="E7" s="108" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D10" s="107" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D11" s="108"/>
       <c r="E11" s="108" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="E12" s="108" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="D14" s="107" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -3239,22 +3293,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="H1" s="98" t="s">
         <v>156</v>
-      </c>
-      <c r="H1" s="98" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="117" x14ac:dyDescent="0.15">
@@ -3262,10 +3316,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -3276,7 +3330,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -3305,7 +3359,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H4" s="118" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -3326,7 +3380,7 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="99"/>
       <c r="D6" t="str">
@@ -3339,7 +3393,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C7" s="99"/>
       <c r="D7" t="str">
@@ -3365,7 +3419,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" t="str">
@@ -3378,7 +3432,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" t="str">
@@ -3391,7 +3445,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" t="str">
@@ -3404,7 +3458,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" t="str">
@@ -3430,7 +3484,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
@@ -3443,7 +3497,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
@@ -3646,8 +3700,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3662,25 +3716,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="103" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="I1" s="98" t="s">
         <v>156</v>
-      </c>
-      <c r="I1" s="98" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="247" x14ac:dyDescent="0.15">
@@ -3688,10 +3742,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" s="99"/>
       <c r="E2" t="str">
@@ -3700,10 +3754,10 @@
       </c>
       <c r="G2" s="100" t="str">
         <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31,E32,E33,E34,E35,E36,E37,E38,E39,E40,E41,E42,E43,E44,E45,E46,E47)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3734,7 +3788,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="I4" s="118" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -3756,10 +3810,10 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="99"/>
       <c r="E6" t="str">
@@ -3772,7 +3826,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C7" s="99"/>
       <c r="D7" s="99"/>
@@ -3800,7 +3854,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" s="99"/>
@@ -3814,7 +3868,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" s="99"/>
@@ -3828,7 +3882,7 @@
         <v>109</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" s="99"/>
@@ -3842,7 +3896,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" s="99"/>
@@ -3856,7 +3910,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C13" s="99"/>
       <c r="D13" s="99"/>
@@ -3884,7 +3938,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" s="99"/>
@@ -3898,7 +3952,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" s="99"/>
@@ -3943,7 +3997,7 @@
         <v>151</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D19" s="99"/>
       <c r="E19" t="str">
@@ -3959,7 +4013,7 @@
         <v>152</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D20" s="99"/>
       <c r="E20" t="str">
@@ -3972,15 +4026,15 @@
         <v>22</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D21" s="99"/>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime DATETIME, </v>
+        <v xml:space="preserve">datetime TEXT, </v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -3988,7 +4042,7 @@
         <v>66</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
@@ -4002,7 +4056,7 @@
         <v>70</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" s="99"/>
       <c r="D23" s="99"/>
@@ -4016,7 +4070,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" s="99"/>
       <c r="D24" s="99"/>
@@ -4030,7 +4084,7 @@
         <v>74</v>
       </c>
       <c r="B25" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" s="99"/>
       <c r="D25" s="99"/>
@@ -4044,7 +4098,7 @@
         <v>75</v>
       </c>
       <c r="B26" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C26" s="99"/>
       <c r="D26" s="99"/>
@@ -4058,7 +4112,7 @@
         <v>76</v>
       </c>
       <c r="B27" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C27" s="99"/>
       <c r="D27" s="99"/>
@@ -4072,7 +4126,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C28" s="99"/>
       <c r="D28" s="99"/>
@@ -4086,7 +4140,7 @@
         <v>81</v>
       </c>
       <c r="B29" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C29" s="99"/>
       <c r="D29" s="99"/>
@@ -4100,7 +4154,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C30" s="99"/>
       <c r="D30" s="99"/>
@@ -4114,7 +4168,7 @@
         <v>84</v>
       </c>
       <c r="B31" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C31" s="99"/>
       <c r="D31" s="99"/>
@@ -4128,7 +4182,7 @@
         <v>85</v>
       </c>
       <c r="B32" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C32" s="99"/>
       <c r="D32" s="99"/>
@@ -4142,7 +4196,7 @@
         <v>86</v>
       </c>
       <c r="B33" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C33" s="99"/>
       <c r="D33" s="99"/>
@@ -4156,7 +4210,7 @@
         <v>89</v>
       </c>
       <c r="B34" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C34" s="99"/>
       <c r="D34" s="99"/>
@@ -4170,7 +4224,7 @@
         <v>90</v>
       </c>
       <c r="B35" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C35" s="99"/>
       <c r="D35" s="99"/>
@@ -4184,7 +4238,7 @@
         <v>91</v>
       </c>
       <c r="B36" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C36" s="99"/>
       <c r="D36" s="99"/>
@@ -4198,7 +4252,7 @@
         <v>92</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C37" s="99"/>
       <c r="D37" s="99"/>
@@ -4212,7 +4266,7 @@
         <v>93</v>
       </c>
       <c r="B38" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C38" s="99"/>
       <c r="D38" s="99"/>
@@ -4226,7 +4280,7 @@
         <v>94</v>
       </c>
       <c r="B39" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" s="99"/>
       <c r="D39" s="99"/>
@@ -4240,7 +4294,7 @@
         <v>95</v>
       </c>
       <c r="B40" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C40" s="99"/>
       <c r="D40" s="99"/>
@@ -4254,7 +4308,7 @@
         <v>97</v>
       </c>
       <c r="B41" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C41" s="99"/>
       <c r="D41" s="99"/>
@@ -4268,7 +4322,7 @@
         <v>98</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C42" s="99"/>
       <c r="D42" s="99"/>
@@ -4282,7 +4336,7 @@
         <v>100</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C43" s="99"/>
       <c r="D43" s="99"/>
@@ -4296,7 +4350,7 @@
         <v>101</v>
       </c>
       <c r="B44" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C44" s="99"/>
       <c r="D44" s="99"/>
@@ -4310,7 +4364,7 @@
         <v>102</v>
       </c>
       <c r="B45" s="99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C45" s="99"/>
       <c r="D45" s="99"/>
@@ -4338,7 +4392,7 @@
         <v>108</v>
       </c>
       <c r="B47" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C47" s="99"/>
       <c r="D47" s="99"/>
@@ -4349,7 +4403,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4362,7 +4416,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4378,22 +4432,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="H1" s="98" t="s">
         <v>156</v>
-      </c>
-      <c r="H1" s="98" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="234" x14ac:dyDescent="0.15">
@@ -4401,10 +4455,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -4412,10 +4466,10 @@
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -4444,7 +4498,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H4" s="118" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -4465,10 +4519,10 @@
         <v>137</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -4493,7 +4547,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" t="str">
@@ -4506,7 +4560,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" t="str">
@@ -4519,7 +4573,7 @@
         <v>109</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="99"/>
       <c r="D10" t="str">
@@ -4532,7 +4586,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="99"/>
       <c r="D11" t="str">
@@ -4545,7 +4599,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" t="str">
@@ -4571,7 +4625,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
@@ -4584,7 +4638,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
@@ -4626,7 +4680,7 @@
         <v>151</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -4641,7 +4695,7 @@
         <v>152</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -4653,14 +4707,14 @@
         <v>22</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime DATETIME, </v>
+        <v xml:space="preserve">datetime TEXT, </v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -4668,7 +4722,7 @@
         <v>66</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C21" s="99"/>
       <c r="D21" t="str">
@@ -4681,7 +4735,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" t="str">
@@ -4694,7 +4748,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" s="99"/>
       <c r="D23" t="str">
@@ -4707,7 +4761,7 @@
         <v>74</v>
       </c>
       <c r="B24" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" s="99"/>
       <c r="D24" t="str">
@@ -4720,7 +4774,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" s="99"/>
       <c r="D25" t="str">
@@ -4733,7 +4787,7 @@
         <v>76</v>
       </c>
       <c r="B26" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C26" s="99"/>
       <c r="D26" t="str">
@@ -4746,10 +4800,10 @@
         <v>78</v>
       </c>
       <c r="B27" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C27" s="99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -4761,7 +4815,7 @@
         <v>81</v>
       </c>
       <c r="B28" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C28" s="99"/>
       <c r="D28" t="str">
@@ -4774,7 +4828,7 @@
         <v>82</v>
       </c>
       <c r="B29" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C29" s="99"/>
       <c r="D29" t="str">
@@ -4787,7 +4841,7 @@
         <v>84</v>
       </c>
       <c r="B30" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C30" s="99"/>
       <c r="D30" t="str">
@@ -4800,7 +4854,7 @@
         <v>85</v>
       </c>
       <c r="B31" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C31" s="99"/>
       <c r="D31" t="str">
@@ -4813,7 +4867,7 @@
         <v>86</v>
       </c>
       <c r="B32" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C32" s="99"/>
       <c r="D32" t="str">
@@ -4826,7 +4880,7 @@
         <v>89</v>
       </c>
       <c r="B33" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C33" s="99"/>
       <c r="D33" t="str">
@@ -4839,7 +4893,7 @@
         <v>90</v>
       </c>
       <c r="B34" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C34" s="99"/>
       <c r="D34" t="str">
@@ -4852,7 +4906,7 @@
         <v>91</v>
       </c>
       <c r="B35" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C35" s="99"/>
       <c r="D35" t="str">
@@ -4865,7 +4919,7 @@
         <v>92</v>
       </c>
       <c r="B36" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C36" s="99"/>
       <c r="D36" t="str">
@@ -4878,7 +4932,7 @@
         <v>93</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C37" s="99"/>
       <c r="D37" t="str">
@@ -4891,7 +4945,7 @@
         <v>94</v>
       </c>
       <c r="B38" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C38" s="99"/>
       <c r="D38" t="str">
@@ -4904,7 +4958,7 @@
         <v>95</v>
       </c>
       <c r="B39" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" s="99"/>
       <c r="D39" t="str">
@@ -4917,7 +4971,7 @@
         <v>97</v>
       </c>
       <c r="B40" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C40" s="99"/>
       <c r="D40" t="str">
@@ -4930,7 +4984,7 @@
         <v>98</v>
       </c>
       <c r="B41" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C41" s="99"/>
       <c r="D41" t="str">
@@ -4943,7 +4997,7 @@
         <v>100</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C42" s="99"/>
       <c r="D42" t="str">
@@ -4956,9 +5010,11 @@
         <v>101</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>248</v>
-      </c>
-      <c r="C43" s="99"/>
+        <v>247</v>
+      </c>
+      <c r="C43" s="99" t="s">
+        <v>262</v>
+      </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ionError DECIMAL(8,4), </v>
@@ -4969,7 +5025,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C44" s="99"/>
       <c r="D44" t="str">
@@ -4995,7 +5051,7 @@
         <v>108</v>
       </c>
       <c r="B46" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C46" s="99"/>
       <c r="D46" t="str">
@@ -5029,22 +5085,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>176</v>
       </c>
       <c r="C1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="G1" s="98" t="s">
         <v>156</v>
-      </c>
-      <c r="G1" s="98" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
@@ -5052,10 +5108,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -5066,7 +5122,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
       </c>
       <c r="G2" s="102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -5096,7 +5152,7 @@
       </c>
       <c r="F4" s="100"/>
       <c r="G4" s="118" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -5134,10 +5190,10 @@
         <v>48</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7:D8" si="1">CONCATENATE(A7, " ",  B7, ", ")</f>
@@ -5150,10 +5206,10 @@
         <v>56</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
@@ -5400,399 +5456,399 @@
   <sheetData>
     <row r="1" spans="1:62" s="111" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="111" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="116" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="117" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="116" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="117" t="s">
-        <v>231</v>
-      </c>
       <c r="D1" s="112" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E1" s="110"/>
       <c r="F1" s="110" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G1" s="110" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H1" s="110"/>
       <c r="I1" s="110"/>
       <c r="J1" s="114" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="L1" s="112" t="s">
         <v>233</v>
-      </c>
-      <c r="L1" s="112" t="s">
-        <v>234</v>
       </c>
       <c r="M1" s="112" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A2" s="110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" s="113" t="s">
         <v>144</v>
       </c>
       <c r="C2" s="113" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="110" t="str">
         <f>IF(C2=D2, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J2" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K2" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L2" s="110" t="str">
         <f t="shared" ref="L2:L47" si="0">IF(J2=K2, " ", "!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N2" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O2" s="110" t="str">
         <f>IF(C2=N2, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Q2" s="110" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R2" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U2" s="110" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="W2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AA2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AC2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AF2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AG2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AI2" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AJ2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AK2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AL2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AM2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AN2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AO2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AQ2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AR2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AS2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AT2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AW2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AX2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AZ2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BA2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BB2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BC2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BD2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BE2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BF2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BG2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BH2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BI2" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BJ2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="110" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="113" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E3" s="110" t="str">
         <f t="shared" ref="E3:E47" si="1">IF(C3=D3, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J3" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K3" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L3" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N3" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O3" s="110" t="str">
         <f t="shared" ref="O3:O47" si="2">IF(C3=N3, " ", "!!!!!!!!!!!!!!!!!")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P3" s="110" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A4" s="110" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="113" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J4" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K4" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L4" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N4" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O4" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P4" s="110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A5" s="110" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="113" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="110" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J5" s="115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K5" s="115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L5" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N5" s="110" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O5" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P5" s="110" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A6" s="110" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B6" s="113" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J6" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K6" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L6" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="M6" s="110" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N6" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O6" s="110" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P6" s="110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A7" s="110" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B7" s="113" t="s">
         <v>137</v>
       </c>
       <c r="C7" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J7" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K7" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L7" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N7" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O7" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5801,29 +5857,29 @@
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A8" s="110" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8" s="113" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F8" s="110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G8" s="110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J8" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K8" s="115" t="e">
         <v>#N/A</v>
@@ -5839,33 +5895,33 @@
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A9" s="110" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B9" s="113" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J9" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K9" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L9" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N9" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O9" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5874,33 +5930,33 @@
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A10" s="110" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" s="113" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J10" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K10" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L10" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N10" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O10" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5909,33 +5965,33 @@
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A11" s="110" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="113" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E11" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J11" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K11" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L11" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N11" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O11" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5944,33 +6000,33 @@
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A12" s="110" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" s="113" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E12" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J12" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K12" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L12" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N12" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="110" t="str">
         <f t="shared" si="2"/>
@@ -5979,39 +6035,39 @@
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A13" s="110" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="113" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D13" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E13" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F13" s="110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G13" s="110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J13" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K13" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L13" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N13" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O13" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6020,33 +6076,33 @@
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A14" s="110" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14" s="113" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D14" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J14" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K14" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L14" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N14" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O14" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6055,33 +6111,33 @@
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A15" s="110" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B15" s="113" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J15" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K15" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L15" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N15" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O15" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6090,39 +6146,39 @@
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A16" s="110" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="113" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D16" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F16" s="110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G16" s="110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J16" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K16" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L16" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N16" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O16" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6131,36 +6187,36 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="110" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="113" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D17" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E17" s="110" t="str">
         <f t="shared" si="1"/>
         <v>!!!!!!!!!!!!!!!!!</v>
       </c>
       <c r="F17" s="110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J17" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K17" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L17" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N17" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O17" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6169,33 +6225,33 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="110" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" s="113" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J18" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L18" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N18" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O18" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6204,33 +6260,33 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="110" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" s="113" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E19" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J19" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K19" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L19" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N19" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O19" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6239,33 +6295,33 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="110" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B20" s="113" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="113" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D20" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E20" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J20" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K20" s="115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L20" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N20" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O20" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6274,36 +6330,36 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="110" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B21" s="113" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E21" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F21" s="110" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J21" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K21" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L21" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N21" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O21" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6312,33 +6368,33 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" s="113" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J22" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K22" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L22" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N22" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O22" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6347,33 +6403,33 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="113" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J23" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K23" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L23" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N23" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O23" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6382,33 +6438,33 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="113" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J24" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K24" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L24" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N24" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O24" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6417,33 +6473,33 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="113" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D25" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J25" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K25" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L25" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N25" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O25" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6452,33 +6508,33 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="113" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D26" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J26" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K26" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L26" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N26" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O26" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6487,33 +6543,33 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" s="113" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D27" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J27" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K27" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L27" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N27" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O27" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6522,33 +6578,33 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="110" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B28" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D28" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J28" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K28" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L28" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N28" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O28" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6557,33 +6613,33 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B29" s="113" t="s">
         <v>81</v>
       </c>
       <c r="C29" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D29" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E29" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J29" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K29" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L29" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N29" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O29" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6592,33 +6648,33 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="110" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B30" s="113" t="s">
         <v>82</v>
       </c>
       <c r="C30" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D30" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E30" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J30" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K30" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L30" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N30" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O30" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6627,33 +6683,33 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" s="113" t="s">
         <v>84</v>
       </c>
       <c r="C31" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D31" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E31" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J31" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K31" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L31" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N31" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O31" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6662,33 +6718,33 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="113" t="s">
         <v>85</v>
       </c>
       <c r="C32" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E32" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J32" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K32" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L32" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N32" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O32" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6697,33 +6753,33 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="110" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B33" s="113" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D33" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E33" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J33" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K33" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L33" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N33" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O33" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6732,33 +6788,33 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="113" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D34" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E34" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J34" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K34" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L34" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N34" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O34" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6767,33 +6823,33 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B35" s="113" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D35" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E35" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J35" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K35" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L35" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N35" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O35" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6802,33 +6858,33 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B36" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D36" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E36" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J36" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K36" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L36" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N36" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O36" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6837,33 +6893,33 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B37" s="113" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D37" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E37" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J37" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K37" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L37" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N37" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O37" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6872,33 +6928,33 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38" s="110" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B38" s="113" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D38" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E38" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J38" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K38" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L38" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N38" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O38" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6907,33 +6963,33 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" s="113" t="s">
         <v>94</v>
       </c>
       <c r="C39" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D39" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E39" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J39" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K39" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L39" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N39" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O39" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6942,33 +6998,33 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40" s="110" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" s="113" t="s">
         <v>95</v>
       </c>
       <c r="C40" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D40" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E40" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J40" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K40" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L40" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N40" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O40" s="110" t="str">
         <f t="shared" si="2"/>
@@ -6977,33 +7033,33 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" s="110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B41" s="113" t="s">
         <v>97</v>
       </c>
       <c r="C41" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D41" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E41" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J41" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K41" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L41" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N41" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O41" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7012,33 +7068,33 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" s="110" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B42" s="113" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D42" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E42" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J42" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K42" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L42" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N42" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O42" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7047,33 +7103,33 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B43" s="113" t="s">
         <v>100</v>
       </c>
       <c r="C43" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D43" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E43" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J43" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K43" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L43" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N43" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O43" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7082,33 +7138,33 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" s="110" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B44" s="113" t="s">
         <v>101</v>
       </c>
       <c r="C44" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D44" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E44" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J44" s="115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K44" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L44" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N44" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O44" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7117,36 +7173,36 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45" s="110" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B45" s="113" t="s">
         <v>102</v>
       </c>
       <c r="C45" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D45" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E45" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G45" s="110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J45" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K45" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L45" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N45" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O45" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7155,36 +7211,36 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46" s="110" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B46" s="113" t="s">
         <v>106</v>
       </c>
       <c r="C46" s="113" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D46" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E46" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G46" s="110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J46" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K46" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L46" s="110" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N46" s="110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O46" s="110" t="str">
         <f t="shared" si="2"/>
@@ -7193,33 +7249,33 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="110" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" s="113" t="s">
         <v>108</v>
       </c>
       <c r="C47" s="113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D47" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E47" s="110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J47" s="115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K47" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L47" s="110" t="str">
         <f t="shared" si="0"/>
         <v>!!!</v>
       </c>
       <c r="N47" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O47" s="110" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
transferring historical & initial data; increases size of flowGageHt data
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A65BD8E-8C8C-3143-9CFF-6904FEF80BCC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C8CC8DD1-5C43-124D-8A7B-6099C8E55A38}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44960" yWindow="2500" windowWidth="24220" windowHeight="14600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44960" yWindow="2500" windowWidth="24220" windowHeight="14600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="265">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -1010,12 +1010,6 @@
     <t>INT PRIMARY KEY NOT NULL AUTO_INCREMENT</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
-  </si>
-  <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime DATETIME, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
-  </si>
-  <si>
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4)</t>
   </si>
   <si>
@@ -1041,6 +1035,15 @@
   </si>
   <si>
     <t>(DATETIME class was producing issues)</t>
+  </si>
+  <si>
+    <t>DECIMAL(16,4)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </t>
   </si>
 </sst>
 </file>
@@ -2878,6 +2881,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F908A1E1-15B7-F04E-8A7E-06B5F346F70D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3359,7 +3416,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H4" s="118" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -3700,8 +3757,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3754,10 +3811,10 @@
       </c>
       <c r="G2" s="100" t="str">
         <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31,E32,E33,E34,E35,E36,E37,E38,E39,E40,E41,E42,E43,E44,E45,E46,E47)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3788,7 +3845,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="I4" s="118" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -3938,13 +3995,13 @@
         <v>42</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" s="99"/>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -3997,7 +4054,7 @@
         <v>151</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D19" s="99"/>
       <c r="E19" t="str">
@@ -4013,7 +4070,7 @@
         <v>152</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D20" s="99"/>
       <c r="E20" t="str">
@@ -4029,7 +4086,7 @@
         <v>150</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D21" s="99"/>
       <c r="E21" t="str">
@@ -4416,8 +4473,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4450,7 +4507,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="234" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="221" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -4466,10 +4523,10 @@
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -4498,7 +4555,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H4" s="118" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -4625,12 +4682,12 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -4680,7 +4737,7 @@
         <v>151</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -4695,7 +4752,7 @@
         <v>152</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -4710,7 +4767,7 @@
         <v>150</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -5013,7 +5070,7 @@
         <v>247</v>
       </c>
       <c r="C43" s="99" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -5122,7 +5179,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
       </c>
       <c r="G2" s="102" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -5152,7 +5209,7 @@
       </c>
       <c r="F4" s="100"/>
       <c r="G4" s="118" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added units to DataStructures sheet
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C8CC8DD1-5C43-124D-8A7B-6099C8E55A38}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{28B2AC44-24C8-FD47-8178-781271B77728}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44960" yWindow="2500" windowWidth="24220" windowHeight="14600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="14600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="historical" sheetId="5" r:id="rId4"/>
     <sheet name="sensor" sheetId="6" r:id="rId5"/>
     <sheet name="RClasses" sheetId="8" r:id="rId6"/>
-    <sheet name="AlmostFinalNames" sheetId="1" r:id="rId7"/>
-    <sheet name="CreatingCommonNames" sheetId="2" r:id="rId8"/>
+    <sheet name="units" sheetId="9" r:id="rId7"/>
+    <sheet name="AlmostFinalNames" sheetId="1" r:id="rId8"/>
+    <sheet name="CreatingCommonNames" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="268">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -1045,12 +1046,21 @@
   <si>
     <t xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </t>
   </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L/s </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1331,8 +1341,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1441,6 +1464,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -1517,7 +1546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1751,6 +1780,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2935,6 +2977,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9745D9B7-2050-6B4E-9860-620219D52ECE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3757,8 +3853,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4473,8 +4569,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7356,6 +7452,1360 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6260233-ECAC-3248-955E-10E3D058E348}">
+  <dimension ref="A1:C1001"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="A15:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" style="120" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="120" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="120" customWidth="1"/>
+    <col min="4" max="16384" width="14.5" style="120"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="119" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="120" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="121"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="121"/>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="120" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="121"/>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="120" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="121"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="120" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="120" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="121"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="121"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="120" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="120" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="120" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="120" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="120" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="121"/>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="120" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="121"/>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="120" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="121"/>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="120" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="120" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="123" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="120" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="120" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="120" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="120" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="120" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="120" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="120" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="120" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="120" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="120" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="120" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="120" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="120" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="120" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="120" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="120" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="120" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="120" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="120" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="120" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="122"/>
+    </row>
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="122"/>
+    </row>
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="16" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:X1003"/>
@@ -33794,12 +35244,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
small clean up, and commenting out most rhandsontable stuff
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{24553989-14B4-AA49-BF8B-D9E0A37BA992}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E4327B4-9B37-B64E-ADC7-E38F6EAC483E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="14600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="14600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="272">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -1061,6 +1061,12 @@
   <si>
     <t>mm/hr</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>REMOVE</t>
+  </si>
 </sst>
 </file>
 
@@ -1804,7 +1810,38 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B833727B-C21B-184C-BD4D-3DD48398FB48}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -3091,6 +3128,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF75CF6-8BA0-9D4C-9971-8CF292524CAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10109200" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3488,10 +3579,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B63FAF-B35B-BB4D-A7FB-6A2BC573DBFB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3539,7 +3630,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,)</f>
+        <f>CONCATENATE(D2,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,)</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
@@ -3548,62 +3639,65 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="99" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="99"/>
+        <v>151</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>258</v>
+      </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D18" si="0">CONCATENATE(A3, " ",  B3, ", ")</f>
-        <v xml:space="preserve">site VARCHAR(20), </v>
-      </c>
+        <f>CONCATENATE(A3, " ",  B3, ", ")</f>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+      <c r="H3" s="101"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="99" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">date DATE, </v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>254</v>
+        <f t="shared" ref="D4:D19" si="0">CONCATENATE(A4, " ",  B4, ", ")</f>
+        <v xml:space="preserve">site VARCHAR(20), </v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="99"/>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">timeEST TIME, </v>
+        <v xml:space="preserve">date DATE, </v>
+      </c>
+      <c r="H5" s="118" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="99" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="C6" s="99"/>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(8,4), </v>
+        <v xml:space="preserve">timeEST TIME, </v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="99" t="s">
-        <v>26</v>
+      <c r="A7" s="104" t="s">
+        <v>137</v>
       </c>
       <c r="B7" s="99" t="s">
         <v>247</v>
@@ -3611,38 +3705,41 @@
       <c r="C7" s="99"/>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
-      </c>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
+      </c>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="99" t="s">
-        <v>30</v>
+      <c r="A8" s="104" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DIC SMALLINT, </v>
-      </c>
+        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
+      </c>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="99" t="s">
-        <v>34</v>
+      <c r="A9" s="104" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>247</v>
+        <v>148</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
-      </c>
+        <v xml:space="preserve">DIC SMALLINT, </v>
+      </c>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="99" t="s">
-        <v>36</v>
+      <c r="A10" s="104" t="s">
+        <v>34</v>
       </c>
       <c r="B10" s="99" t="s">
         <v>247</v>
@@ -3650,12 +3747,13 @@
       <c r="C10" s="99"/>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(8,4), </v>
-      </c>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
+      </c>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="99" t="s">
-        <v>37</v>
+      <c r="A11" s="104" t="s">
+        <v>36</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>247</v>
@@ -3663,12 +3761,13 @@
       <c r="C11" s="99"/>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
-      </c>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
+      </c>
+      <c r="F11" s="123"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="99" t="s">
-        <v>38</v>
+      <c r="A12" s="104" t="s">
+        <v>37</v>
       </c>
       <c r="B12" s="99" t="s">
         <v>247</v>
@@ -3676,91 +3775,101 @@
       <c r="C12" s="99"/>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
-      </c>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
+      </c>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="99" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>145</v>
+        <v>247</v>
       </c>
       <c r="C13" s="99"/>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
-      </c>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+      </c>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>248</v>
+        <v>145</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
+        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="99" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="99" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="99" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">notes TEXT, </v>
+        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="99" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
+        <v xml:space="preserve">notes TEXT, </v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="99"/>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
         <v xml:space="preserve">archived VARCHAR(20), </v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="99"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="99"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="99"/>
@@ -3768,7 +3877,9 @@
       <c r="C20" s="99"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="99"/>
+      <c r="A21" s="105" t="s">
+        <v>160</v>
+      </c>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
     </row>
@@ -3902,7 +4013,18 @@
       <c r="B47" s="99"/>
       <c r="C47" s="99"/>
     </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="99"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="99"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="F7:F13">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3911,716 +4033,791 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A8635-60E1-404A-9A09-732833EFAF77}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A47"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="7" max="7" width="50.5" customWidth="1"/>
-    <col min="9" max="9" width="50.5" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="8" max="8" width="50.5" customWidth="1"/>
+    <col min="10" max="10" width="50.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B1" s="103" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="C1" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="D1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="E1" s="103" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="F1" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="H1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="98" t="s">
+      <c r="J1" s="98" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="247" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="247" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="99" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="C2" s="99" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="99" t="s">
+      <c r="D2" s="99" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" t="str">
-        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
+      <c r="E2" s="99"/>
+      <c r="F2" t="str">
+        <f>CONCATENATE(B2, " ",  C2, ", ")</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
-      <c r="G2" s="100" t="str">
-        <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31,E32,E33,E34,E35,E36,E37,E38,E39,E40,E41,E42,E43,E44,E45,E46,E47)</f>
+      <c r="H2" s="100" t="str">
+        <f>CONCATENATE(F2,F3,F4,F5,F6,F7,F8,F9,F10,F11,F12,F13,F14,F15,F16,F17,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28,F29,F30,F31,F32,F33,F34,F35,F36,F37,F38,F39,F40,F41,F42,F43,F44,F45,F46,F47)</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="J2" s="101" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="C3" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="99"/>
       <c r="D3" s="99"/>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E47" si="0">CONCATENATE(A3, " ",  B3, ", ")</f>
+      <c r="E3" s="99"/>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F47" si="0">CONCATENATE(B3, " ",  C3, ", ")</f>
         <v xml:space="preserve">site VARCHAR(20), </v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H3" s="99"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="C4" s="99" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="99"/>
       <c r="D4" s="99"/>
-      <c r="E4" t="str">
+      <c r="E4" s="99"/>
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">date DATE, </v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="H4" s="99"/>
+      <c r="J4" s="118" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="C5" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="99"/>
       <c r="D5" s="99"/>
-      <c r="E5" t="str">
+      <c r="E5" s="99"/>
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">timeEST TIME, </v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="104" t="s">
+      <c r="H5" s="99"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="104" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="C6" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="D6" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" t="str">
+      <c r="E6" s="99"/>
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">pH DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="104" t="s">
+      <c r="H6" s="99"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="99" t="s">
+      <c r="C7" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="99"/>
       <c r="D7" s="99"/>
-      <c r="E7" t="str">
+      <c r="E7" s="99"/>
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" s="104" t="s">
+      <c r="H7" s="99"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="C8" s="99" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="99"/>
       <c r="D8" s="99"/>
-      <c r="E8" t="str">
+      <c r="E8" s="99"/>
+      <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">DIC SMALLINT, </v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="104" t="s">
+      <c r="H8" s="99"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="C9" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="99"/>
       <c r="D9" s="99"/>
-      <c r="E9" t="str">
+      <c r="E9" s="99"/>
+      <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">spCond DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="104" t="s">
+      <c r="H9" s="99"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="C10" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C10" s="99"/>
       <c r="D10" s="99"/>
-      <c r="E10" t="str">
+      <c r="E10" s="99"/>
+      <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">temp DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A11" s="104" t="s">
+      <c r="H10" s="99"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="104" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="C11" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C11" s="99"/>
       <c r="D11" s="99"/>
-      <c r="E11" t="str">
+      <c r="E11" s="99"/>
+      <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="104" t="s">
+      <c r="H11" s="99"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="99" t="s">
+      <c r="C12" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C12" s="99"/>
       <c r="D12" s="99"/>
-      <c r="E12" t="str">
+      <c r="E12" s="99"/>
+      <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H12" s="99"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="C13" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C13" s="99"/>
       <c r="D13" s="99"/>
-      <c r="E13" t="str">
+      <c r="E13" s="99"/>
+      <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H13" s="99"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="C14" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="99"/>
       <c r="D14" s="99"/>
-      <c r="E14" t="str">
+      <c r="E14" s="99"/>
+      <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H14" s="99"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="C15" s="99" t="s">
         <v>262</v>
       </c>
-      <c r="C15" s="99"/>
       <c r="D15" s="99"/>
-      <c r="E15" t="str">
+      <c r="E15" s="99"/>
+      <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H15" s="99"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B16" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="C16" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C16" s="99"/>
       <c r="D16" s="99"/>
-      <c r="E16" t="str">
+      <c r="E16" s="99"/>
+      <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="H16" s="99"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="C17" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="99"/>
       <c r="D17" s="99"/>
-      <c r="E17" t="str">
+      <c r="E17" s="99"/>
+      <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">fieldCode VARCHAR(50), </v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="H17" s="99"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="99" t="s">
+      <c r="C18" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="99"/>
       <c r="D18" s="99"/>
-      <c r="E18" t="str">
+      <c r="E18" s="99"/>
+      <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">notes TEXT, </v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="99" t="s">
+      <c r="H18" s="99"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="99"/>
+      <c r="B19" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="C19" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="99" t="s">
+      <c r="D19" s="99" t="s">
         <v>258</v>
       </c>
-      <c r="D19" s="99"/>
-      <c r="E19" t="str">
+      <c r="E19" s="99"/>
+      <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="99" t="s">
+      <c r="H19" s="99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="C20" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="99" t="s">
+      <c r="D20" s="99" t="s">
         <v>259</v>
       </c>
-      <c r="D20" s="99"/>
-      <c r="E20" t="str">
+      <c r="E20" s="99"/>
+      <c r="F20" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">waterYr YEAR, </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="99" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="99" t="s">
+      <c r="C21" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="D21" s="99" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="99"/>
-      <c r="E21" t="str">
+      <c r="E21" s="99"/>
+      <c r="F21" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">datetime TEXT, </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="104" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="C22" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C22" s="99"/>
       <c r="D22" s="99"/>
-      <c r="E22" t="str">
+      <c r="E22" s="99"/>
+      <c r="F22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Ca DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="104" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="C23" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C23" s="99"/>
       <c r="D23" s="99"/>
-      <c r="E23" t="str">
+      <c r="E23" s="99"/>
+      <c r="F23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Mg DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="104" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="C24" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C24" s="99"/>
       <c r="D24" s="99"/>
-      <c r="E24" t="str">
+      <c r="E24" s="99"/>
+      <c r="F24" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">K DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="104" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="99" t="s">
+      <c r="C25" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C25" s="99"/>
       <c r="D25" s="99"/>
-      <c r="E25" t="str">
+      <c r="E25" s="99"/>
+      <c r="F25" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Na DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="104" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B26" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="99" t="s">
+      <c r="C26" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C26" s="99"/>
       <c r="D26" s="99"/>
-      <c r="E26" t="str">
+      <c r="E26" s="99"/>
+      <c r="F26" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="104" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B27" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="C27" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C27" s="99"/>
       <c r="D27" s="99"/>
-      <c r="E27" t="str">
+      <c r="E27" s="99"/>
+      <c r="F27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="104" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B28" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="99" t="s">
+      <c r="C28" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C28" s="99"/>
       <c r="D28" s="99"/>
-      <c r="E28" t="str">
+      <c r="E28" s="99"/>
+      <c r="F28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="104" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B29" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="99" t="s">
+      <c r="C29" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C29" s="99"/>
       <c r="D29" s="99"/>
-      <c r="E29" t="str">
+      <c r="E29" s="99"/>
+      <c r="F29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="104" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B30" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="99" t="s">
+      <c r="C30" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C30" s="99"/>
       <c r="D30" s="99"/>
-      <c r="E30" t="str">
+      <c r="E30" s="99"/>
+      <c r="F30" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="104" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B31" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="99" t="s">
+      <c r="C31" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C31" s="99"/>
       <c r="D31" s="99"/>
-      <c r="E31" t="str">
+      <c r="E31" s="99"/>
+      <c r="F31" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="104" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B32" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="99" t="s">
+      <c r="C32" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C32" s="99"/>
       <c r="D32" s="99"/>
-      <c r="E32" t="str">
+      <c r="E32" s="99"/>
+      <c r="F32" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Cl DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="104" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B33" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="99" t="s">
+      <c r="C33" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="99"/>
       <c r="D33" s="99"/>
-      <c r="E33" t="str">
+      <c r="E33" s="99"/>
+      <c r="F33" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="104" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B34" s="104" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="99" t="s">
+      <c r="C34" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C34" s="99"/>
       <c r="D34" s="99"/>
-      <c r="E34" t="str">
+      <c r="E34" s="99"/>
+      <c r="F34" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">DOC DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="104" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B35" s="104" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="C35" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C35" s="99"/>
       <c r="D35" s="99"/>
-      <c r="E35" t="str">
+      <c r="E35" s="99"/>
+      <c r="F35" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">TDN DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="104" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B36" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="99" t="s">
+      <c r="C36" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C36" s="99"/>
       <c r="D36" s="99"/>
-      <c r="E36" t="str">
+      <c r="E36" s="99"/>
+      <c r="F36" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">DON DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="104" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B37" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="99" t="s">
+      <c r="C37" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="99"/>
       <c r="D37" s="99"/>
-      <c r="E37" t="str">
+      <c r="E37" s="99"/>
+      <c r="F37" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="104" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B38" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="99" t="s">
+      <c r="C38" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="99"/>
       <c r="D38" s="99"/>
-      <c r="E38" t="str">
+      <c r="E38" s="99"/>
+      <c r="F38" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Mn DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="104" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B39" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="99" t="s">
+      <c r="C39" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C39" s="99"/>
       <c r="D39" s="99"/>
-      <c r="E39" t="str">
+      <c r="E39" s="99"/>
+      <c r="F39" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Fe DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="104" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B40" s="104" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="99" t="s">
+      <c r="C40" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C40" s="99"/>
       <c r="D40" s="99"/>
-      <c r="E40" t="str">
+      <c r="E40" s="99"/>
+      <c r="F40" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">F DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="104" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B41" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="99" t="s">
+      <c r="C41" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C41" s="99"/>
       <c r="D41" s="99"/>
-      <c r="E41" t="str">
+      <c r="E41" s="99"/>
+      <c r="F41" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="104" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B42" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="99" t="s">
+      <c r="C42" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C42" s="99"/>
       <c r="D42" s="99"/>
-      <c r="E42" t="str">
+      <c r="E42" s="99"/>
+      <c r="F42" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="104" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B43" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="99" t="s">
+      <c r="C43" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="99"/>
       <c r="D43" s="99"/>
-      <c r="E43" t="str">
+      <c r="E43" s="99"/>
+      <c r="F43" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="99" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B44" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="99" t="s">
+      <c r="C44" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C44" s="99"/>
       <c r="D44" s="99"/>
-      <c r="E44" t="str">
+      <c r="E44" s="99"/>
+      <c r="F44" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ionError DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="99" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B45" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="99" t="s">
+      <c r="C45" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="99"/>
       <c r="D45" s="99"/>
-      <c r="E45" t="str">
+      <c r="E45" s="99"/>
+      <c r="F45" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">duplicate VARCHAR(10), </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="99" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B46" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="99" t="s">
+      <c r="C46" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="99"/>
       <c r="D46" s="99"/>
-      <c r="E46" t="str">
+      <c r="E46" s="99"/>
+      <c r="F46" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">sampleType VARCHAR(20), </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="104" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B47" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="99" t="s">
+      <c r="C47" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C47" s="99"/>
       <c r="D47" s="99"/>
-      <c r="E47" t="str">
+      <c r="E47" s="99"/>
+      <c r="F47" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="105" t="s">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B50" s="105" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576 H3:H19">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7515,7 +7712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6260233-ECAC-3248-955E-10E3D058E348}">
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
committing tiny change in comment to make merge possible
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1255B149-7A9B-8E40-88C4-D1FECEC0C08A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{77E07DFC-F407-5A49-8AB9-A28C3C477C29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="21640" windowHeight="14600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="21640" windowHeight="14600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="203">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -858,7 +858,7 @@
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
   </si>
 </sst>
 </file>
@@ -3415,10 +3415,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B63FAF-B35B-BB4D-A7FB-6A2BC573DBFB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3451,7 +3451,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="130" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="143" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -3466,8 +3466,8 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
+        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
         <v>202</v>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="C4" s="99"/>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D20" si="0">CONCATENATE(A4, " ",  B4, ", ")</f>
+        <f t="shared" ref="D4:D21" si="0">CONCATENATE(A4, " ",  B4, ", ")</f>
         <v xml:space="preserve">site VARCHAR(20), </v>
       </c>
     </row>
@@ -3631,111 +3631,120 @@
       <c r="F13" s="115"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="99" t="s">
-        <v>38</v>
+      <c r="A14" s="104" t="s">
+        <v>109</v>
       </c>
       <c r="B14" s="99" t="s">
         <v>177</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+        <f t="shared" ref="D14" si="1">CONCATENATE(A14, " ",  B14, ", ")</f>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
       </c>
       <c r="F14" s="115"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="99" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
-      </c>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+      </c>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
+        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="99" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="99" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="99" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" s="99"/>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">notes TEXT, </v>
+        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="99" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C20" s="99"/>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
+        <v xml:space="preserve">notes TEXT, </v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="99"/>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
         <v xml:space="preserve">archived VARCHAR(20), </v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="99"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="105" t="s">
-        <v>160</v>
-      </c>
+      <c r="A22" s="99"/>
       <c r="B22" s="99"/>
       <c r="C22" s="99"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="99"/>
+      <c r="A23" s="105" t="s">
+        <v>160</v>
+      </c>
       <c r="B23" s="99"/>
       <c r="C23" s="99"/>
     </row>
@@ -3869,11 +3878,16 @@
       <c r="B49" s="99"/>
       <c r="C49" s="99"/>
     </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="99"/>
+      <c r="B50" s="99"/>
+      <c r="C50" s="99"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F14">
+  <conditionalFormatting sqref="F8:F15">
     <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
+  <conditionalFormatting sqref="A23">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
@@ -3888,7 +3902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
@@ -6193,7 +6207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6260233-ECAC-3248-955E-10E3D058E348}">
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding documentation (data templates, data template examples, dashboard documentation)
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{77E07DFC-F407-5A49-8AB9-A28C3C477C29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F62333CE-27AF-A64C-804C-9E29F2CCACF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="21640" windowHeight="14600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42240" yWindow="800" windowWidth="21640" windowHeight="14600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="203">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -786,9 +786,6 @@
     <t>DECIMAL(8,4)</t>
   </si>
   <si>
-    <t>DECIMAL(10,4)</t>
-  </si>
-  <si>
     <t>Do not include in dataset; automatically generated upon upload.</t>
   </si>
   <si>
@@ -831,9 +828,6 @@
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
   <si>
-    <t xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -858,7 +852,13 @@
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
+    <t>DECIMAL(20,4)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
 </sst>
 </file>
@@ -3417,8 +3417,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3456,10 +3456,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -3467,10 +3467,10 @@
       </c>
       <c r="F2" s="100" t="str">
         <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(10,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -3481,7 +3481,7 @@
         <v>151</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" t="str">
         <f>CONCATENATE(A3, " ",  B3, ", ")</f>
@@ -3515,7 +3515,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H5" s="110" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -3539,7 +3539,7 @@
         <v>152</v>
       </c>
       <c r="C7" s="99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" t="str">
         <f>CONCATENATE(A7, " ",  B7, ", ")</f>
@@ -3676,12 +3676,12 @@
         <v>42</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(10,4), </v>
+        <v xml:space="preserve">flowGageHt DECIMAL(20,4), </v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -3902,8 +3902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3944,10 +3944,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" s="99"/>
       <c r="E2" t="str">
@@ -3959,7 +3959,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3970,7 +3970,7 @@
         <v>151</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="99"/>
       <c r="E3" t="str">
@@ -3989,7 +3989,7 @@
         <v>152</v>
       </c>
       <c r="C4" s="99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="99"/>
       <c r="E4" t="str">
@@ -4006,7 +4006,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D5" s="99"/>
       <c r="E5" t="str">
@@ -4436,10 +4436,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -4450,7 +4450,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -4479,7 +4479,7 @@
         <v xml:space="preserve">date DATE, </v>
       </c>
       <c r="H4" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -4606,7 +4606,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="99"/>
       <c r="D14" t="str">
@@ -4661,7 +4661,7 @@
         <v>151</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -4676,7 +4676,7 @@
         <v>152</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -4691,7 +4691,7 @@
         <v>150</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -4994,7 +4994,7 @@
         <v>177</v>
       </c>
       <c r="C43" s="99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -5089,10 +5089,10 @@
         <v>144</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(A2, " ",  B2, ", ")</f>
@@ -5103,7 +5103,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
       </c>
       <c r="G2" s="102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="F4" s="100"/>
       <c r="G4" s="110" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -5171,7 +5171,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="99" t="s">
         <v>159</v>
@@ -5187,7 +5187,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" s="99" t="s">
         <v>159</v>
@@ -5415,10 +5415,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A8635-60E1-404A-9A09-732833EFAF77}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5456,16 +5456,16 @@
     </row>
     <row r="2" spans="1:10" ht="247" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" s="99" t="s">
         <v>144</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" s="99"/>
       <c r="F2" t="str">
@@ -5473,16 +5473,16 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="H2" s="100" t="str">
-        <f>CONCATENATE(F2,F3,F4,F5,F6,F7,F8,F9,F10,F11,F12,F13,F14,F15,F16,F17,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28,F29,F30,F31,F32,F33,F34,F35,F36,F37,F38,F39,F40,F41,F42,F43,F44,F45,F46,F47)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <f>CONCATENATE(F2,F3,F4,F5,F6,F7,F8,F9,F10,F11,F12,F13,F14,F15,F16,F17,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28,F29,F30,F31,F32,F33,F34,F35,F36,F37,F38,F39,F40,F41,F42,F43,F44,F45,F46,F47,F48)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="J2" s="101" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3" s="99" t="s">
         <v>17</v>
@@ -5493,14 +5493,14 @@
       <c r="D3" s="99"/>
       <c r="E3" s="99"/>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F47" si="0">CONCATENATE(B3, " ",  C3, ", ")</f>
+        <f t="shared" ref="F3:F48" si="0">CONCATENATE(B3, " ",  C3, ", ")</f>
         <v xml:space="preserve">site VARCHAR(20), </v>
       </c>
       <c r="H3" s="99"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B4" s="99" t="s">
         <v>19</v>
@@ -5516,12 +5516,12 @@
       </c>
       <c r="H4" s="99"/>
       <c r="J4" s="110" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B5" s="99" t="s">
         <v>21</v>
@@ -5539,7 +5539,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B6" s="104" t="s">
         <v>137</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B7" s="104" t="s">
         <v>26</v>
@@ -5577,7 +5577,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B8" s="104" t="s">
         <v>30</v>
@@ -5595,7 +5595,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" s="104" t="s">
         <v>34</v>
@@ -5613,7 +5613,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B10" s="104" t="s">
         <v>36</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B11" s="104" t="s">
         <v>109</v>
@@ -5649,7 +5649,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B12" s="104" t="s">
         <v>37</v>
@@ -5667,7 +5667,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B13" s="99" t="s">
         <v>38</v>
@@ -5685,7 +5685,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B14" s="99" t="s">
         <v>40</v>
@@ -5703,13 +5703,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B15" s="99" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="99"/>
       <c r="E15" s="99"/>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B16" s="99" t="s">
         <v>55</v>
@@ -5739,7 +5739,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B17" s="99" t="s">
         <v>59</v>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B18" s="99" t="s">
         <v>62</v>
@@ -5776,72 +5776,71 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="99"/>
       <c r="B19" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="99"/>
+      <c r="F19" t="str">
+        <f>CONCATENATE(B19, " ",  C19, ", ")</f>
+        <v xml:space="preserve">archived VARCHAR(20), </v>
+      </c>
+      <c r="H19" s="99"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="99"/>
+      <c r="B20" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="99" t="s">
+      <c r="C20" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="99" t="s">
-        <v>187</v>
-      </c>
-      <c r="E19" s="99"/>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-      <c r="H19" s="99" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="99" t="s">
-        <v>152</v>
-      </c>
       <c r="D20" s="99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E20" s="99"/>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">waterYr YEAR, </v>
-      </c>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+      <c r="H20" s="99"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B21" s="99" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D21" s="99" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E21" s="99"/>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime TEXT, </v>
+        <v xml:space="preserve">waterYr YEAR, </v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="104" t="s">
-        <v>66</v>
+      <c r="B22" s="99" t="s">
+        <v>22</v>
       </c>
       <c r="C22" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="99"/>
+        <v>150</v>
+      </c>
+      <c r="D22" s="99" t="s">
+        <v>189</v>
+      </c>
       <c r="E22" s="99"/>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
+        <v xml:space="preserve">datetime TEXT, </v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B23" s="104" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C23" s="99" t="s">
         <v>177</v>
@@ -5850,12 +5849,12 @@
       <c r="E23" s="99"/>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B24" s="104" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" s="99" t="s">
         <v>177</v>
@@ -5864,12 +5863,12 @@
       <c r="E24" s="99"/>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(8,4), </v>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B25" s="104" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="99" t="s">
         <v>177</v>
@@ -5878,12 +5877,12 @@
       <c r="E25" s="99"/>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(8,4), </v>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B26" s="104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="99" t="s">
         <v>177</v>
@@ -5892,12 +5891,12 @@
       <c r="E26" s="99"/>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B27" s="104" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="99" t="s">
         <v>177</v>
@@ -5906,12 +5905,12 @@
       <c r="E27" s="99"/>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B28" s="104" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="99" t="s">
         <v>177</v>
@@ -5920,12 +5919,12 @@
       <c r="E28" s="99"/>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B29" s="104" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C29" s="99" t="s">
         <v>177</v>
@@ -5934,12 +5933,12 @@
       <c r="E29" s="99"/>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B30" s="104" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="99" t="s">
         <v>177</v>
@@ -5948,12 +5947,12 @@
       <c r="E30" s="99"/>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B31" s="104" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31" s="99" t="s">
         <v>177</v>
@@ -5962,12 +5961,12 @@
       <c r="E31" s="99"/>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B32" s="104" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="99" t="s">
         <v>177</v>
@@ -5976,12 +5975,12 @@
       <c r="E32" s="99"/>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="104" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" s="99" t="s">
         <v>177</v>
@@ -5990,12 +5989,12 @@
       <c r="E33" s="99"/>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B34" s="104" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C34" s="99" t="s">
         <v>177</v>
@@ -6004,12 +6003,12 @@
       <c r="E34" s="99"/>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B35" s="104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="99" t="s">
         <v>177</v>
@@ -6018,12 +6017,12 @@
       <c r="E35" s="99"/>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B36" s="104" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="99" t="s">
         <v>177</v>
@@ -6032,12 +6031,12 @@
       <c r="E36" s="99"/>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(8,4), </v>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B37" s="104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="99" t="s">
         <v>177</v>
@@ -6046,12 +6045,12 @@
       <c r="E37" s="99"/>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B38" s="104" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="99" t="s">
         <v>177</v>
@@ -6060,12 +6059,12 @@
       <c r="E38" s="99"/>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B39" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" s="99" t="s">
         <v>177</v>
@@ -6074,12 +6073,12 @@
       <c r="E39" s="99"/>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B40" s="104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="99" t="s">
         <v>177</v>
@@ -6088,12 +6087,12 @@
       <c r="E40" s="99"/>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(8,4), </v>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B41" s="104" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" s="99" t="s">
         <v>177</v>
@@ -6102,12 +6101,12 @@
       <c r="E41" s="99"/>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B42" s="104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="99" t="s">
         <v>177</v>
@@ -6116,12 +6115,12 @@
       <c r="E42" s="99"/>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B43" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="99" t="s">
         <v>177</v>
@@ -6130,12 +6129,12 @@
       <c r="E43" s="99"/>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B44" s="99" t="s">
-        <v>101</v>
+      <c r="B44" s="104" t="s">
+        <v>100</v>
       </c>
       <c r="C44" s="99" t="s">
         <v>177</v>
@@ -6144,59 +6143,73 @@
       <c r="E44" s="99"/>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B45" s="99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="99" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="D45" s="99"/>
       <c r="E45" s="99"/>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">duplicate VARCHAR(10), </v>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B46" s="99" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C46" s="99" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D46" s="99"/>
       <c r="E46" s="99"/>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">sampleType VARCHAR(20), </v>
+        <v xml:space="preserve">duplicate VARCHAR(10), </v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B47" s="104" t="s">
-        <v>108</v>
+      <c r="B47" s="99" t="s">
+        <v>106</v>
       </c>
       <c r="C47" s="99" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="D47" s="99"/>
       <c r="E47" s="99"/>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
+        <v xml:space="preserve">sampleType VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B48" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="D48" s="99"/>
+      <c r="E48" s="99"/>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B50" s="105" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B51" s="105" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576 H3:H19">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B1:B18 H3:H20 B20:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6224,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="111" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6232,7 +6245,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="113"/>
     </row>
@@ -6241,7 +6254,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C3" s="113"/>
     </row>
@@ -6250,7 +6263,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="113"/>
     </row>
@@ -6259,7 +6272,7 @@
         <v>137</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" s="113"/>
     </row>
@@ -6302,7 +6315,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="112" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6310,7 +6323,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C11" s="113"/>
     </row>
@@ -6319,7 +6332,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12" s="113"/>
     </row>
@@ -6328,7 +6341,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C13" s="113"/>
     </row>
@@ -6345,7 +6358,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6353,7 +6366,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="112" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6513,7 +6526,7 @@
         <v>97</v>
       </c>
       <c r="B36" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6521,7 +6534,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6529,7 +6542,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6537,7 +6550,7 @@
         <v>101</v>
       </c>
       <c r="B39" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6550,7 +6563,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6558,7 +6571,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6566,7 +6579,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6574,7 +6587,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6582,7 +6595,7 @@
         <v>106</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -6596,7 +6609,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="112" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
latest updates to documentation files
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F62333CE-27AF-A64C-804C-9E29F2CCACF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04F607A2-42E0-464D-9F9D-14E70B7374EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42240" yWindow="800" windowWidth="21640" windowHeight="14600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="30300" windowHeight="19600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="209">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -846,9 +846,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>REMOVE</t>
-  </si>
-  <si>
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
   <si>
@@ -860,12 +857,33 @@
   <si>
     <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
   </si>
+  <si>
+    <t>Has codes applied?</t>
+  </si>
+  <si>
+    <t>MyRefNo</t>
+  </si>
+  <si>
+    <t>au254</t>
+  </si>
+  <si>
+    <t>au275</t>
+  </si>
+  <si>
+    <t>au295</t>
+  </si>
+  <si>
+    <t>au350</t>
+  </si>
+  <si>
+    <t>au400</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1146,6 +1164,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -1338,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1567,6 +1591,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3418,7 +3445,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A22" sqref="A22:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3470,7 +3497,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -3676,7 +3703,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
@@ -3737,35 +3764,47 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="99"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
+      <c r="A22" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="105" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
+      <c r="A23" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="118"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="99"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="118"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="118"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="99"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
+      <c r="A25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" s="118"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="99"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
+      <c r="A26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="118"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="118"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="99"/>
-      <c r="B27" s="99"/>
       <c r="C27" s="99"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
@@ -3774,7 +3813,9 @@
       <c r="C28" s="99"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="99"/>
+      <c r="A29" s="105" t="s">
+        <v>160</v>
+      </c>
       <c r="B29" s="99"/>
       <c r="C29" s="99"/>
     </row>
@@ -3887,7 +3928,7 @@
   <conditionalFormatting sqref="F8:F15">
     <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
+  <conditionalFormatting sqref="A29">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
@@ -3902,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3959,7 +4000,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -5415,801 +5456,1033 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A8635-60E1-404A-9A09-732833EFAF77}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="8" max="8" width="50.5" customWidth="1"/>
-    <col min="10" max="10" width="50.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="116"/>
+    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="9" max="9" width="50.5" customWidth="1"/>
+    <col min="11" max="11" width="50.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B1" s="103" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="C1" s="103" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="D1" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="E1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="G1" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="I1" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="98" t="s">
+      <c r="K1" s="98" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="247" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
-        <v>198</v>
+    <row r="2" spans="1:11" ht="247" x14ac:dyDescent="0.15">
+      <c r="A2" s="116" t="s">
+        <v>203</v>
       </c>
       <c r="B2" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="99" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="99" t="s">
+      <c r="D2" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="99" t="s">
+      <c r="E2" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="99"/>
-      <c r="F2" t="str">
-        <f>CONCATENATE(B2, " ",  C2, ", ")</f>
+      <c r="F2" s="99"/>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2" si="0">CONCATENATE(C2, " ",  D2, ", ")</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
-      <c r="H2" s="100" t="str">
-        <f>CONCATENATE(F2,F3,F4,F5,F6,F7,F8,F9,F10,F11,F12,F13,F14,F15,F16,F17,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28,F29,F30,F31,F32,F33,F34,F35,F36,F37,F38,F39,F40,F41,F42,F43,F44,F45,F46,F47,F48)</f>
+      <c r="I2" s="100" t="str">
+        <f>CONCATENATE(G2,G3,G4,G5,G6,G7,G8,G9,G10,G11,G12,G13,G14,G15,G16,G17,G18,G19,G20,G21,G22,G23,G24,G25,G26,G27,G28,G29,G30,G31,G32,G33,G34,G35,G36,G37,G38,G39,G40,G41,G42,G43,G44,G45,G46,G47,G48)</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
-      <c r="J2" s="101" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
+      <c r="K2" s="101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="116">
+        <v>1</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G48" si="1">CONCATENATE(C3, " ",  D3, ", ")</f>
+        <v xml:space="preserve">site VARCHAR(20), </v>
+      </c>
+      <c r="I3" s="99"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="116">
+        <v>2</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">date DATE, </v>
+      </c>
+      <c r="I4" s="99"/>
+      <c r="K4" s="110" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="116">
+        <v>3</v>
+      </c>
+      <c r="B5" s="99">
+        <v>9</v>
+      </c>
+      <c r="C5" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">timeEST TIME, </v>
+      </c>
+      <c r="I5" s="99"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="116">
+        <v>4</v>
+      </c>
+      <c r="B6" s="99" t="s">
         <v>197</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="C6" s="104" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="99"/>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
+      </c>
+      <c r="I6" s="99"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="116">
+        <v>5</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
+      </c>
+      <c r="I7" s="99"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="116">
+        <v>6</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">DIC SMALLINT, </v>
+      </c>
+      <c r="I8" s="99"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="116">
+        <v>7</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
+      </c>
+      <c r="I9" s="99"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="116">
+        <v>8</v>
+      </c>
+      <c r="B10" s="99">
+        <v>9</v>
+      </c>
+      <c r="C10" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
+      </c>
+      <c r="I10" s="99"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="116">
+        <v>9</v>
+      </c>
+      <c r="B11" s="99">
+        <v>9</v>
+      </c>
+      <c r="C11" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
+      </c>
+      <c r="I11" s="99"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="116">
+        <v>10</v>
+      </c>
+      <c r="B12" s="99">
+        <v>9</v>
+      </c>
+      <c r="C12" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="99"/>
+      <c r="F12" s="99"/>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
+      </c>
+      <c r="I12" s="99"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="116">
+        <v>11</v>
+      </c>
+      <c r="B13" s="99"/>
+      <c r="C13" s="99" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+      </c>
+      <c r="I13" s="99"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="116">
+        <v>12</v>
+      </c>
+      <c r="B14" s="99"/>
+      <c r="C14" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
+      </c>
+      <c r="I14" s="99"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="116">
+        <v>13</v>
+      </c>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
+      </c>
+      <c r="I15" s="99"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="116">
+        <v>14</v>
+      </c>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
+      </c>
+      <c r="I16" s="99"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="116">
+        <v>15</v>
+      </c>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
+      </c>
+      <c r="I17" s="99"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="116">
+        <v>16</v>
+      </c>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">notes TEXT, </v>
+      </c>
+      <c r="I18" s="99"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="116">
         <v>17</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="B19" s="99"/>
+      <c r="C19" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F48" si="0">CONCATENATE(B3, " ",  C3, ", ")</f>
-        <v xml:space="preserve">site VARCHAR(20), </v>
-      </c>
-      <c r="H3" s="99"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="99" t="s">
+      <c r="E19" s="99"/>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">archived VARCHAR(20), </v>
+      </c>
+      <c r="I19" s="99"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="116">
+        <v>18</v>
+      </c>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="99" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" s="99"/>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+      <c r="I20" s="99"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="116">
+        <v>19</v>
+      </c>
+      <c r="C21" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="99"/>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">waterYr YEAR, </v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="116">
+        <v>20</v>
+      </c>
+      <c r="C22" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="99"/>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">datetime TEXT, </v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="116">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">date DATE, </v>
-      </c>
-      <c r="H4" s="99"/>
-      <c r="J4" s="110" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="99" t="s">
+      <c r="C23" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="116">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">timeEST TIME, </v>
-      </c>
-      <c r="H5" s="99"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="99" t="s">
+      <c r="C24" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="116">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="104" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="99" t="s">
+      <c r="C25" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="99" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" s="99"/>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(8,4), </v>
-      </c>
-      <c r="H6" s="99"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="99" t="s">
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="116">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="C26" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="99"/>
+      <c r="F26" s="99"/>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="116">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="116">
         <v>26</v>
       </c>
-      <c r="C7" s="99" t="s">
+      <c r="B28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
-      </c>
-      <c r="H7" s="99"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="99" t="s">
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="116">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="C29" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="116">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="99"/>
+      <c r="F30" s="99"/>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="116">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="116">
         <v>30</v>
       </c>
-      <c r="C8" s="99" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DIC SMALLINT, </v>
-      </c>
-      <c r="H8" s="99"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="99" t="s">
+      <c r="B32" t="s">
         <v>197</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="C32" s="104" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="116">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="104" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="116">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="104" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="116">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="116">
         <v>34</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="B36" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
-      </c>
-      <c r="H9" s="99"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="99" t="s">
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="116">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>197</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="C37" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="99"/>
+      <c r="F37" s="99"/>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="116">
         <v>36</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(8,4), </v>
-      </c>
-      <c r="H10" s="99"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="99" t="s">
+      <c r="E38" s="99"/>
+      <c r="F38" s="99"/>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="116">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>197</v>
       </c>
-      <c r="B11" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="99" t="s">
+      <c r="C39" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
-      </c>
-      <c r="H11" s="99"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="99" t="s">
+      <c r="E39" s="99"/>
+      <c r="F39" s="99"/>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="116">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="99" t="s">
+      <c r="C40" s="104" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
-      </c>
-      <c r="H12" s="99"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="99" t="s">
+      <c r="E40" s="99"/>
+      <c r="F40" s="99"/>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="116">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="99" t="s">
+      <c r="C41" s="104" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
-      </c>
-      <c r="H13" s="99"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" s="99" t="s">
+      <c r="E41" s="99"/>
+      <c r="F41" s="99"/>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="116">
         <v>40</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C42" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="99"/>
+      <c r="F42" s="99"/>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="116">
+        <v>41</v>
+      </c>
+      <c r="C43" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E43" s="99"/>
+      <c r="F43" s="99"/>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="116">
+        <v>42</v>
+      </c>
+      <c r="C44" s="104" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" s="99"/>
+      <c r="F44" s="99"/>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45" s="116">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="99"/>
+      <c r="F45" s="99"/>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46" s="116">
+        <v>44</v>
+      </c>
+      <c r="C46" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="99"/>
+      <c r="F46" s="99"/>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">duplicate VARCHAR(10), </v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="116">
+        <v>45</v>
+      </c>
+      <c r="C47" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
-      </c>
-      <c r="H14" s="99"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B15" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="99" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
-      </c>
-      <c r="H15" s="99"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B16" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="99" t="s">
+      <c r="E47" s="99"/>
+      <c r="F47" s="99"/>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">sampleType VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="116">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
-      </c>
-      <c r="H16" s="99"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="99" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
-      </c>
-      <c r="H17" s="99"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B18" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">notes TEXT, </v>
-      </c>
-      <c r="H18" s="99"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="99"/>
-      <c r="B19" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="99"/>
-      <c r="F19" t="str">
-        <f>CONCATENATE(B19, " ",  C19, ", ")</f>
-        <v xml:space="preserve">archived VARCHAR(20), </v>
-      </c>
-      <c r="H19" s="99"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="99"/>
-      <c r="B20" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="99" t="s">
-        <v>186</v>
-      </c>
-      <c r="E20" s="99"/>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-      <c r="H20" s="99"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="99" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>187</v>
-      </c>
-      <c r="E21" s="99"/>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">waterYr YEAR, </v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="99" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="99" t="s">
-        <v>189</v>
-      </c>
-      <c r="E22" s="99"/>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime TEXT, </v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D23" s="99"/>
-      <c r="E23" s="99"/>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="104" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="104" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D25" s="99"/>
-      <c r="E25" s="99"/>
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="104" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D32" s="99"/>
-      <c r="E32" s="99"/>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B33" s="104" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B34" s="104" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B35" s="104" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B36" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B37" s="104" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
-      <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B38" s="104" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B39" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B40" s="104" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B41" s="104" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B42" s="104" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D42" s="99"/>
-      <c r="E42" s="99"/>
-      <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B43" s="104" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D43" s="99"/>
-      <c r="E43" s="99"/>
-      <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B44" s="104" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" s="99"/>
-      <c r="E44" s="99"/>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B45" s="99" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D45" s="99"/>
-      <c r="E45" s="99"/>
-      <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B46" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="99" t="s">
-        <v>153</v>
-      </c>
-      <c r="D46" s="99"/>
-      <c r="E46" s="99"/>
-      <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">duplicate VARCHAR(10), </v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B47" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="99"/>
-      <c r="E47" s="99"/>
-      <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">sampleType VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B48" s="104" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D48" s="99"/>
       <c r="E48" s="99"/>
-      <c r="F48" t="str">
-        <f t="shared" si="0"/>
+      <c r="F48" s="99"/>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B51" s="105" t="s">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C49" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" s="117"/>
+      <c r="E49" s="117"/>
+      <c r="F49" s="118"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C50" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" s="118"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="118"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C51" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" s="118"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="118"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="118"/>
+      <c r="E52" s="117"/>
+      <c r="F52" s="118"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" s="118"/>
+      <c r="E53" s="117"/>
+      <c r="F53" s="118"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C55" s="105" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B18 H3:H20 B20:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <sortState ref="A3:K48">
+    <sortCondition ref="A3:A48"/>
+  </sortState>
+  <conditionalFormatting sqref="C1:C18 I3:I20 C20:C48 C60:C1048576 C54:C55">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7577,7 +7850,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:X1003"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes in documentation files
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04F607A2-42E0-464D-9F9D-14E70B7374EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F37CAF-81C0-8142-A10F-5B68EDA0F065}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="30300" windowHeight="19600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="chemistry" sheetId="10" r:id="rId3"/>
     <sheet name="historical" sheetId="5" r:id="rId4"/>
     <sheet name="sensor" sheetId="6" r:id="rId5"/>
-    <sheet name="currentOLD" sheetId="4" r:id="rId6"/>
+    <sheet name="current" sheetId="4" r:id="rId6"/>
     <sheet name="units" sheetId="9" r:id="rId7"/>
     <sheet name="AlmostFinalNames" sheetId="1" r:id="rId8"/>
     <sheet name="CreatingCommonNames" sheetId="2" r:id="rId9"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="211">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -878,6 +878,12 @@
   <si>
     <t>au400</t>
   </si>
+  <si>
+    <t>Need to put in database</t>
+  </si>
+  <si>
+    <t>Remove?</t>
+  </si>
 </sst>
 </file>
 
@@ -1362,7 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1594,6 +1600,8 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3478,7 +3486,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="143" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="154" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -3943,7 +3951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3980,7 +3988,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="169" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -4472,7 +4480,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="221" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="238" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -5125,7 +5133,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -5456,10 +5464,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A8635-60E1-404A-9A09-732833EFAF77}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:AZ55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5473,7 +5481,7 @@
     <col min="11" max="11" width="50.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.15">
       <c r="C1" s="103" t="s">
         <v>174</v>
       </c>
@@ -5496,7 +5504,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="247" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:52" ht="266" x14ac:dyDescent="0.15">
       <c r="A2" s="116" t="s">
         <v>203</v>
       </c>
@@ -5525,7 +5533,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A3" s="116">
         <v>1</v>
       </c>
@@ -5544,7 +5552,7 @@
       </c>
       <c r="I3" s="99"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A4" s="116">
         <v>2</v>
       </c>
@@ -5566,7 +5574,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A5" s="116">
         <v>3</v>
       </c>
@@ -5587,7 +5595,7 @@
       </c>
       <c r="I5" s="99"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A6" s="116">
         <v>4</v>
       </c>
@@ -5610,7 +5618,7 @@
       </c>
       <c r="I6" s="99"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A7" s="116">
         <v>5</v>
       </c>
@@ -5631,7 +5639,7 @@
       </c>
       <c r="I7" s="99"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A8" s="116">
         <v>6</v>
       </c>
@@ -5650,9 +5658,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">DIC SMALLINT, </v>
       </c>
-      <c r="I8" s="99"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="119"/>
+      <c r="Q8" s="119"/>
+      <c r="R8" s="119"/>
+      <c r="S8" s="119"/>
+      <c r="T8" s="119"/>
+      <c r="U8" s="119"/>
+      <c r="V8" s="119"/>
+      <c r="W8" s="119"/>
+      <c r="X8" s="119"/>
+      <c r="Y8" s="119"/>
+      <c r="Z8" s="119"/>
+      <c r="AA8" s="119"/>
+      <c r="AB8" s="119"/>
+      <c r="AC8" s="119"/>
+      <c r="AD8" s="119"/>
+      <c r="AE8" s="119"/>
+      <c r="AF8" s="119"/>
+      <c r="AG8" s="119"/>
+      <c r="AH8" s="119"/>
+      <c r="AI8" s="119"/>
+      <c r="AJ8" s="119"/>
+      <c r="AK8" s="119"/>
+      <c r="AL8" s="119"/>
+      <c r="AM8" s="119"/>
+      <c r="AN8" s="119"/>
+      <c r="AO8" s="119"/>
+      <c r="AP8" s="119"/>
+      <c r="AQ8" s="119"/>
+      <c r="AR8" s="119"/>
+      <c r="AS8" s="119"/>
+      <c r="AT8" s="119"/>
+      <c r="AU8" s="119"/>
+      <c r="AV8" s="119"/>
+      <c r="AW8" s="119"/>
+      <c r="AX8" s="119"/>
+      <c r="AY8" s="119"/>
+      <c r="AZ8" s="119"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A9" s="116">
         <v>7</v>
       </c>
@@ -5671,9 +5722,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">spCond DECIMAL(8,4), </v>
       </c>
-      <c r="I9" s="99"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+      <c r="Q9" s="119"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119"/>
+      <c r="T9" s="119"/>
+      <c r="U9" s="119"/>
+      <c r="V9" s="119"/>
+      <c r="W9" s="119"/>
+      <c r="X9" s="119"/>
+      <c r="Y9" s="119"/>
+      <c r="Z9" s="119"/>
+      <c r="AA9" s="119"/>
+      <c r="AB9" s="119"/>
+      <c r="AC9" s="119"/>
+      <c r="AD9" s="119"/>
+      <c r="AE9" s="119"/>
+      <c r="AF9" s="119"/>
+      <c r="AG9" s="119"/>
+      <c r="AH9" s="119"/>
+      <c r="AI9" s="119"/>
+      <c r="AJ9" s="119"/>
+      <c r="AK9" s="119"/>
+      <c r="AL9" s="119"/>
+      <c r="AM9" s="119"/>
+      <c r="AN9" s="119"/>
+      <c r="AO9" s="119"/>
+      <c r="AP9" s="119"/>
+      <c r="AQ9" s="119"/>
+      <c r="AR9" s="119"/>
+      <c r="AS9" s="119"/>
+      <c r="AT9" s="119"/>
+      <c r="AU9" s="119"/>
+      <c r="AV9" s="119"/>
+      <c r="AW9" s="119"/>
+      <c r="AX9" s="119"/>
+      <c r="AY9" s="119"/>
+      <c r="AZ9" s="119"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A10" s="116">
         <v>8</v>
       </c>
@@ -5692,9 +5786,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">temp DECIMAL(8,4), </v>
       </c>
-      <c r="I10" s="99"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
+      <c r="T10" s="119"/>
+      <c r="U10" s="119"/>
+      <c r="V10" s="119"/>
+      <c r="W10" s="119"/>
+      <c r="X10" s="119"/>
+      <c r="Y10" s="119"/>
+      <c r="Z10" s="119"/>
+      <c r="AA10" s="119"/>
+      <c r="AB10" s="119"/>
+      <c r="AC10" s="119"/>
+      <c r="AD10" s="119"/>
+      <c r="AE10" s="119"/>
+      <c r="AF10" s="119"/>
+      <c r="AG10" s="119"/>
+      <c r="AH10" s="119"/>
+      <c r="AI10" s="119"/>
+      <c r="AJ10" s="119"/>
+      <c r="AK10" s="119"/>
+      <c r="AL10" s="119"/>
+      <c r="AM10" s="119"/>
+      <c r="AN10" s="119"/>
+      <c r="AO10" s="119"/>
+      <c r="AP10" s="119"/>
+      <c r="AQ10" s="119"/>
+      <c r="AR10" s="119"/>
+      <c r="AS10" s="119"/>
+      <c r="AT10" s="119"/>
+      <c r="AU10" s="119"/>
+      <c r="AV10" s="119"/>
+      <c r="AW10" s="119"/>
+      <c r="AX10" s="119"/>
+      <c r="AY10" s="119"/>
+      <c r="AZ10" s="119"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A11" s="116">
         <v>9</v>
       </c>
@@ -5713,9 +5850,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
       </c>
-      <c r="I11" s="99"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="119"/>
+      <c r="T11" s="119"/>
+      <c r="U11" s="119"/>
+      <c r="V11" s="119"/>
+      <c r="W11" s="119"/>
+      <c r="X11" s="119"/>
+      <c r="Y11" s="119"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="119"/>
+      <c r="AB11" s="119"/>
+      <c r="AC11" s="119"/>
+      <c r="AD11" s="119"/>
+      <c r="AE11" s="119"/>
+      <c r="AF11" s="119"/>
+      <c r="AG11" s="119"/>
+      <c r="AH11" s="119"/>
+      <c r="AI11" s="119"/>
+      <c r="AJ11" s="119"/>
+      <c r="AK11" s="119"/>
+      <c r="AL11" s="119"/>
+      <c r="AM11" s="119"/>
+      <c r="AN11" s="119"/>
+      <c r="AO11" s="119"/>
+      <c r="AP11" s="119"/>
+      <c r="AQ11" s="119"/>
+      <c r="AR11" s="119"/>
+      <c r="AS11" s="119"/>
+      <c r="AT11" s="119"/>
+      <c r="AU11" s="119"/>
+      <c r="AV11" s="119"/>
+      <c r="AW11" s="119"/>
+      <c r="AX11" s="119"/>
+      <c r="AY11" s="119"/>
+      <c r="AZ11" s="119"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A12" s="116">
         <v>10</v>
       </c>
@@ -5734,9 +5914,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
       </c>
-      <c r="I12" s="99"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="119"/>
+      <c r="T12" s="119"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="119"/>
+      <c r="W12" s="119"/>
+      <c r="X12" s="119"/>
+      <c r="Y12" s="119"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="119"/>
+      <c r="AB12" s="119"/>
+      <c r="AC12" s="119"/>
+      <c r="AD12" s="119"/>
+      <c r="AE12" s="119"/>
+      <c r="AF12" s="119"/>
+      <c r="AG12" s="119"/>
+      <c r="AH12" s="119"/>
+      <c r="AI12" s="119"/>
+      <c r="AJ12" s="119"/>
+      <c r="AK12" s="119"/>
+      <c r="AL12" s="119"/>
+      <c r="AM12" s="119"/>
+      <c r="AN12" s="119"/>
+      <c r="AO12" s="119"/>
+      <c r="AP12" s="119"/>
+      <c r="AQ12" s="119"/>
+      <c r="AR12" s="119"/>
+      <c r="AS12" s="119"/>
+      <c r="AT12" s="119"/>
+      <c r="AU12" s="119"/>
+      <c r="AV12" s="119"/>
+      <c r="AW12" s="119"/>
+      <c r="AX12" s="119"/>
+      <c r="AY12" s="119"/>
+      <c r="AZ12" s="119"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A13" s="116">
         <v>11</v>
       </c>
@@ -5753,9 +5976,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
       </c>
-      <c r="I13" s="99"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
+      <c r="N13" s="119"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="119"/>
+      <c r="Q13" s="119"/>
+      <c r="R13" s="119"/>
+      <c r="S13" s="119"/>
+      <c r="T13" s="119"/>
+      <c r="U13" s="119"/>
+      <c r="V13" s="119"/>
+      <c r="W13" s="119"/>
+      <c r="X13" s="119"/>
+      <c r="Y13" s="119"/>
+      <c r="Z13" s="119"/>
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="119"/>
+      <c r="AC13" s="119"/>
+      <c r="AD13" s="119"/>
+      <c r="AE13" s="119"/>
+      <c r="AF13" s="119"/>
+      <c r="AG13" s="119"/>
+      <c r="AH13" s="119"/>
+      <c r="AI13" s="119"/>
+      <c r="AJ13" s="119"/>
+      <c r="AK13" s="119"/>
+      <c r="AL13" s="119"/>
+      <c r="AM13" s="119"/>
+      <c r="AN13" s="119"/>
+      <c r="AO13" s="119"/>
+      <c r="AP13" s="119"/>
+      <c r="AQ13" s="119"/>
+      <c r="AR13" s="119"/>
+      <c r="AS13" s="119"/>
+      <c r="AT13" s="119"/>
+      <c r="AU13" s="119"/>
+      <c r="AV13" s="119"/>
+      <c r="AW13" s="119"/>
+      <c r="AX13" s="119"/>
+      <c r="AY13" s="119"/>
+      <c r="AZ13" s="119"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A14" s="116">
         <v>12</v>
       </c>
@@ -5772,9 +6038,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
       </c>
-      <c r="I14" s="99"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I14" s="119"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="119"/>
+      <c r="M14" s="119"/>
+      <c r="N14" s="119"/>
+      <c r="O14" s="119"/>
+      <c r="P14" s="119"/>
+      <c r="Q14" s="119"/>
+      <c r="R14" s="119"/>
+      <c r="S14" s="119"/>
+      <c r="T14" s="119"/>
+      <c r="U14" s="119"/>
+      <c r="V14" s="119"/>
+      <c r="W14" s="119"/>
+      <c r="X14" s="119"/>
+      <c r="Y14" s="119"/>
+      <c r="Z14" s="119"/>
+      <c r="AA14" s="119"/>
+      <c r="AB14" s="119"/>
+      <c r="AC14" s="119"/>
+      <c r="AD14" s="119"/>
+      <c r="AE14" s="119"/>
+      <c r="AF14" s="119"/>
+      <c r="AG14" s="119"/>
+      <c r="AH14" s="119"/>
+      <c r="AI14" s="119"/>
+      <c r="AJ14" s="119"/>
+      <c r="AK14" s="119"/>
+      <c r="AL14" s="119"/>
+      <c r="AM14" s="119"/>
+      <c r="AN14" s="119"/>
+      <c r="AO14" s="119"/>
+      <c r="AP14" s="119"/>
+      <c r="AQ14" s="119"/>
+      <c r="AR14" s="119"/>
+      <c r="AS14" s="119"/>
+      <c r="AT14" s="119"/>
+      <c r="AU14" s="119"/>
+      <c r="AV14" s="119"/>
+      <c r="AW14" s="119"/>
+      <c r="AX14" s="119"/>
+      <c r="AY14" s="119"/>
+      <c r="AZ14" s="119"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A15" s="116">
         <v>13</v>
       </c>
@@ -5791,9 +6100,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
       </c>
-      <c r="I15" s="99"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
+      <c r="Z15" s="119"/>
+      <c r="AA15" s="119"/>
+      <c r="AB15" s="119"/>
+      <c r="AC15" s="119"/>
+      <c r="AD15" s="119"/>
+      <c r="AE15" s="119"/>
+      <c r="AF15" s="119"/>
+      <c r="AG15" s="119"/>
+      <c r="AH15" s="119"/>
+      <c r="AI15" s="119"/>
+      <c r="AJ15" s="119"/>
+      <c r="AK15" s="119"/>
+      <c r="AL15" s="119"/>
+      <c r="AM15" s="119"/>
+      <c r="AN15" s="119"/>
+      <c r="AO15" s="119"/>
+      <c r="AP15" s="119"/>
+      <c r="AQ15" s="119"/>
+      <c r="AR15" s="119"/>
+      <c r="AS15" s="119"/>
+      <c r="AT15" s="119"/>
+      <c r="AU15" s="119"/>
+      <c r="AV15" s="119"/>
+      <c r="AW15" s="119"/>
+      <c r="AX15" s="119"/>
+      <c r="AY15" s="119"/>
+      <c r="AZ15" s="119"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A16" s="116">
         <v>14</v>
       </c>
@@ -5810,9 +6162,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
       </c>
-      <c r="I16" s="99"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
+      <c r="Q16" s="119"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="119"/>
+      <c r="Y16" s="119"/>
+      <c r="Z16" s="119"/>
+      <c r="AA16" s="119"/>
+      <c r="AB16" s="119"/>
+      <c r="AC16" s="119"/>
+      <c r="AD16" s="119"/>
+      <c r="AE16" s="119"/>
+      <c r="AF16" s="119"/>
+      <c r="AG16" s="119"/>
+      <c r="AH16" s="119"/>
+      <c r="AI16" s="119"/>
+      <c r="AJ16" s="119"/>
+      <c r="AK16" s="119"/>
+      <c r="AL16" s="119"/>
+      <c r="AM16" s="119"/>
+      <c r="AN16" s="119"/>
+      <c r="AO16" s="119"/>
+      <c r="AP16" s="119"/>
+      <c r="AQ16" s="119"/>
+      <c r="AR16" s="119"/>
+      <c r="AS16" s="119"/>
+      <c r="AT16" s="119"/>
+      <c r="AU16" s="119"/>
+      <c r="AV16" s="119"/>
+      <c r="AW16" s="119"/>
+      <c r="AX16" s="119"/>
+      <c r="AY16" s="119"/>
+      <c r="AZ16" s="119"/>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A17" s="116">
         <v>15</v>
       </c>
@@ -5829,9 +6224,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">fieldCode VARCHAR(50), </v>
       </c>
-      <c r="I17" s="99"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
+      <c r="Z17" s="119"/>
+      <c r="AA17" s="119"/>
+      <c r="AB17" s="119"/>
+      <c r="AC17" s="119"/>
+      <c r="AD17" s="119"/>
+      <c r="AE17" s="119"/>
+      <c r="AF17" s="119"/>
+      <c r="AG17" s="119"/>
+      <c r="AH17" s="119"/>
+      <c r="AI17" s="119"/>
+      <c r="AJ17" s="119"/>
+      <c r="AK17" s="119"/>
+      <c r="AL17" s="119"/>
+      <c r="AM17" s="119"/>
+      <c r="AN17" s="119"/>
+      <c r="AO17" s="119"/>
+      <c r="AP17" s="119"/>
+      <c r="AQ17" s="119"/>
+      <c r="AR17" s="119"/>
+      <c r="AS17" s="119"/>
+      <c r="AT17" s="119"/>
+      <c r="AU17" s="119"/>
+      <c r="AV17" s="119"/>
+      <c r="AW17" s="119"/>
+      <c r="AX17" s="119"/>
+      <c r="AY17" s="119"/>
+      <c r="AZ17" s="119"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A18" s="116">
         <v>16</v>
       </c>
@@ -5848,9 +6286,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">notes TEXT, </v>
       </c>
-      <c r="I18" s="99"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="119"/>
+      <c r="O18" s="119"/>
+      <c r="P18" s="119"/>
+      <c r="Q18" s="119"/>
+      <c r="R18" s="119"/>
+      <c r="S18" s="119"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="119"/>
+      <c r="V18" s="119"/>
+      <c r="W18" s="119"/>
+      <c r="X18" s="119"/>
+      <c r="Y18" s="119"/>
+      <c r="Z18" s="119"/>
+      <c r="AA18" s="119"/>
+      <c r="AB18" s="119"/>
+      <c r="AC18" s="119"/>
+      <c r="AD18" s="119"/>
+      <c r="AE18" s="119"/>
+      <c r="AF18" s="119"/>
+      <c r="AG18" s="119"/>
+      <c r="AH18" s="119"/>
+      <c r="AI18" s="119"/>
+      <c r="AJ18" s="119"/>
+      <c r="AK18" s="119"/>
+      <c r="AL18" s="119"/>
+      <c r="AM18" s="119"/>
+      <c r="AN18" s="119"/>
+      <c r="AO18" s="119"/>
+      <c r="AP18" s="119"/>
+      <c r="AQ18" s="119"/>
+      <c r="AR18" s="119"/>
+      <c r="AS18" s="119"/>
+      <c r="AT18" s="119"/>
+      <c r="AU18" s="119"/>
+      <c r="AV18" s="119"/>
+      <c r="AW18" s="119"/>
+      <c r="AX18" s="119"/>
+      <c r="AY18" s="119"/>
+      <c r="AZ18" s="119"/>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A19" s="116">
         <v>17</v>
       </c>
@@ -5858,17 +6339,63 @@
       <c r="C19" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="120" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="99"/>
+      <c r="E19" s="120" t="s">
+        <v>210</v>
+      </c>
+      <c r="F19" s="120"/>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">archived VARCHAR(20), </v>
       </c>
-      <c r="I19" s="99"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I19" s="119"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="119"/>
+      <c r="L19" s="119"/>
+      <c r="M19" s="119"/>
+      <c r="N19" s="119"/>
+      <c r="O19" s="119"/>
+      <c r="P19" s="119"/>
+      <c r="Q19" s="119"/>
+      <c r="R19" s="119"/>
+      <c r="S19" s="119"/>
+      <c r="T19" s="119"/>
+      <c r="U19" s="119"/>
+      <c r="V19" s="119"/>
+      <c r="W19" s="119"/>
+      <c r="X19" s="119"/>
+      <c r="Y19" s="119"/>
+      <c r="Z19" s="119"/>
+      <c r="AA19" s="119"/>
+      <c r="AB19" s="119"/>
+      <c r="AC19" s="119"/>
+      <c r="AD19" s="119"/>
+      <c r="AE19" s="119"/>
+      <c r="AF19" s="119"/>
+      <c r="AG19" s="119"/>
+      <c r="AH19" s="119"/>
+      <c r="AI19" s="119"/>
+      <c r="AJ19" s="119"/>
+      <c r="AK19" s="119"/>
+      <c r="AL19" s="119"/>
+      <c r="AM19" s="119"/>
+      <c r="AN19" s="119"/>
+      <c r="AO19" s="119"/>
+      <c r="AP19" s="119"/>
+      <c r="AQ19" s="119"/>
+      <c r="AR19" s="119"/>
+      <c r="AS19" s="119"/>
+      <c r="AT19" s="119"/>
+      <c r="AU19" s="119"/>
+      <c r="AV19" s="119"/>
+      <c r="AW19" s="119"/>
+      <c r="AX19" s="119"/>
+      <c r="AY19" s="119"/>
+      <c r="AZ19" s="119"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A20" s="116">
         <v>18</v>
       </c>
@@ -5887,9 +6414,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
       </c>
-      <c r="I20" s="99"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I20" s="119"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="119"/>
+      <c r="L20" s="119"/>
+      <c r="M20" s="119"/>
+      <c r="N20" s="119"/>
+      <c r="O20" s="119"/>
+      <c r="P20" s="119"/>
+      <c r="Q20" s="119"/>
+      <c r="R20" s="119"/>
+      <c r="S20" s="119"/>
+      <c r="T20" s="119"/>
+      <c r="U20" s="119"/>
+      <c r="V20" s="119"/>
+      <c r="W20" s="119"/>
+      <c r="X20" s="119"/>
+      <c r="Y20" s="119"/>
+      <c r="Z20" s="119"/>
+      <c r="AA20" s="119"/>
+      <c r="AB20" s="119"/>
+      <c r="AC20" s="119"/>
+      <c r="AD20" s="119"/>
+      <c r="AE20" s="119"/>
+      <c r="AF20" s="119"/>
+      <c r="AG20" s="119"/>
+      <c r="AH20" s="119"/>
+      <c r="AI20" s="119"/>
+      <c r="AJ20" s="119"/>
+      <c r="AK20" s="119"/>
+      <c r="AL20" s="119"/>
+      <c r="AM20" s="119"/>
+      <c r="AN20" s="119"/>
+      <c r="AO20" s="119"/>
+      <c r="AP20" s="119"/>
+      <c r="AQ20" s="119"/>
+      <c r="AR20" s="119"/>
+      <c r="AS20" s="119"/>
+      <c r="AT20" s="119"/>
+      <c r="AU20" s="119"/>
+      <c r="AV20" s="119"/>
+      <c r="AW20" s="119"/>
+      <c r="AX20" s="119"/>
+      <c r="AY20" s="119"/>
+      <c r="AZ20" s="119"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A21" s="116">
         <v>19</v>
       </c>
@@ -5907,8 +6477,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">waterYr YEAR, </v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I21" s="119"/>
+      <c r="J21" s="119"/>
+      <c r="K21" s="119"/>
+      <c r="L21" s="119"/>
+      <c r="M21" s="119"/>
+      <c r="N21" s="119"/>
+      <c r="O21" s="119"/>
+      <c r="P21" s="119"/>
+      <c r="Q21" s="119"/>
+      <c r="R21" s="119"/>
+      <c r="S21" s="119"/>
+      <c r="T21" s="119"/>
+      <c r="U21" s="119"/>
+      <c r="V21" s="119"/>
+      <c r="W21" s="119"/>
+      <c r="X21" s="119"/>
+      <c r="Y21" s="119"/>
+      <c r="Z21" s="119"/>
+      <c r="AA21" s="119"/>
+      <c r="AB21" s="119"/>
+      <c r="AC21" s="119"/>
+      <c r="AD21" s="119"/>
+      <c r="AE21" s="119"/>
+      <c r="AF21" s="119"/>
+      <c r="AG21" s="119"/>
+      <c r="AH21" s="119"/>
+      <c r="AI21" s="119"/>
+      <c r="AJ21" s="119"/>
+      <c r="AK21" s="119"/>
+      <c r="AL21" s="119"/>
+      <c r="AM21" s="119"/>
+      <c r="AN21" s="119"/>
+      <c r="AO21" s="119"/>
+      <c r="AP21" s="119"/>
+      <c r="AQ21" s="119"/>
+      <c r="AR21" s="119"/>
+      <c r="AS21" s="119"/>
+      <c r="AT21" s="119"/>
+      <c r="AU21" s="119"/>
+      <c r="AV21" s="119"/>
+      <c r="AW21" s="119"/>
+      <c r="AX21" s="119"/>
+      <c r="AY21" s="119"/>
+      <c r="AZ21" s="119"/>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A22" s="116">
         <v>20</v>
       </c>
@@ -5926,8 +6540,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">datetime TEXT, </v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="119"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="119"/>
+      <c r="P22" s="119"/>
+      <c r="Q22" s="119"/>
+      <c r="R22" s="119"/>
+      <c r="S22" s="119"/>
+      <c r="T22" s="119"/>
+      <c r="U22" s="119"/>
+      <c r="V22" s="119"/>
+      <c r="W22" s="119"/>
+      <c r="X22" s="119"/>
+      <c r="Y22" s="119"/>
+      <c r="Z22" s="119"/>
+      <c r="AA22" s="119"/>
+      <c r="AB22" s="119"/>
+      <c r="AC22" s="119"/>
+      <c r="AD22" s="119"/>
+      <c r="AE22" s="119"/>
+      <c r="AF22" s="119"/>
+      <c r="AG22" s="119"/>
+      <c r="AH22" s="119"/>
+      <c r="AI22" s="119"/>
+      <c r="AJ22" s="119"/>
+      <c r="AK22" s="119"/>
+      <c r="AL22" s="119"/>
+      <c r="AM22" s="119"/>
+      <c r="AN22" s="119"/>
+      <c r="AO22" s="119"/>
+      <c r="AP22" s="119"/>
+      <c r="AQ22" s="119"/>
+      <c r="AR22" s="119"/>
+      <c r="AS22" s="119"/>
+      <c r="AT22" s="119"/>
+      <c r="AU22" s="119"/>
+      <c r="AV22" s="119"/>
+      <c r="AW22" s="119"/>
+      <c r="AX22" s="119"/>
+      <c r="AY22" s="119"/>
+      <c r="AZ22" s="119"/>
+    </row>
+    <row r="23" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A23" s="116">
         <v>21</v>
       </c>
@@ -5946,8 +6604,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Ca DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="119"/>
+      <c r="P23" s="119"/>
+      <c r="Q23" s="119"/>
+      <c r="R23" s="119"/>
+      <c r="S23" s="119"/>
+      <c r="T23" s="119"/>
+      <c r="U23" s="119"/>
+      <c r="V23" s="119"/>
+      <c r="W23" s="119"/>
+      <c r="X23" s="119"/>
+      <c r="Y23" s="119"/>
+      <c r="Z23" s="119"/>
+      <c r="AA23" s="119"/>
+      <c r="AB23" s="119"/>
+      <c r="AC23" s="119"/>
+      <c r="AD23" s="119"/>
+      <c r="AE23" s="119"/>
+      <c r="AF23" s="119"/>
+      <c r="AG23" s="119"/>
+      <c r="AH23" s="119"/>
+      <c r="AI23" s="119"/>
+      <c r="AJ23" s="119"/>
+      <c r="AK23" s="119"/>
+      <c r="AL23" s="119"/>
+      <c r="AM23" s="119"/>
+      <c r="AN23" s="119"/>
+      <c r="AO23" s="119"/>
+      <c r="AP23" s="119"/>
+      <c r="AQ23" s="119"/>
+      <c r="AR23" s="119"/>
+      <c r="AS23" s="119"/>
+      <c r="AT23" s="119"/>
+      <c r="AU23" s="119"/>
+      <c r="AV23" s="119"/>
+      <c r="AW23" s="119"/>
+      <c r="AX23" s="119"/>
+      <c r="AY23" s="119"/>
+      <c r="AZ23" s="119"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A24" s="116">
         <v>22</v>
       </c>
@@ -5966,8 +6668,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Mg DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I24" s="119"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="119"/>
+      <c r="P24" s="119"/>
+      <c r="Q24" s="119"/>
+      <c r="R24" s="119"/>
+      <c r="S24" s="119"/>
+      <c r="T24" s="119"/>
+      <c r="U24" s="119"/>
+      <c r="V24" s="119"/>
+      <c r="W24" s="119"/>
+      <c r="X24" s="119"/>
+      <c r="Y24" s="119"/>
+      <c r="Z24" s="119"/>
+      <c r="AA24" s="119"/>
+      <c r="AB24" s="119"/>
+      <c r="AC24" s="119"/>
+      <c r="AD24" s="119"/>
+      <c r="AE24" s="119"/>
+      <c r="AF24" s="119"/>
+      <c r="AG24" s="119"/>
+      <c r="AH24" s="119"/>
+      <c r="AI24" s="119"/>
+      <c r="AJ24" s="119"/>
+      <c r="AK24" s="119"/>
+      <c r="AL24" s="119"/>
+      <c r="AM24" s="119"/>
+      <c r="AN24" s="119"/>
+      <c r="AO24" s="119"/>
+      <c r="AP24" s="119"/>
+      <c r="AQ24" s="119"/>
+      <c r="AR24" s="119"/>
+      <c r="AS24" s="119"/>
+      <c r="AT24" s="119"/>
+      <c r="AU24" s="119"/>
+      <c r="AV24" s="119"/>
+      <c r="AW24" s="119"/>
+      <c r="AX24" s="119"/>
+      <c r="AY24" s="119"/>
+      <c r="AZ24" s="119"/>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A25" s="116">
         <v>23</v>
       </c>
@@ -5986,8 +6732,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">K DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I25" s="119"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
+      <c r="P25" s="119"/>
+      <c r="Q25" s="119"/>
+      <c r="R25" s="119"/>
+      <c r="S25" s="119"/>
+      <c r="T25" s="119"/>
+      <c r="U25" s="119"/>
+      <c r="V25" s="119"/>
+      <c r="W25" s="119"/>
+      <c r="X25" s="119"/>
+      <c r="Y25" s="119"/>
+      <c r="Z25" s="119"/>
+      <c r="AA25" s="119"/>
+      <c r="AB25" s="119"/>
+      <c r="AC25" s="119"/>
+      <c r="AD25" s="119"/>
+      <c r="AE25" s="119"/>
+      <c r="AF25" s="119"/>
+      <c r="AG25" s="119"/>
+      <c r="AH25" s="119"/>
+      <c r="AI25" s="119"/>
+      <c r="AJ25" s="119"/>
+      <c r="AK25" s="119"/>
+      <c r="AL25" s="119"/>
+      <c r="AM25" s="119"/>
+      <c r="AN25" s="119"/>
+      <c r="AO25" s="119"/>
+      <c r="AP25" s="119"/>
+      <c r="AQ25" s="119"/>
+      <c r="AR25" s="119"/>
+      <c r="AS25" s="119"/>
+      <c r="AT25" s="119"/>
+      <c r="AU25" s="119"/>
+      <c r="AV25" s="119"/>
+      <c r="AW25" s="119"/>
+      <c r="AX25" s="119"/>
+      <c r="AY25" s="119"/>
+      <c r="AZ25" s="119"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A26" s="116">
         <v>24</v>
       </c>
@@ -6006,8 +6796,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Na DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119"/>
+      <c r="P26" s="119"/>
+      <c r="Q26" s="119"/>
+      <c r="R26" s="119"/>
+      <c r="S26" s="119"/>
+      <c r="T26" s="119"/>
+      <c r="U26" s="119"/>
+      <c r="V26" s="119"/>
+      <c r="W26" s="119"/>
+      <c r="X26" s="119"/>
+      <c r="Y26" s="119"/>
+      <c r="Z26" s="119"/>
+      <c r="AA26" s="119"/>
+      <c r="AB26" s="119"/>
+      <c r="AC26" s="119"/>
+      <c r="AD26" s="119"/>
+      <c r="AE26" s="119"/>
+      <c r="AF26" s="119"/>
+      <c r="AG26" s="119"/>
+      <c r="AH26" s="119"/>
+      <c r="AI26" s="119"/>
+      <c r="AJ26" s="119"/>
+      <c r="AK26" s="119"/>
+      <c r="AL26" s="119"/>
+      <c r="AM26" s="119"/>
+      <c r="AN26" s="119"/>
+      <c r="AO26" s="119"/>
+      <c r="AP26" s="119"/>
+      <c r="AQ26" s="119"/>
+      <c r="AR26" s="119"/>
+      <c r="AS26" s="119"/>
+      <c r="AT26" s="119"/>
+      <c r="AU26" s="119"/>
+      <c r="AV26" s="119"/>
+      <c r="AW26" s="119"/>
+      <c r="AX26" s="119"/>
+      <c r="AY26" s="119"/>
+      <c r="AZ26" s="119"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A27" s="116">
         <v>25</v>
       </c>
@@ -6026,8 +6860,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I27" s="119"/>
+      <c r="J27" s="119"/>
+      <c r="K27" s="119"/>
+      <c r="L27" s="119"/>
+      <c r="M27" s="119"/>
+      <c r="N27" s="119"/>
+      <c r="O27" s="119"/>
+      <c r="P27" s="119"/>
+      <c r="Q27" s="119"/>
+      <c r="R27" s="119"/>
+      <c r="S27" s="119"/>
+      <c r="T27" s="119"/>
+      <c r="U27" s="119"/>
+      <c r="V27" s="119"/>
+      <c r="W27" s="119"/>
+      <c r="X27" s="119"/>
+      <c r="Y27" s="119"/>
+      <c r="Z27" s="119"/>
+      <c r="AA27" s="119"/>
+      <c r="AB27" s="119"/>
+      <c r="AC27" s="119"/>
+      <c r="AD27" s="119"/>
+      <c r="AE27" s="119"/>
+      <c r="AF27" s="119"/>
+      <c r="AG27" s="119"/>
+      <c r="AH27" s="119"/>
+      <c r="AI27" s="119"/>
+      <c r="AJ27" s="119"/>
+      <c r="AK27" s="119"/>
+      <c r="AL27" s="119"/>
+      <c r="AM27" s="119"/>
+      <c r="AN27" s="119"/>
+      <c r="AO27" s="119"/>
+      <c r="AP27" s="119"/>
+      <c r="AQ27" s="119"/>
+      <c r="AR27" s="119"/>
+      <c r="AS27" s="119"/>
+      <c r="AT27" s="119"/>
+      <c r="AU27" s="119"/>
+      <c r="AV27" s="119"/>
+      <c r="AW27" s="119"/>
+      <c r="AX27" s="119"/>
+      <c r="AY27" s="119"/>
+      <c r="AZ27" s="119"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A28" s="116">
         <v>26</v>
       </c>
@@ -6046,8 +6924,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I28" s="119"/>
+      <c r="J28" s="119"/>
+      <c r="K28" s="119"/>
+      <c r="L28" s="119"/>
+      <c r="M28" s="119"/>
+      <c r="N28" s="119"/>
+      <c r="O28" s="119"/>
+      <c r="P28" s="119"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="119"/>
+      <c r="S28" s="119"/>
+      <c r="T28" s="119"/>
+      <c r="U28" s="119"/>
+      <c r="V28" s="119"/>
+      <c r="W28" s="119"/>
+      <c r="X28" s="119"/>
+      <c r="Y28" s="119"/>
+      <c r="Z28" s="119"/>
+      <c r="AA28" s="119"/>
+      <c r="AB28" s="119"/>
+      <c r="AC28" s="119"/>
+      <c r="AD28" s="119"/>
+      <c r="AE28" s="119"/>
+      <c r="AF28" s="119"/>
+      <c r="AG28" s="119"/>
+      <c r="AH28" s="119"/>
+      <c r="AI28" s="119"/>
+      <c r="AJ28" s="119"/>
+      <c r="AK28" s="119"/>
+      <c r="AL28" s="119"/>
+      <c r="AM28" s="119"/>
+      <c r="AN28" s="119"/>
+      <c r="AO28" s="119"/>
+      <c r="AP28" s="119"/>
+      <c r="AQ28" s="119"/>
+      <c r="AR28" s="119"/>
+      <c r="AS28" s="119"/>
+      <c r="AT28" s="119"/>
+      <c r="AU28" s="119"/>
+      <c r="AV28" s="119"/>
+      <c r="AW28" s="119"/>
+      <c r="AX28" s="119"/>
+      <c r="AY28" s="119"/>
+      <c r="AZ28" s="119"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A29" s="116">
         <v>27</v>
       </c>
@@ -6066,8 +6988,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I29" s="119"/>
+      <c r="J29" s="119"/>
+      <c r="K29" s="119"/>
+      <c r="L29" s="119"/>
+      <c r="M29" s="119"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
+      <c r="P29" s="119"/>
+      <c r="Q29" s="119"/>
+      <c r="R29" s="119"/>
+      <c r="S29" s="119"/>
+      <c r="T29" s="119"/>
+      <c r="U29" s="119"/>
+      <c r="V29" s="119"/>
+      <c r="W29" s="119"/>
+      <c r="X29" s="119"/>
+      <c r="Y29" s="119"/>
+      <c r="Z29" s="119"/>
+      <c r="AA29" s="119"/>
+      <c r="AB29" s="119"/>
+      <c r="AC29" s="119"/>
+      <c r="AD29" s="119"/>
+      <c r="AE29" s="119"/>
+      <c r="AF29" s="119"/>
+      <c r="AG29" s="119"/>
+      <c r="AH29" s="119"/>
+      <c r="AI29" s="119"/>
+      <c r="AJ29" s="119"/>
+      <c r="AK29" s="119"/>
+      <c r="AL29" s="119"/>
+      <c r="AM29" s="119"/>
+      <c r="AN29" s="119"/>
+      <c r="AO29" s="119"/>
+      <c r="AP29" s="119"/>
+      <c r="AQ29" s="119"/>
+      <c r="AR29" s="119"/>
+      <c r="AS29" s="119"/>
+      <c r="AT29" s="119"/>
+      <c r="AU29" s="119"/>
+      <c r="AV29" s="119"/>
+      <c r="AW29" s="119"/>
+      <c r="AX29" s="119"/>
+      <c r="AY29" s="119"/>
+      <c r="AZ29" s="119"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A30" s="116">
         <v>28</v>
       </c>
@@ -6086,8 +7052,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
+      <c r="P30" s="119"/>
+      <c r="Q30" s="119"/>
+      <c r="R30" s="119"/>
+      <c r="S30" s="119"/>
+      <c r="T30" s="119"/>
+      <c r="U30" s="119"/>
+      <c r="V30" s="119"/>
+      <c r="W30" s="119"/>
+      <c r="X30" s="119"/>
+      <c r="Y30" s="119"/>
+      <c r="Z30" s="119"/>
+      <c r="AA30" s="119"/>
+      <c r="AB30" s="119"/>
+      <c r="AC30" s="119"/>
+      <c r="AD30" s="119"/>
+      <c r="AE30" s="119"/>
+      <c r="AF30" s="119"/>
+      <c r="AG30" s="119"/>
+      <c r="AH30" s="119"/>
+      <c r="AI30" s="119"/>
+      <c r="AJ30" s="119"/>
+      <c r="AK30" s="119"/>
+      <c r="AL30" s="119"/>
+      <c r="AM30" s="119"/>
+      <c r="AN30" s="119"/>
+      <c r="AO30" s="119"/>
+      <c r="AP30" s="119"/>
+      <c r="AQ30" s="119"/>
+      <c r="AR30" s="119"/>
+      <c r="AS30" s="119"/>
+      <c r="AT30" s="119"/>
+      <c r="AU30" s="119"/>
+      <c r="AV30" s="119"/>
+      <c r="AW30" s="119"/>
+      <c r="AX30" s="119"/>
+      <c r="AY30" s="119"/>
+      <c r="AZ30" s="119"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A31" s="116">
         <v>29</v>
       </c>
@@ -6106,8 +7116,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
+      <c r="P31" s="119"/>
+      <c r="Q31" s="119"/>
+      <c r="R31" s="119"/>
+      <c r="S31" s="119"/>
+      <c r="T31" s="119"/>
+      <c r="U31" s="119"/>
+      <c r="V31" s="119"/>
+      <c r="W31" s="119"/>
+      <c r="X31" s="119"/>
+      <c r="Y31" s="119"/>
+      <c r="Z31" s="119"/>
+      <c r="AA31" s="119"/>
+      <c r="AB31" s="119"/>
+      <c r="AC31" s="119"/>
+      <c r="AD31" s="119"/>
+      <c r="AE31" s="119"/>
+      <c r="AF31" s="119"/>
+      <c r="AG31" s="119"/>
+      <c r="AH31" s="119"/>
+      <c r="AI31" s="119"/>
+      <c r="AJ31" s="119"/>
+      <c r="AK31" s="119"/>
+      <c r="AL31" s="119"/>
+      <c r="AM31" s="119"/>
+      <c r="AN31" s="119"/>
+      <c r="AO31" s="119"/>
+      <c r="AP31" s="119"/>
+      <c r="AQ31" s="119"/>
+      <c r="AR31" s="119"/>
+      <c r="AS31" s="119"/>
+      <c r="AT31" s="119"/>
+      <c r="AU31" s="119"/>
+      <c r="AV31" s="119"/>
+      <c r="AW31" s="119"/>
+      <c r="AX31" s="119"/>
+      <c r="AY31" s="119"/>
+      <c r="AZ31" s="119"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A32" s="116">
         <v>30</v>
       </c>
@@ -6126,8 +7180,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I32" s="119"/>
+      <c r="J32" s="119"/>
+      <c r="K32" s="119"/>
+      <c r="L32" s="119"/>
+      <c r="M32" s="119"/>
+      <c r="N32" s="119"/>
+      <c r="O32" s="119"/>
+      <c r="P32" s="119"/>
+      <c r="Q32" s="119"/>
+      <c r="R32" s="119"/>
+      <c r="S32" s="119"/>
+      <c r="T32" s="119"/>
+      <c r="U32" s="119"/>
+      <c r="V32" s="119"/>
+      <c r="W32" s="119"/>
+      <c r="X32" s="119"/>
+      <c r="Y32" s="119"/>
+      <c r="Z32" s="119"/>
+      <c r="AA32" s="119"/>
+      <c r="AB32" s="119"/>
+      <c r="AC32" s="119"/>
+      <c r="AD32" s="119"/>
+      <c r="AE32" s="119"/>
+      <c r="AF32" s="119"/>
+      <c r="AG32" s="119"/>
+      <c r="AH32" s="119"/>
+      <c r="AI32" s="119"/>
+      <c r="AJ32" s="119"/>
+      <c r="AK32" s="119"/>
+      <c r="AL32" s="119"/>
+      <c r="AM32" s="119"/>
+      <c r="AN32" s="119"/>
+      <c r="AO32" s="119"/>
+      <c r="AP32" s="119"/>
+      <c r="AQ32" s="119"/>
+      <c r="AR32" s="119"/>
+      <c r="AS32" s="119"/>
+      <c r="AT32" s="119"/>
+      <c r="AU32" s="119"/>
+      <c r="AV32" s="119"/>
+      <c r="AW32" s="119"/>
+      <c r="AX32" s="119"/>
+      <c r="AY32" s="119"/>
+      <c r="AZ32" s="119"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A33" s="116">
         <v>31</v>
       </c>
@@ -6146,8 +7244,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Cl DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I33" s="119"/>
+      <c r="J33" s="119"/>
+      <c r="K33" s="119"/>
+      <c r="L33" s="119"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
+      <c r="P33" s="119"/>
+      <c r="Q33" s="119"/>
+      <c r="R33" s="119"/>
+      <c r="S33" s="119"/>
+      <c r="T33" s="119"/>
+      <c r="U33" s="119"/>
+      <c r="V33" s="119"/>
+      <c r="W33" s="119"/>
+      <c r="X33" s="119"/>
+      <c r="Y33" s="119"/>
+      <c r="Z33" s="119"/>
+      <c r="AA33" s="119"/>
+      <c r="AB33" s="119"/>
+      <c r="AC33" s="119"/>
+      <c r="AD33" s="119"/>
+      <c r="AE33" s="119"/>
+      <c r="AF33" s="119"/>
+      <c r="AG33" s="119"/>
+      <c r="AH33" s="119"/>
+      <c r="AI33" s="119"/>
+      <c r="AJ33" s="119"/>
+      <c r="AK33" s="119"/>
+      <c r="AL33" s="119"/>
+      <c r="AM33" s="119"/>
+      <c r="AN33" s="119"/>
+      <c r="AO33" s="119"/>
+      <c r="AP33" s="119"/>
+      <c r="AQ33" s="119"/>
+      <c r="AR33" s="119"/>
+      <c r="AS33" s="119"/>
+      <c r="AT33" s="119"/>
+      <c r="AU33" s="119"/>
+      <c r="AV33" s="119"/>
+      <c r="AW33" s="119"/>
+      <c r="AX33" s="119"/>
+      <c r="AY33" s="119"/>
+      <c r="AZ33" s="119"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A34" s="116">
         <v>32</v>
       </c>
@@ -6166,8 +7308,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I34" s="119"/>
+      <c r="J34" s="119"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
+      <c r="N34" s="119"/>
+      <c r="O34" s="119"/>
+      <c r="P34" s="119"/>
+      <c r="Q34" s="119"/>
+      <c r="R34" s="119"/>
+      <c r="S34" s="119"/>
+      <c r="T34" s="119"/>
+      <c r="U34" s="119"/>
+      <c r="V34" s="119"/>
+      <c r="W34" s="119"/>
+      <c r="X34" s="119"/>
+      <c r="Y34" s="119"/>
+      <c r="Z34" s="119"/>
+      <c r="AA34" s="119"/>
+      <c r="AB34" s="119"/>
+      <c r="AC34" s="119"/>
+      <c r="AD34" s="119"/>
+      <c r="AE34" s="119"/>
+      <c r="AF34" s="119"/>
+      <c r="AG34" s="119"/>
+      <c r="AH34" s="119"/>
+      <c r="AI34" s="119"/>
+      <c r="AJ34" s="119"/>
+      <c r="AK34" s="119"/>
+      <c r="AL34" s="119"/>
+      <c r="AM34" s="119"/>
+      <c r="AN34" s="119"/>
+      <c r="AO34" s="119"/>
+      <c r="AP34" s="119"/>
+      <c r="AQ34" s="119"/>
+      <c r="AR34" s="119"/>
+      <c r="AS34" s="119"/>
+      <c r="AT34" s="119"/>
+      <c r="AU34" s="119"/>
+      <c r="AV34" s="119"/>
+      <c r="AW34" s="119"/>
+      <c r="AX34" s="119"/>
+      <c r="AY34" s="119"/>
+      <c r="AZ34" s="119"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A35" s="116">
         <v>33</v>
       </c>
@@ -6186,8 +7372,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">DOC DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I35" s="119"/>
+      <c r="J35" s="119"/>
+      <c r="K35" s="119"/>
+      <c r="L35" s="119"/>
+      <c r="M35" s="119"/>
+      <c r="N35" s="119"/>
+      <c r="O35" s="119"/>
+      <c r="P35" s="119"/>
+      <c r="Q35" s="119"/>
+      <c r="R35" s="119"/>
+      <c r="S35" s="119"/>
+      <c r="T35" s="119"/>
+      <c r="U35" s="119"/>
+      <c r="V35" s="119"/>
+      <c r="W35" s="119"/>
+      <c r="X35" s="119"/>
+      <c r="Y35" s="119"/>
+      <c r="Z35" s="119"/>
+      <c r="AA35" s="119"/>
+      <c r="AB35" s="119"/>
+      <c r="AC35" s="119"/>
+      <c r="AD35" s="119"/>
+      <c r="AE35" s="119"/>
+      <c r="AF35" s="119"/>
+      <c r="AG35" s="119"/>
+      <c r="AH35" s="119"/>
+      <c r="AI35" s="119"/>
+      <c r="AJ35" s="119"/>
+      <c r="AK35" s="119"/>
+      <c r="AL35" s="119"/>
+      <c r="AM35" s="119"/>
+      <c r="AN35" s="119"/>
+      <c r="AO35" s="119"/>
+      <c r="AP35" s="119"/>
+      <c r="AQ35" s="119"/>
+      <c r="AR35" s="119"/>
+      <c r="AS35" s="119"/>
+      <c r="AT35" s="119"/>
+      <c r="AU35" s="119"/>
+      <c r="AV35" s="119"/>
+      <c r="AW35" s="119"/>
+      <c r="AX35" s="119"/>
+      <c r="AY35" s="119"/>
+      <c r="AZ35" s="119"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A36" s="116">
         <v>34</v>
       </c>
@@ -6206,8 +7436,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">TDN DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I36" s="119"/>
+      <c r="J36" s="119"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="119"/>
+      <c r="N36" s="119"/>
+      <c r="O36" s="119"/>
+      <c r="P36" s="119"/>
+      <c r="Q36" s="119"/>
+      <c r="R36" s="119"/>
+      <c r="S36" s="119"/>
+      <c r="T36" s="119"/>
+      <c r="U36" s="119"/>
+      <c r="V36" s="119"/>
+      <c r="W36" s="119"/>
+      <c r="X36" s="119"/>
+      <c r="Y36" s="119"/>
+      <c r="Z36" s="119"/>
+      <c r="AA36" s="119"/>
+      <c r="AB36" s="119"/>
+      <c r="AC36" s="119"/>
+      <c r="AD36" s="119"/>
+      <c r="AE36" s="119"/>
+      <c r="AF36" s="119"/>
+      <c r="AG36" s="119"/>
+      <c r="AH36" s="119"/>
+      <c r="AI36" s="119"/>
+      <c r="AJ36" s="119"/>
+      <c r="AK36" s="119"/>
+      <c r="AL36" s="119"/>
+      <c r="AM36" s="119"/>
+      <c r="AN36" s="119"/>
+      <c r="AO36" s="119"/>
+      <c r="AP36" s="119"/>
+      <c r="AQ36" s="119"/>
+      <c r="AR36" s="119"/>
+      <c r="AS36" s="119"/>
+      <c r="AT36" s="119"/>
+      <c r="AU36" s="119"/>
+      <c r="AV36" s="119"/>
+      <c r="AW36" s="119"/>
+      <c r="AX36" s="119"/>
+      <c r="AY36" s="119"/>
+      <c r="AZ36" s="119"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A37" s="116">
         <v>35</v>
       </c>
@@ -6226,8 +7500,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">DON DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I37" s="119"/>
+      <c r="J37" s="119"/>
+      <c r="K37" s="119"/>
+      <c r="L37" s="119"/>
+      <c r="M37" s="119"/>
+      <c r="N37" s="119"/>
+      <c r="O37" s="119"/>
+      <c r="P37" s="119"/>
+      <c r="Q37" s="119"/>
+      <c r="R37" s="119"/>
+      <c r="S37" s="119"/>
+      <c r="T37" s="119"/>
+      <c r="U37" s="119"/>
+      <c r="V37" s="119"/>
+      <c r="W37" s="119"/>
+      <c r="X37" s="119"/>
+      <c r="Y37" s="119"/>
+      <c r="Z37" s="119"/>
+      <c r="AA37" s="119"/>
+      <c r="AB37" s="119"/>
+      <c r="AC37" s="119"/>
+      <c r="AD37" s="119"/>
+      <c r="AE37" s="119"/>
+      <c r="AF37" s="119"/>
+      <c r="AG37" s="119"/>
+      <c r="AH37" s="119"/>
+      <c r="AI37" s="119"/>
+      <c r="AJ37" s="119"/>
+      <c r="AK37" s="119"/>
+      <c r="AL37" s="119"/>
+      <c r="AM37" s="119"/>
+      <c r="AN37" s="119"/>
+      <c r="AO37" s="119"/>
+      <c r="AP37" s="119"/>
+      <c r="AQ37" s="119"/>
+      <c r="AR37" s="119"/>
+      <c r="AS37" s="119"/>
+      <c r="AT37" s="119"/>
+      <c r="AU37" s="119"/>
+      <c r="AV37" s="119"/>
+      <c r="AW37" s="119"/>
+      <c r="AX37" s="119"/>
+      <c r="AY37" s="119"/>
+      <c r="AZ37" s="119"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A38" s="116">
         <v>36</v>
       </c>
@@ -6246,8 +7564,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="119"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
+      <c r="N38" s="119"/>
+      <c r="O38" s="119"/>
+      <c r="P38" s="119"/>
+      <c r="Q38" s="119"/>
+      <c r="R38" s="119"/>
+      <c r="S38" s="119"/>
+      <c r="T38" s="119"/>
+      <c r="U38" s="119"/>
+      <c r="V38" s="119"/>
+      <c r="W38" s="119"/>
+      <c r="X38" s="119"/>
+      <c r="Y38" s="119"/>
+      <c r="Z38" s="119"/>
+      <c r="AA38" s="119"/>
+      <c r="AB38" s="119"/>
+      <c r="AC38" s="119"/>
+      <c r="AD38" s="119"/>
+      <c r="AE38" s="119"/>
+      <c r="AF38" s="119"/>
+      <c r="AG38" s="119"/>
+      <c r="AH38" s="119"/>
+      <c r="AI38" s="119"/>
+      <c r="AJ38" s="119"/>
+      <c r="AK38" s="119"/>
+      <c r="AL38" s="119"/>
+      <c r="AM38" s="119"/>
+      <c r="AN38" s="119"/>
+      <c r="AO38" s="119"/>
+      <c r="AP38" s="119"/>
+      <c r="AQ38" s="119"/>
+      <c r="AR38" s="119"/>
+      <c r="AS38" s="119"/>
+      <c r="AT38" s="119"/>
+      <c r="AU38" s="119"/>
+      <c r="AV38" s="119"/>
+      <c r="AW38" s="119"/>
+      <c r="AX38" s="119"/>
+      <c r="AY38" s="119"/>
+      <c r="AZ38" s="119"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A39" s="116">
         <v>37</v>
       </c>
@@ -6266,8 +7628,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Mn DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="119"/>
+      <c r="P39" s="119"/>
+      <c r="Q39" s="119"/>
+      <c r="R39" s="119"/>
+      <c r="S39" s="119"/>
+      <c r="T39" s="119"/>
+      <c r="U39" s="119"/>
+      <c r="V39" s="119"/>
+      <c r="W39" s="119"/>
+      <c r="X39" s="119"/>
+      <c r="Y39" s="119"/>
+      <c r="Z39" s="119"/>
+      <c r="AA39" s="119"/>
+      <c r="AB39" s="119"/>
+      <c r="AC39" s="119"/>
+      <c r="AD39" s="119"/>
+      <c r="AE39" s="119"/>
+      <c r="AF39" s="119"/>
+      <c r="AG39" s="119"/>
+      <c r="AH39" s="119"/>
+      <c r="AI39" s="119"/>
+      <c r="AJ39" s="119"/>
+      <c r="AK39" s="119"/>
+      <c r="AL39" s="119"/>
+      <c r="AM39" s="119"/>
+      <c r="AN39" s="119"/>
+      <c r="AO39" s="119"/>
+      <c r="AP39" s="119"/>
+      <c r="AQ39" s="119"/>
+      <c r="AR39" s="119"/>
+      <c r="AS39" s="119"/>
+      <c r="AT39" s="119"/>
+      <c r="AU39" s="119"/>
+      <c r="AV39" s="119"/>
+      <c r="AW39" s="119"/>
+      <c r="AX39" s="119"/>
+      <c r="AY39" s="119"/>
+      <c r="AZ39" s="119"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A40" s="116">
         <v>38</v>
       </c>
@@ -6286,8 +7692,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">Fe DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
+      <c r="M40" s="119"/>
+      <c r="N40" s="119"/>
+      <c r="O40" s="119"/>
+      <c r="P40" s="119"/>
+      <c r="Q40" s="119"/>
+      <c r="R40" s="119"/>
+      <c r="S40" s="119"/>
+      <c r="T40" s="119"/>
+      <c r="U40" s="119"/>
+      <c r="V40" s="119"/>
+      <c r="W40" s="119"/>
+      <c r="X40" s="119"/>
+      <c r="Y40" s="119"/>
+      <c r="Z40" s="119"/>
+      <c r="AA40" s="119"/>
+      <c r="AB40" s="119"/>
+      <c r="AC40" s="119"/>
+      <c r="AD40" s="119"/>
+      <c r="AE40" s="119"/>
+      <c r="AF40" s="119"/>
+      <c r="AG40" s="119"/>
+      <c r="AH40" s="119"/>
+      <c r="AI40" s="119"/>
+      <c r="AJ40" s="119"/>
+      <c r="AK40" s="119"/>
+      <c r="AL40" s="119"/>
+      <c r="AM40" s="119"/>
+      <c r="AN40" s="119"/>
+      <c r="AO40" s="119"/>
+      <c r="AP40" s="119"/>
+      <c r="AQ40" s="119"/>
+      <c r="AR40" s="119"/>
+      <c r="AS40" s="119"/>
+      <c r="AT40" s="119"/>
+      <c r="AU40" s="119"/>
+      <c r="AV40" s="119"/>
+      <c r="AW40" s="119"/>
+      <c r="AX40" s="119"/>
+      <c r="AY40" s="119"/>
+      <c r="AZ40" s="119"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A41" s="116">
         <v>39</v>
       </c>
@@ -6306,8 +7756,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">F DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I41" s="119"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="119"/>
+      <c r="L41" s="119"/>
+      <c r="M41" s="119"/>
+      <c r="N41" s="119"/>
+      <c r="O41" s="119"/>
+      <c r="P41" s="119"/>
+      <c r="Q41" s="119"/>
+      <c r="R41" s="119"/>
+      <c r="S41" s="119"/>
+      <c r="T41" s="119"/>
+      <c r="U41" s="119"/>
+      <c r="V41" s="119"/>
+      <c r="W41" s="119"/>
+      <c r="X41" s="119"/>
+      <c r="Y41" s="119"/>
+      <c r="Z41" s="119"/>
+      <c r="AA41" s="119"/>
+      <c r="AB41" s="119"/>
+      <c r="AC41" s="119"/>
+      <c r="AD41" s="119"/>
+      <c r="AE41" s="119"/>
+      <c r="AF41" s="119"/>
+      <c r="AG41" s="119"/>
+      <c r="AH41" s="119"/>
+      <c r="AI41" s="119"/>
+      <c r="AJ41" s="119"/>
+      <c r="AK41" s="119"/>
+      <c r="AL41" s="119"/>
+      <c r="AM41" s="119"/>
+      <c r="AN41" s="119"/>
+      <c r="AO41" s="119"/>
+      <c r="AP41" s="119"/>
+      <c r="AQ41" s="119"/>
+      <c r="AR41" s="119"/>
+      <c r="AS41" s="119"/>
+      <c r="AT41" s="119"/>
+      <c r="AU41" s="119"/>
+      <c r="AV41" s="119"/>
+      <c r="AW41" s="119"/>
+      <c r="AX41" s="119"/>
+      <c r="AY41" s="119"/>
+      <c r="AZ41" s="119"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A42" s="116">
         <v>40</v>
       </c>
@@ -6323,8 +7817,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I42" s="119"/>
+      <c r="J42" s="119"/>
+      <c r="K42" s="119"/>
+      <c r="L42" s="119"/>
+      <c r="M42" s="119"/>
+      <c r="N42" s="119"/>
+      <c r="O42" s="119"/>
+      <c r="P42" s="119"/>
+      <c r="Q42" s="119"/>
+      <c r="R42" s="119"/>
+      <c r="S42" s="119"/>
+      <c r="T42" s="119"/>
+      <c r="U42" s="119"/>
+      <c r="V42" s="119"/>
+      <c r="W42" s="119"/>
+      <c r="X42" s="119"/>
+      <c r="Y42" s="119"/>
+      <c r="Z42" s="119"/>
+      <c r="AA42" s="119"/>
+      <c r="AB42" s="119"/>
+      <c r="AC42" s="119"/>
+      <c r="AD42" s="119"/>
+      <c r="AE42" s="119"/>
+      <c r="AF42" s="119"/>
+      <c r="AG42" s="119"/>
+      <c r="AH42" s="119"/>
+      <c r="AI42" s="119"/>
+      <c r="AJ42" s="119"/>
+      <c r="AK42" s="119"/>
+      <c r="AL42" s="119"/>
+      <c r="AM42" s="119"/>
+      <c r="AN42" s="119"/>
+      <c r="AO42" s="119"/>
+      <c r="AP42" s="119"/>
+      <c r="AQ42" s="119"/>
+      <c r="AR42" s="119"/>
+      <c r="AS42" s="119"/>
+      <c r="AT42" s="119"/>
+      <c r="AU42" s="119"/>
+      <c r="AV42" s="119"/>
+      <c r="AW42" s="119"/>
+      <c r="AX42" s="119"/>
+      <c r="AY42" s="119"/>
+      <c r="AZ42" s="119"/>
+    </row>
+    <row r="43" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A43" s="116">
         <v>41</v>
       </c>
@@ -6340,8 +7878,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="119"/>
+      <c r="N43" s="119"/>
+      <c r="O43" s="119"/>
+      <c r="P43" s="119"/>
+      <c r="Q43" s="119"/>
+      <c r="R43" s="119"/>
+      <c r="S43" s="119"/>
+      <c r="T43" s="119"/>
+      <c r="U43" s="119"/>
+      <c r="V43" s="119"/>
+      <c r="W43" s="119"/>
+      <c r="X43" s="119"/>
+      <c r="Y43" s="119"/>
+      <c r="Z43" s="119"/>
+      <c r="AA43" s="119"/>
+      <c r="AB43" s="119"/>
+      <c r="AC43" s="119"/>
+      <c r="AD43" s="119"/>
+      <c r="AE43" s="119"/>
+      <c r="AF43" s="119"/>
+      <c r="AG43" s="119"/>
+      <c r="AH43" s="119"/>
+      <c r="AI43" s="119"/>
+      <c r="AJ43" s="119"/>
+      <c r="AK43" s="119"/>
+      <c r="AL43" s="119"/>
+      <c r="AM43" s="119"/>
+      <c r="AN43" s="119"/>
+      <c r="AO43" s="119"/>
+      <c r="AP43" s="119"/>
+      <c r="AQ43" s="119"/>
+      <c r="AR43" s="119"/>
+      <c r="AS43" s="119"/>
+      <c r="AT43" s="119"/>
+      <c r="AU43" s="119"/>
+      <c r="AV43" s="119"/>
+      <c r="AW43" s="119"/>
+      <c r="AX43" s="119"/>
+      <c r="AY43" s="119"/>
+      <c r="AZ43" s="119"/>
+    </row>
+    <row r="44" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A44" s="116">
         <v>42</v>
       </c>
@@ -6357,8 +7939,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="119"/>
+      <c r="M44" s="119"/>
+      <c r="N44" s="119"/>
+      <c r="O44" s="119"/>
+      <c r="P44" s="119"/>
+      <c r="Q44" s="119"/>
+      <c r="R44" s="119"/>
+      <c r="S44" s="119"/>
+      <c r="T44" s="119"/>
+      <c r="U44" s="119"/>
+      <c r="V44" s="119"/>
+      <c r="W44" s="119"/>
+      <c r="X44" s="119"/>
+      <c r="Y44" s="119"/>
+      <c r="Z44" s="119"/>
+      <c r="AA44" s="119"/>
+      <c r="AB44" s="119"/>
+      <c r="AC44" s="119"/>
+      <c r="AD44" s="119"/>
+      <c r="AE44" s="119"/>
+      <c r="AF44" s="119"/>
+      <c r="AG44" s="119"/>
+      <c r="AH44" s="119"/>
+      <c r="AI44" s="119"/>
+      <c r="AJ44" s="119"/>
+      <c r="AK44" s="119"/>
+      <c r="AL44" s="119"/>
+      <c r="AM44" s="119"/>
+      <c r="AN44" s="119"/>
+      <c r="AO44" s="119"/>
+      <c r="AP44" s="119"/>
+      <c r="AQ44" s="119"/>
+      <c r="AR44" s="119"/>
+      <c r="AS44" s="119"/>
+      <c r="AT44" s="119"/>
+      <c r="AU44" s="119"/>
+      <c r="AV44" s="119"/>
+      <c r="AW44" s="119"/>
+      <c r="AX44" s="119"/>
+      <c r="AY44" s="119"/>
+      <c r="AZ44" s="119"/>
+    </row>
+    <row r="45" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A45" s="116">
         <v>43</v>
       </c>
@@ -6377,8 +8003,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">ionError DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I45" s="119"/>
+      <c r="J45" s="119"/>
+      <c r="K45" s="119"/>
+      <c r="L45" s="119"/>
+      <c r="M45" s="119"/>
+      <c r="N45" s="119"/>
+      <c r="O45" s="119"/>
+      <c r="P45" s="119"/>
+      <c r="Q45" s="119"/>
+      <c r="R45" s="119"/>
+      <c r="S45" s="119"/>
+      <c r="T45" s="119"/>
+      <c r="U45" s="119"/>
+      <c r="V45" s="119"/>
+      <c r="W45" s="119"/>
+      <c r="X45" s="119"/>
+      <c r="Y45" s="119"/>
+      <c r="Z45" s="119"/>
+      <c r="AA45" s="119"/>
+      <c r="AB45" s="119"/>
+      <c r="AC45" s="119"/>
+      <c r="AD45" s="119"/>
+      <c r="AE45" s="119"/>
+      <c r="AF45" s="119"/>
+      <c r="AG45" s="119"/>
+      <c r="AH45" s="119"/>
+      <c r="AI45" s="119"/>
+      <c r="AJ45" s="119"/>
+      <c r="AK45" s="119"/>
+      <c r="AL45" s="119"/>
+      <c r="AM45" s="119"/>
+      <c r="AN45" s="119"/>
+      <c r="AO45" s="119"/>
+      <c r="AP45" s="119"/>
+      <c r="AQ45" s="119"/>
+      <c r="AR45" s="119"/>
+      <c r="AS45" s="119"/>
+      <c r="AT45" s="119"/>
+      <c r="AU45" s="119"/>
+      <c r="AV45" s="119"/>
+      <c r="AW45" s="119"/>
+      <c r="AX45" s="119"/>
+      <c r="AY45" s="119"/>
+      <c r="AZ45" s="119"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A46" s="116">
         <v>44</v>
       </c>
@@ -6394,8 +8064,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">duplicate VARCHAR(10), </v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I46" s="119"/>
+      <c r="J46" s="119"/>
+      <c r="K46" s="119"/>
+      <c r="L46" s="119"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="119"/>
+      <c r="O46" s="119"/>
+      <c r="P46" s="119"/>
+      <c r="Q46" s="119"/>
+      <c r="R46" s="119"/>
+      <c r="S46" s="119"/>
+      <c r="T46" s="119"/>
+      <c r="U46" s="119"/>
+      <c r="V46" s="119"/>
+      <c r="W46" s="119"/>
+      <c r="X46" s="119"/>
+      <c r="Y46" s="119"/>
+      <c r="Z46" s="119"/>
+      <c r="AA46" s="119"/>
+      <c r="AB46" s="119"/>
+      <c r="AC46" s="119"/>
+      <c r="AD46" s="119"/>
+      <c r="AE46" s="119"/>
+      <c r="AF46" s="119"/>
+      <c r="AG46" s="119"/>
+      <c r="AH46" s="119"/>
+      <c r="AI46" s="119"/>
+      <c r="AJ46" s="119"/>
+      <c r="AK46" s="119"/>
+      <c r="AL46" s="119"/>
+      <c r="AM46" s="119"/>
+      <c r="AN46" s="119"/>
+      <c r="AO46" s="119"/>
+      <c r="AP46" s="119"/>
+      <c r="AQ46" s="119"/>
+      <c r="AR46" s="119"/>
+      <c r="AS46" s="119"/>
+      <c r="AT46" s="119"/>
+      <c r="AU46" s="119"/>
+      <c r="AV46" s="119"/>
+      <c r="AW46" s="119"/>
+      <c r="AX46" s="119"/>
+      <c r="AY46" s="119"/>
+      <c r="AZ46" s="119"/>
+    </row>
+    <row r="47" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A47" s="116">
         <v>45</v>
       </c>
@@ -6411,8 +8125,52 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">sampleType VARCHAR(20), </v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I47" s="119"/>
+      <c r="J47" s="119"/>
+      <c r="K47" s="119"/>
+      <c r="L47" s="119"/>
+      <c r="M47" s="119"/>
+      <c r="N47" s="119"/>
+      <c r="O47" s="119"/>
+      <c r="P47" s="119"/>
+      <c r="Q47" s="119"/>
+      <c r="R47" s="119"/>
+      <c r="S47" s="119"/>
+      <c r="T47" s="119"/>
+      <c r="U47" s="119"/>
+      <c r="V47" s="119"/>
+      <c r="W47" s="119"/>
+      <c r="X47" s="119"/>
+      <c r="Y47" s="119"/>
+      <c r="Z47" s="119"/>
+      <c r="AA47" s="119"/>
+      <c r="AB47" s="119"/>
+      <c r="AC47" s="119"/>
+      <c r="AD47" s="119"/>
+      <c r="AE47" s="119"/>
+      <c r="AF47" s="119"/>
+      <c r="AG47" s="119"/>
+      <c r="AH47" s="119"/>
+      <c r="AI47" s="119"/>
+      <c r="AJ47" s="119"/>
+      <c r="AK47" s="119"/>
+      <c r="AL47" s="119"/>
+      <c r="AM47" s="119"/>
+      <c r="AN47" s="119"/>
+      <c r="AO47" s="119"/>
+      <c r="AP47" s="119"/>
+      <c r="AQ47" s="119"/>
+      <c r="AR47" s="119"/>
+      <c r="AS47" s="119"/>
+      <c r="AT47" s="119"/>
+      <c r="AU47" s="119"/>
+      <c r="AV47" s="119"/>
+      <c r="AW47" s="119"/>
+      <c r="AX47" s="119"/>
+      <c r="AY47" s="119"/>
+      <c r="AZ47" s="119"/>
+    </row>
+    <row r="48" spans="1:52" x14ac:dyDescent="0.15">
       <c r="A48" s="116">
         <v>46</v>
       </c>
@@ -6431,48 +8189,234 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
       </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="I48" s="119"/>
+      <c r="J48" s="119"/>
+      <c r="K48" s="119"/>
+      <c r="L48" s="119"/>
+      <c r="M48" s="119"/>
+      <c r="N48" s="119"/>
+      <c r="O48" s="119"/>
+      <c r="P48" s="119"/>
+      <c r="Q48" s="119"/>
+      <c r="R48" s="119"/>
+      <c r="S48" s="119"/>
+      <c r="T48" s="119"/>
+      <c r="U48" s="119"/>
+      <c r="V48" s="119"/>
+      <c r="W48" s="119"/>
+      <c r="X48" s="119"/>
+      <c r="Y48" s="119"/>
+      <c r="Z48" s="119"/>
+      <c r="AA48" s="119"/>
+      <c r="AB48" s="119"/>
+      <c r="AC48" s="119"/>
+      <c r="AD48" s="119"/>
+      <c r="AE48" s="119"/>
+      <c r="AF48" s="119"/>
+      <c r="AG48" s="119"/>
+      <c r="AH48" s="119"/>
+      <c r="AI48" s="119"/>
+      <c r="AJ48" s="119"/>
+      <c r="AK48" s="119"/>
+      <c r="AL48" s="119"/>
+      <c r="AM48" s="119"/>
+      <c r="AN48" s="119"/>
+      <c r="AO48" s="119"/>
+      <c r="AP48" s="119"/>
+      <c r="AQ48" s="119"/>
+      <c r="AR48" s="119"/>
+      <c r="AS48" s="119"/>
+      <c r="AT48" s="119"/>
+      <c r="AU48" s="119"/>
+      <c r="AV48" s="119"/>
+      <c r="AW48" s="119"/>
+      <c r="AX48" s="119"/>
+      <c r="AY48" s="119"/>
+      <c r="AZ48" s="119"/>
+    </row>
+    <row r="49" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C49" s="99" t="s">
         <v>204</v>
       </c>
       <c r="D49" s="117"/>
-      <c r="E49" s="117"/>
+      <c r="E49" s="117" t="s">
+        <v>209</v>
+      </c>
       <c r="F49" s="118"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="I49" s="119"/>
+      <c r="J49" s="119"/>
+      <c r="K49" s="119"/>
+      <c r="L49" s="119"/>
+      <c r="M49" s="119"/>
+      <c r="N49" s="119"/>
+      <c r="O49" s="119"/>
+      <c r="P49" s="119"/>
+      <c r="Q49" s="119"/>
+      <c r="R49" s="119"/>
+      <c r="S49" s="119"/>
+      <c r="T49" s="119"/>
+      <c r="U49" s="119"/>
+      <c r="V49" s="119"/>
+      <c r="W49" s="119"/>
+      <c r="X49" s="119"/>
+      <c r="Y49" s="119"/>
+      <c r="Z49" s="119"/>
+      <c r="AA49" s="119"/>
+      <c r="AB49" s="119"/>
+      <c r="AC49" s="119"/>
+      <c r="AD49" s="119"/>
+      <c r="AE49" s="119"/>
+      <c r="AF49" s="119"/>
+      <c r="AG49" s="119"/>
+      <c r="AH49" s="119"/>
+      <c r="AI49" s="119"/>
+      <c r="AJ49" s="119"/>
+      <c r="AK49" s="119"/>
+      <c r="AL49" s="119"/>
+      <c r="AM49" s="119"/>
+      <c r="AN49" s="119"/>
+      <c r="AO49" s="119"/>
+      <c r="AP49" s="119"/>
+      <c r="AQ49" s="119"/>
+      <c r="AR49" s="119"/>
+      <c r="AS49" s="119"/>
+      <c r="AT49" s="119"/>
+      <c r="AU49" s="119"/>
+      <c r="AV49" s="119"/>
+      <c r="AW49" s="119"/>
+      <c r="AX49" s="119"/>
+      <c r="AY49" s="119"/>
+      <c r="AZ49" s="119"/>
+    </row>
+    <row r="50" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C50" s="99" t="s">
         <v>205</v>
       </c>
       <c r="D50" s="118"/>
-      <c r="E50" s="117"/>
+      <c r="E50" s="117" t="s">
+        <v>209</v>
+      </c>
       <c r="F50" s="118"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="I50" s="119"/>
+      <c r="J50" s="119"/>
+      <c r="K50" s="119"/>
+      <c r="L50" s="119"/>
+      <c r="M50" s="119"/>
+      <c r="N50" s="119"/>
+      <c r="O50" s="119"/>
+      <c r="P50" s="119"/>
+      <c r="Q50" s="119"/>
+      <c r="R50" s="119"/>
+      <c r="S50" s="119"/>
+      <c r="T50" s="119"/>
+      <c r="U50" s="119"/>
+      <c r="V50" s="119"/>
+      <c r="W50" s="119"/>
+      <c r="X50" s="119"/>
+      <c r="Y50" s="119"/>
+      <c r="Z50" s="119"/>
+      <c r="AA50" s="119"/>
+      <c r="AB50" s="119"/>
+      <c r="AC50" s="119"/>
+      <c r="AD50" s="119"/>
+      <c r="AE50" s="119"/>
+      <c r="AF50" s="119"/>
+      <c r="AG50" s="119"/>
+      <c r="AH50" s="119"/>
+      <c r="AI50" s="119"/>
+      <c r="AJ50" s="119"/>
+      <c r="AK50" s="119"/>
+      <c r="AL50" s="119"/>
+      <c r="AM50" s="119"/>
+      <c r="AN50" s="119"/>
+      <c r="AO50" s="119"/>
+      <c r="AP50" s="119"/>
+      <c r="AQ50" s="119"/>
+      <c r="AR50" s="119"/>
+      <c r="AS50" s="119"/>
+      <c r="AT50" s="119"/>
+      <c r="AU50" s="119"/>
+      <c r="AV50" s="119"/>
+      <c r="AW50" s="119"/>
+      <c r="AX50" s="119"/>
+      <c r="AY50" s="119"/>
+      <c r="AZ50" s="119"/>
+    </row>
+    <row r="51" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C51" t="s">
         <v>206</v>
       </c>
       <c r="D51" s="118"/>
-      <c r="E51" s="117"/>
+      <c r="E51" s="117" t="s">
+        <v>209</v>
+      </c>
       <c r="F51" s="118"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="I51" s="119"/>
+      <c r="J51" s="119"/>
+      <c r="K51" s="119"/>
+      <c r="L51" s="119"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="119"/>
+      <c r="O51" s="119"/>
+      <c r="P51" s="119"/>
+      <c r="Q51" s="119"/>
+      <c r="R51" s="119"/>
+      <c r="S51" s="119"/>
+      <c r="T51" s="119"/>
+      <c r="U51" s="119"/>
+      <c r="V51" s="119"/>
+      <c r="W51" s="119"/>
+      <c r="X51" s="119"/>
+      <c r="Y51" s="119"/>
+      <c r="Z51" s="119"/>
+      <c r="AA51" s="119"/>
+      <c r="AB51" s="119"/>
+      <c r="AC51" s="119"/>
+      <c r="AD51" s="119"/>
+      <c r="AE51" s="119"/>
+      <c r="AF51" s="119"/>
+      <c r="AG51" s="119"/>
+      <c r="AH51" s="119"/>
+      <c r="AI51" s="119"/>
+      <c r="AJ51" s="119"/>
+      <c r="AK51" s="119"/>
+      <c r="AL51" s="119"/>
+      <c r="AM51" s="119"/>
+      <c r="AN51" s="119"/>
+      <c r="AO51" s="119"/>
+      <c r="AP51" s="119"/>
+      <c r="AQ51" s="119"/>
+      <c r="AR51" s="119"/>
+      <c r="AS51" s="119"/>
+      <c r="AT51" s="119"/>
+      <c r="AU51" s="119"/>
+      <c r="AV51" s="119"/>
+      <c r="AW51" s="119"/>
+      <c r="AX51" s="119"/>
+      <c r="AY51" s="119"/>
+      <c r="AZ51" s="119"/>
+    </row>
+    <row r="52" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C52" t="s">
         <v>207</v>
       </c>
       <c r="D52" s="118"/>
-      <c r="E52" s="117"/>
+      <c r="E52" s="117" t="s">
+        <v>209</v>
+      </c>
       <c r="F52" s="118"/>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.15">
+    <row r="53" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C53" t="s">
         <v>208</v>
       </c>
       <c r="D53" s="118"/>
-      <c r="E53" s="117"/>
+      <c r="E53" s="117" t="s">
+        <v>209</v>
+      </c>
       <c r="F53" s="118"/>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.15">
+    <row r="55" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C55" s="105" t="s">
         <v>160</v>
       </c>
@@ -34637,7 +36581,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
updated DataStructures.xlsx file, and finalized global.R to exclue initial and chem
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F37CAF-81C0-8142-A10F-5B68EDA0F065}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC587077-B809-864C-B83F-9F24980B975F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="1620" windowWidth="28660" windowHeight="18500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
-    <sheet name="initial" sheetId="3" r:id="rId2"/>
-    <sheet name="chemistry" sheetId="10" r:id="rId3"/>
-    <sheet name="historical" sheetId="5" r:id="rId4"/>
-    <sheet name="sensor" sheetId="6" r:id="rId5"/>
-    <sheet name="current" sheetId="4" r:id="rId6"/>
-    <sheet name="units" sheetId="9" r:id="rId7"/>
+    <sheet name="current" sheetId="4" r:id="rId2"/>
+    <sheet name="historical" sheetId="5" r:id="rId3"/>
+    <sheet name="sensor" sheetId="6" r:id="rId4"/>
+    <sheet name="units" sheetId="9" r:id="rId5"/>
+    <sheet name="OLD_initial" sheetId="3" r:id="rId6"/>
+    <sheet name="OLD_current" sheetId="10" r:id="rId7"/>
     <sheet name="AlmostFinalNames" sheetId="1" r:id="rId8"/>
     <sheet name="CreatingCommonNames" sheetId="2" r:id="rId9"/>
   </sheets>
@@ -3448,2031 +3448,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B63FAF-B35B-BB4D-A7FB-6A2BC573DBFB}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="103" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="98" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="98" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="154" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="99" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" t="str">
-        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
-      </c>
-      <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
-      </c>
-      <c r="H2" s="101" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="99" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="str">
-        <f>CONCATENATE(A3, " ",  B3, ", ")</f>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-      <c r="H3" s="101"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="99" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="99"/>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D21" si="0">CONCATENATE(A4, " ",  B4, ", ")</f>
-        <v xml:space="preserve">site VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="99"/>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">date DATE, </v>
-      </c>
-      <c r="H5" s="110" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="99"/>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">timeEST TIME, </v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="99" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="99" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" t="str">
-        <f>CONCATENATE(A7, " ",  B7, ", ")</f>
-        <v xml:space="preserve">waterYr YEAR, </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="104" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="99"/>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(8,4), </v>
-      </c>
-      <c r="F8" s="115"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="99"/>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
-      </c>
-      <c r="F9" s="115"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="99" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="99"/>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DIC SMALLINT, </v>
-      </c>
-      <c r="F10" s="115"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="99"/>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
-      </c>
-      <c r="F11" s="115"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="99"/>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(8,4), </v>
-      </c>
-      <c r="F12" s="115"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C13" s="99"/>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
-      </c>
-      <c r="F13" s="115"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C14" s="99"/>
-      <c r="D14" t="str">
-        <f t="shared" ref="D14" si="1">CONCATENATE(A14, " ",  B14, ", ")</f>
-        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
-      </c>
-      <c r="F14" s="115"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="99"/>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
-      </c>
-      <c r="F15" s="115"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="99" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="99"/>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="99" t="s">
-        <v>199</v>
-      </c>
-      <c r="C17" s="99"/>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(20,4), </v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="99"/>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="99" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="99"/>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="99"/>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">notes TEXT, </v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="99"/>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">archived VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="99" t="s">
-        <v>204</v>
-      </c>
-      <c r="B22" s="117"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="118"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="99" t="s">
-        <v>205</v>
-      </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="117"/>
-      <c r="D23" s="118"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>206</v>
-      </c>
-      <c r="B24" s="118"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="118"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>207</v>
-      </c>
-      <c r="B25" s="118"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="118"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>208</v>
-      </c>
-      <c r="B26" s="118"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="118"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="99"/>
-      <c r="C27" s="99"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="99"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="99"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="105" t="s">
-        <v>160</v>
-      </c>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="99"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="99"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="99"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="99"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="99"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="99"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="99"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="99"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="99"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="99"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="99"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="99"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="99"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="99"/>
-      <c r="B43" s="99"/>
-      <c r="C43" s="99"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="99"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="99"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="99"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="99"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="99"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="99"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="99"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="99"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="99"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="99"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" s="99"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="99"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="F8:F15">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
-  <dimension ref="A1:I34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="7" max="7" width="50.5" customWidth="1"/>
-    <col min="9" max="9" width="50.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="103" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="103" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="98" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="98" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="99" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" s="99"/>
-      <c r="E2" t="str">
-        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
-      </c>
-      <c r="G2" s="100" t="str">
-        <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
-      </c>
-      <c r="I2" s="101" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="99" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="99"/>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E31" si="0">CONCATENATE(A3, " ",  B3, ", ")</f>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-      <c r="G3" s="99" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="99" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="99" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" s="99"/>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">waterYr YEAR, </v>
-      </c>
-      <c r="I4" s="110"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="99" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="99"/>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime TEXT, </v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="104" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" s="104" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="104" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A11" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="104" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="104" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="104" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="104" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="104" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="104" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="104" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="104" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="104" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="104" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="99"/>
-      <c r="D28" s="99"/>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="99" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">duplicate VARCHAR(10), </v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">sampleType VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="104" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="105" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A1048576 G3">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F550B6-2737-6444-9C2F-C54D4FE9A82E}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H46"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53" customWidth="1"/>
-    <col min="8" max="8" width="53" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="103" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="98" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="98" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="238" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="99" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
-      </c>
-      <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
-      </c>
-      <c r="H2" s="101" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="99"/>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">site VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="99"/>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">date DATE, </v>
-      </c>
-      <c r="H4" s="110" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="99" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="99"/>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">timeEST TIME, </v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="99" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" s="99" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pH DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="99" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="99"/>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DIC SMALLINT, </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="99"/>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="99" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="99"/>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">temp DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="99"/>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="99" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="99"/>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="99"/>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="99" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="99"/>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="99" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="99"/>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="99"/>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="99" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="99"/>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="99"/>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">notes TEXT, </v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="99" t="s">
-        <v>186</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="99" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" s="99" t="s">
-        <v>187</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">waterYr YEAR, </v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="99" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="99" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="99" t="s">
-        <v>189</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">datetime TEXT, </v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="99"/>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="99" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="99"/>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="99" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C23" s="99"/>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">K DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="99" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C24" s="99"/>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Na DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="99" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C25" s="99"/>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="99" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="99"/>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="99" t="s">
-        <v>158</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="99" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="99"/>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="99" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="99"/>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="99" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="99"/>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="99" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="99"/>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="99" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="99"/>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="99"/>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="99" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="99"/>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="99" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C35" s="99"/>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">DON DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="99" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C36" s="99"/>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="99" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C37" s="99"/>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="99" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="99"/>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="99" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="99"/>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">F DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="99" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="99"/>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C41" s="99"/>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="99" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C42" s="99"/>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C43" s="99" t="s">
-        <v>188</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="99" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="99"/>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">duplicate VARCHAR(10), </v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="99"/>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">sampleType VARCHAR(20), </v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="99" t="s">
-        <v>108</v>
-      </c>
-      <c r="B46" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="99"/>
-      <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB057EB0-7D51-3A4D-BF90-400EEA7362FF}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="103" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="98" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="98" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="99" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" t="str">
-        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
-      </c>
-      <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5, D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="99"/>
-      <c r="D3" t="str">
-        <f>CONCATENATE(A3, " ",  B3, ", ")</f>
-        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="99" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="99"/>
-      <c r="D4" t="str">
-        <f>CONCATENATE(A4, " ",  B4, ", ")</f>
-        <v xml:space="preserve">site VARCHAR(20), </v>
-      </c>
-      <c r="F4" s="100"/>
-      <c r="G4" s="110" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="99"/>
-      <c r="D5" t="str">
-        <f t="shared" ref="D5:D6" si="0">CONCATENATE(A5, " ",  B5, ", ")</f>
-        <v xml:space="preserve">date DATE, </v>
-      </c>
-      <c r="F5" s="100"/>
-      <c r="G5" s="102"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="99"/>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">timeEST TIME, </v>
-      </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="102"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="99" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="99" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" s="99" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" ref="D7:D8" si="1">CONCATENATE(A7, " ",  B7, ", ")</f>
-        <v xml:space="preserve">flowSensor DECIMAL(13,4), </v>
-      </c>
-      <c r="E7" s="99"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="99" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="99" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="99" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">precipETI DECIMAL(13,4), </v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="99"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="99"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="99"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="99"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="99"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="99"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="99"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="99"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="99"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="99"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="99"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="99"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="99"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="99"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="99"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="99"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="99"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="99"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="99"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="99"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="99"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="99"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="99"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="99"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="99"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="99"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="99"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="99"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="99"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="99"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="99"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="99"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="99"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="99"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="99"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="99"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="99"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="99"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="99"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="99"/>
-      <c r="B43" s="99"/>
-      <c r="C43" s="99"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="99"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="99"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="99"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="99"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="99"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="99"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="99"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="99"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="99"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="99"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" s="99"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="99"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A8635-60E1-404A-9A09-732833EFAF77}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AZ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="116"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
@@ -8426,14 +6413,1034 @@
     <sortCondition ref="A3:A48"/>
   </sortState>
   <conditionalFormatting sqref="C1:C18 I3:I20 C20:C48 C60:C1048576 C54:C55">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F550B6-2737-6444-9C2F-C54D4FE9A82E}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53" customWidth="1"/>
+    <col min="8" max="8" width="53" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="98" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="238" x14ac:dyDescent="0.15">
+      <c r="A2" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
+      </c>
+      <c r="F2" s="100" t="str">
+        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+      </c>
+      <c r="H2" s="101" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">site VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="99"/>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">date DATE, </v>
+      </c>
+      <c r="H4" s="110" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">timeEST TIME, </v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="99" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="99" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="99"/>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DIC SMALLINT, </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="99" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="99"/>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="99" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="99"/>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="99" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="99"/>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="99" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="99"/>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="99"/>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">flowGageHt DECIMAL(16,4), </v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="99"/>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="99"/>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="99"/>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">notes TEXT, </v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="99" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">waterYr YEAR, </v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">datetime TEXT, </v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="99"/>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="99"/>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="99"/>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="99"/>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="99"/>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="99"/>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="99"/>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="99"/>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="99"/>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="99"/>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="99"/>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="99"/>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="99"/>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="99"/>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="99" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="99"/>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="99"/>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="99"/>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="99"/>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="99"/>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="99"/>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="99"/>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">duplicate VARCHAR(10), </v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="99"/>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">sampleType VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="99"/>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB057EB0-7D51-3A4D-BF90-400EEA7362FF}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="98" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
+      </c>
+      <c r="F2" s="100" t="str">
+        <f>CONCATENATE(D2,D3,D4,D5, D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, flowSensor DECIMAL(13,4), precipETI DECIMAL(13,4), </v>
+      </c>
+      <c r="G2" s="102" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" t="str">
+        <f>CONCATENATE(A3, " ",  B3, ", ")</f>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="99"/>
+      <c r="D4" t="str">
+        <f>CONCATENATE(A4, " ",  B4, ", ")</f>
+        <v xml:space="preserve">site VARCHAR(20), </v>
+      </c>
+      <c r="F4" s="100"/>
+      <c r="G4" s="110" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" t="str">
+        <f t="shared" ref="D5:D6" si="0">CONCATENATE(A5, " ",  B5, ", ")</f>
+        <v xml:space="preserve">date DATE, </v>
+      </c>
+      <c r="F5" s="100"/>
+      <c r="G5" s="102"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="99"/>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">timeEST TIME, </v>
+      </c>
+      <c r="F6" s="100"/>
+      <c r="G6" s="102"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" ref="D7:D8" si="1">CONCATENATE(A7, " ",  B7, ", ")</f>
+        <v xml:space="preserve">flowSensor DECIMAL(13,4), </v>
+      </c>
+      <c r="E7" s="99"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">precipETI DECIMAL(13,4), </v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="99"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="99"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="99"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="99"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="99"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="99"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="99"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="99"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="99"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="99"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="99"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="99"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="99"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="99"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="99"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="99"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="99"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="99"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="99"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="99"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="99"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="99"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="99"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="99"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="99"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="99"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="99"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="99"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="99"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="99"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="99"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="99"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="99"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="99"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="99"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="99"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="99"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="99"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="99"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="99"/>
+      <c r="B42" s="99"/>
+      <c r="C42" s="99"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="99"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="99"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="99"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="99"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="99"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="99"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="99"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="99"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="99"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="99"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="99"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="99"/>
+      <c r="B49" s="99"/>
+      <c r="C49" s="99"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="99"/>
+      <c r="B50" s="99"/>
+      <c r="C50" s="99"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6260233-ECAC-3248-955E-10E3D058E348}">
   <dimension ref="A1:C1001"/>
   <sheetViews>
@@ -9789,6 +8796,1000 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B63FAF-B35B-BB4D-A7FB-6A2BC573DBFB}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="98" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="154" x14ac:dyDescent="0.15">
+      <c r="A2" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
+      </c>
+      <c r="F2" s="100" t="str">
+        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
+      </c>
+      <c r="H2" s="101" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE(A3, " ",  B3, ", ")</f>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+      <c r="H3" s="101"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="99"/>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D21" si="0">CONCATENATE(A4, " ",  B4, ", ")</f>
+        <v xml:space="preserve">site VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">date DATE, </v>
+      </c>
+      <c r="H5" s="110" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="99"/>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">timeEST TIME, </v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="str">
+        <f>CONCATENATE(A7, " ",  B7, ", ")</f>
+        <v xml:space="preserve">waterYr YEAR, </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="104" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="99"/>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">pH DECIMAL(8,4), </v>
+      </c>
+      <c r="F8" s="115"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">pHmetrohm DECIMAL(8,4), </v>
+      </c>
+      <c r="F9" s="115"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="104" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="99"/>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DIC SMALLINT, </v>
+      </c>
+      <c r="F10" s="115"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="99"/>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">spCond DECIMAL(8,4), </v>
+      </c>
+      <c r="F11" s="115"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="99"/>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">temp DECIMAL(8,4), </v>
+      </c>
+      <c r="F12" s="115"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ANCMet DECIMAL(8,4), </v>
+      </c>
+      <c r="F13" s="115"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="99"/>
+      <c r="D14" t="str">
+        <f t="shared" ref="D14" si="1">CONCATENATE(A14, " ",  B14, ", ")</f>
+        <v xml:space="preserve">ANC960 DECIMAL(8,4), </v>
+      </c>
+      <c r="F14" s="115"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="99" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="99"/>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">gageHt DECIMAL(8,4), </v>
+      </c>
+      <c r="F15" s="115"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="99"/>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">hydroGraph VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" s="99"/>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">flowGageHt DECIMAL(20,4), </v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="99"/>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">precipCatch DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="99"/>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">fieldCode VARCHAR(50), </v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="99"/>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">notes TEXT, </v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="99"/>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">archived VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="118"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="118"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="118"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" s="118"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="118"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="118"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="99"/>
+      <c r="C27" s="99"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="99"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="105" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="99"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="99"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="99"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="99"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="99"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="99"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="99"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="99"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="99"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="99"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="99"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="99"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="99"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="99"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="99"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="99"/>
+      <c r="B42" s="99"/>
+      <c r="C42" s="99"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="99"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="99"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="99"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="99"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="99"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="99"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="99"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="99"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="99"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="99"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="99"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="99"/>
+      <c r="B49" s="99"/>
+      <c r="C49" s="99"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="99"/>
+      <c r="B50" s="99"/>
+      <c r="C50" s="99"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F8:F15">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6302B58-8B97-A648-9738-377C00C8F8A4}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="7" max="7" width="50.5" customWidth="1"/>
+    <col min="9" max="9" width="50.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="98" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.15">
+      <c r="A2" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="99"/>
+      <c r="E2" t="str">
+        <f>CONCATENATE(A2, " ",  B2, ", ")</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
+      </c>
+      <c r="G2" s="100" t="str">
+        <f>CONCATENATE(E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29,E30,E31)</f>
+        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+      </c>
+      <c r="I2" s="101" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="99"/>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E31" si="0">CONCATENATE(A3, " ",  B3, ", ")</f>
+        <v xml:space="preserve">uniqueID VARCHAR(50) UNIQUE NOT NULL, </v>
+      </c>
+      <c r="G3" s="99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="99"/>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">waterYr YEAR, </v>
+      </c>
+      <c r="I4" s="110"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="99"/>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">datetime TEXT, </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ca DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Mg DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">K DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Na DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OMAl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Al_ICP DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NH4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">SO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NO3 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="104" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Cl DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="104" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PO4 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DOC DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TDN DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DON DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">SiO2 DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Mn DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="104" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Fe DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">F DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">cationCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">anionCharge DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="104" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">theoryCond DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ionError DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">duplicate VARCHAR(10), </v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">sampleType VARCHAR(20), </v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="105" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576 G3">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet5"/>

</xml_diff>

<commit_message>
few design fixes to free-for-all tab
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC587077-B809-864C-B83F-9F24980B975F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBC16A3-F664-7D4B-8A23-E5360C62B203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="1620" windowWidth="28660" windowHeight="18500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="1580" windowWidth="28660" windowHeight="18500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="AlmostFinalNames" sheetId="1" r:id="rId8"/>
     <sheet name="CreatingCommonNames" sheetId="2" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="212">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -825,9 +825,6 @@
     <t>DECIMAL(16,4)</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -883,6 +880,12 @@
   </si>
   <si>
     <t>Remove?</t>
+  </si>
+  <si>
+    <t>added Jan-24-2019</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), canonical VARCHAR(20)</t>
   </si>
 </sst>
 </file>
@@ -3493,10 +3496,10 @@
     </row>
     <row r="2" spans="1:52" ht="266" x14ac:dyDescent="0.15">
       <c r="A2" s="116" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="99" t="s">
         <v>144</v>
@@ -3517,7 +3520,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="K2" s="101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.15">
@@ -3587,7 +3590,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="104" t="s">
         <v>137</v>
@@ -3610,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>26</v>
@@ -3631,7 +3634,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" s="104" t="s">
         <v>30</v>
@@ -3695,7 +3698,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9" s="104" t="s">
         <v>34</v>
@@ -4330,7 +4333,7 @@
         <v>145</v>
       </c>
       <c r="E19" s="120" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F19" s="120"/>
       <c r="G19" t="str">
@@ -4577,7 +4580,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="104" t="s">
         <v>66</v>
@@ -4641,7 +4644,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C24" s="104" t="s">
         <v>70</v>
@@ -4705,7 +4708,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" s="104" t="s">
         <v>72</v>
@@ -4769,7 +4772,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" s="104" t="s">
         <v>74</v>
@@ -4833,7 +4836,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>75</v>
@@ -4897,7 +4900,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" s="104" t="s">
         <v>76</v>
@@ -4961,7 +4964,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>78</v>
@@ -5025,7 +5028,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C30" s="104" t="s">
         <v>81</v>
@@ -5089,7 +5092,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="104" t="s">
         <v>82</v>
@@ -5153,7 +5156,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C32" s="104" t="s">
         <v>84</v>
@@ -5217,7 +5220,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C33" s="104" t="s">
         <v>85</v>
@@ -5281,7 +5284,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="104" t="s">
         <v>86</v>
@@ -5345,7 +5348,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" s="104" t="s">
         <v>89</v>
@@ -5409,7 +5412,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" s="104" t="s">
         <v>90</v>
@@ -5473,7 +5476,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C37" s="104" t="s">
         <v>91</v>
@@ -5537,7 +5540,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C38" s="104" t="s">
         <v>92</v>
@@ -5601,7 +5604,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39" s="104" t="s">
         <v>93</v>
@@ -5665,7 +5668,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C40" s="104" t="s">
         <v>94</v>
@@ -5729,7 +5732,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C41" s="104" t="s">
         <v>95</v>
@@ -6223,11 +6226,11 @@
     </row>
     <row r="49" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C49" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="117"/>
       <c r="E49" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F49" s="118"/>
       <c r="I49" s="119"/>
@@ -6277,11 +6280,11 @@
     </row>
     <row r="50" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C50" s="99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="118"/>
       <c r="E50" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F50" s="118"/>
       <c r="I50" s="119"/>
@@ -6331,11 +6334,11 @@
     </row>
     <row r="51" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="118"/>
       <c r="E51" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F51" s="118"/>
       <c r="I51" s="119"/>
@@ -6385,21 +6388,21 @@
     </row>
     <row r="52" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" s="118"/>
       <c r="E52" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F52" s="118"/>
     </row>
     <row r="53" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D53" s="118"/>
       <c r="E53" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F53" s="118"/>
     </row>
@@ -6423,10 +6426,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F550B6-2737-6444-9C2F-C54D4FE9A82E}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6459,7 +6462,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="238" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="252" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -6470,15 +6473,15 @@
         <v>178</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
+        <f t="shared" ref="D2:D47" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46, D47)</f>
+        <v>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), canonical VARCHAR(20)</v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -7066,6 +7069,21 @@
       <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" t="str">
+        <f>CONCATENATE(A47, " ",  B47)</f>
+        <v>canonical VARCHAR(20)</v>
       </c>
     </row>
   </sheetData>
@@ -7461,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="111" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7469,7 +7487,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="113"/>
     </row>
@@ -7478,7 +7496,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" s="113"/>
     </row>
@@ -7487,7 +7505,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="113"/>
     </row>
@@ -7496,7 +7514,7 @@
         <v>137</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="113"/>
     </row>
@@ -7539,7 +7557,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="112" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7547,7 +7565,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="113"/>
     </row>
@@ -7556,7 +7574,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="113"/>
     </row>
@@ -7565,7 +7583,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C13" s="113"/>
     </row>
@@ -7582,7 +7600,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7590,7 +7608,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="112" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7750,7 +7768,7 @@
         <v>97</v>
       </c>
       <c r="B36" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7758,7 +7776,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7766,7 +7784,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7774,7 +7792,7 @@
         <v>101</v>
       </c>
       <c r="B39" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7787,7 +7805,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7795,7 +7813,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7803,7 +7821,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7811,7 +7829,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7819,7 +7837,7 @@
         <v>106</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7833,7 +7851,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2"/>
@@ -8854,7 +8872,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -9060,7 +9078,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
@@ -9122,7 +9140,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" s="117"/>
       <c r="C22" s="117"/>
@@ -9130,7 +9148,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="118"/>
       <c r="C23" s="117"/>
@@ -9138,7 +9156,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="118"/>
       <c r="C24" s="117"/>
@@ -9146,7 +9164,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B25" s="118"/>
       <c r="C25" s="117"/>
@@ -9154,7 +9172,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26" s="118"/>
       <c r="C26" s="117"/>
@@ -9357,7 +9375,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
saving changes to DataStructures and metadata files
</commit_message>
<xml_diff>
--- a/restricted_QAQC/documentation/DataStructures.xlsx
+++ b/restricted_QAQC/documentation/DataStructures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CTRoeRaymond/Dropbox/WORK/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theRoeRaymonds/Dropbox/Work/DataVizProjects/HBEF/shiny/restricted_QAQC/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC587077-B809-864C-B83F-9F24980B975F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBC16A3-F664-7D4B-8A23-E5360C62B203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="1620" windowWidth="28660" windowHeight="18500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="1580" windowWidth="28660" windowHeight="18500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="AlmostFinalNames" sheetId="1" r:id="rId8"/>
     <sheet name="CreatingCommonNames" sheetId="2" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="212">
   <si>
     <t>Standardized Name</t>
   </si>
@@ -825,9 +825,6 @@
     <t>DECIMAL(16,4)</t>
   </si>
   <si>
-    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4)</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -883,6 +880,12 @@
   </si>
   <si>
     <t>Remove?</t>
+  </si>
+  <si>
+    <t>added Jan-24-2019</t>
+  </si>
+  <si>
+    <t>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), canonical VARCHAR(20)</t>
   </si>
 </sst>
 </file>
@@ -3493,10 +3496,10 @@
     </row>
     <row r="2" spans="1:52" ht="266" x14ac:dyDescent="0.15">
       <c r="A2" s="116" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="99" t="s">
         <v>144</v>
@@ -3517,7 +3520,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="K2" s="101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.15">
@@ -3587,7 +3590,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="104" t="s">
         <v>137</v>
@@ -3610,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>26</v>
@@ -3631,7 +3634,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" s="104" t="s">
         <v>30</v>
@@ -3695,7 +3698,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9" s="104" t="s">
         <v>34</v>
@@ -4330,7 +4333,7 @@
         <v>145</v>
       </c>
       <c r="E19" s="120" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F19" s="120"/>
       <c r="G19" t="str">
@@ -4577,7 +4580,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="104" t="s">
         <v>66</v>
@@ -4641,7 +4644,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C24" s="104" t="s">
         <v>70</v>
@@ -4705,7 +4708,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" s="104" t="s">
         <v>72</v>
@@ -4769,7 +4772,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" s="104" t="s">
         <v>74</v>
@@ -4833,7 +4836,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>75</v>
@@ -4897,7 +4900,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" s="104" t="s">
         <v>76</v>
@@ -4961,7 +4964,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>78</v>
@@ -5025,7 +5028,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C30" s="104" t="s">
         <v>81</v>
@@ -5089,7 +5092,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="104" t="s">
         <v>82</v>
@@ -5153,7 +5156,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C32" s="104" t="s">
         <v>84</v>
@@ -5217,7 +5220,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C33" s="104" t="s">
         <v>85</v>
@@ -5281,7 +5284,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="104" t="s">
         <v>86</v>
@@ -5345,7 +5348,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" s="104" t="s">
         <v>89</v>
@@ -5409,7 +5412,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" s="104" t="s">
         <v>90</v>
@@ -5473,7 +5476,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C37" s="104" t="s">
         <v>91</v>
@@ -5537,7 +5540,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C38" s="104" t="s">
         <v>92</v>
@@ -5601,7 +5604,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39" s="104" t="s">
         <v>93</v>
@@ -5665,7 +5668,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C40" s="104" t="s">
         <v>94</v>
@@ -5729,7 +5732,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C41" s="104" t="s">
         <v>95</v>
@@ -6223,11 +6226,11 @@
     </row>
     <row r="49" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C49" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="117"/>
       <c r="E49" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F49" s="118"/>
       <c r="I49" s="119"/>
@@ -6277,11 +6280,11 @@
     </row>
     <row r="50" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C50" s="99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="118"/>
       <c r="E50" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F50" s="118"/>
       <c r="I50" s="119"/>
@@ -6331,11 +6334,11 @@
     </row>
     <row r="51" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="118"/>
       <c r="E51" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F51" s="118"/>
       <c r="I51" s="119"/>
@@ -6385,21 +6388,21 @@
     </row>
     <row r="52" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" s="118"/>
       <c r="E52" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F52" s="118"/>
     </row>
     <row r="53" spans="3:52" x14ac:dyDescent="0.15">
       <c r="C53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D53" s="118"/>
       <c r="E53" s="117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F53" s="118"/>
     </row>
@@ -6423,10 +6426,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F550B6-2737-6444-9C2F-C54D4FE9A82E}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6459,7 +6462,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="238" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="252" x14ac:dyDescent="0.15">
       <c r="A2" s="99" t="s">
         <v>144</v>
       </c>
@@ -6470,15 +6473,15 @@
         <v>178</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D46" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
+        <f t="shared" ref="D2:D47" si="0">CONCATENATE(A2, " ",  B2, ", ")</f>
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, </v>
       </c>
       <c r="F2" s="100" t="str">
-        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46)</f>
-        <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
+        <f>CONCATENATE(D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46, D47)</f>
+        <v>refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, site VARCHAR(20), date DATE, timeEST TIME, pH DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANC960 DECIMAL(8,4), ANCMet DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(16,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), canonical VARCHAR(20)</v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -7066,6 +7069,21 @@
       <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ionBalance DECIMAL(8,4), </v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" t="str">
+        <f>CONCATENATE(A47, " ",  B47)</f>
+        <v>canonical VARCHAR(20)</v>
       </c>
     </row>
   </sheetData>
@@ -7461,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="111" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7469,7 +7487,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="113"/>
     </row>
@@ -7478,7 +7496,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" s="113"/>
     </row>
@@ -7487,7 +7505,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="113"/>
     </row>
@@ -7496,7 +7514,7 @@
         <v>137</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="113"/>
     </row>
@@ -7539,7 +7557,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="112" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7547,7 +7565,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="113"/>
     </row>
@@ -7556,7 +7574,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="113"/>
     </row>
@@ -7565,7 +7583,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C13" s="113"/>
     </row>
@@ -7582,7 +7600,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7590,7 +7608,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="112" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7750,7 +7768,7 @@
         <v>97</v>
       </c>
       <c r="B36" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7758,7 +7776,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7766,7 +7784,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7774,7 +7792,7 @@
         <v>101</v>
       </c>
       <c r="B39" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7787,7 +7805,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7795,7 +7813,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7803,7 +7821,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7811,7 +7829,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7819,7 +7837,7 @@
         <v>106</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7833,7 +7851,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2"/>
@@ -8854,7 +8872,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, site VARCHAR(20), date DATE, timeEST TIME, waterYr YEAR, pH DECIMAL(8,4), pHmetrohm DECIMAL(8,4), DIC SMALLINT, spCond DECIMAL(8,4), temp DECIMAL(8,4), ANCMet DECIMAL(8,4), ANC960 DECIMAL(8,4), gageHt DECIMAL(8,4), hydroGraph VARCHAR(20), flowGageHt DECIMAL(20,4), precipCatch DECIMAL(8,4), fieldCode VARCHAR(50), notes TEXT, archived VARCHAR(20), </v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -9060,7 +9078,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="99"/>
       <c r="D17" t="str">
@@ -9122,7 +9140,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" s="117"/>
       <c r="C22" s="117"/>
@@ -9130,7 +9148,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="118"/>
       <c r="C23" s="117"/>
@@ -9138,7 +9156,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="118"/>
       <c r="C24" s="117"/>
@@ -9146,7 +9164,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B25" s="118"/>
       <c r="C25" s="117"/>
@@ -9154,7 +9172,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26" s="118"/>
       <c r="C26" s="117"/>
@@ -9357,7 +9375,7 @@
         <v xml:space="preserve">refNo INT PRIMARY KEY NOT NULL AUTO_INCREMENT, uniqueID VARCHAR(50) UNIQUE NOT NULL, waterYr YEAR, datetime TEXT, Ca DECIMAL(8,4), Mg DECIMAL(8,4), K DECIMAL(8,4), Na DECIMAL(8,4), TMAl DECIMAL(8,4), OMAl DECIMAL(8,4), Al_ICP DECIMAL(8,4), NH4 DECIMAL(8,4), SO4 DECIMAL(8,4), NO3 DECIMAL(8,4), Cl DECIMAL(8,4), PO4 DECIMAL(8,4), DOC DECIMAL(8,4), TDN DECIMAL(8,4), DON DECIMAL(8,4), SiO2 DECIMAL(8,4), Mn DECIMAL(8,4), Fe DECIMAL(8,4), F DECIMAL(8,4), cationCharge DECIMAL(8,4), anionCharge DECIMAL(8,4), theoryCond DECIMAL(8,4), ionError DECIMAL(8,4), duplicate VARCHAR(10), sampleType VARCHAR(20), ionBalance DECIMAL(8,4), </v>
       </c>
       <c r="I2" s="101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>